<commit_message>
remove old files, minore enhancements
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\bioindustrial-park\BioSTEAM 2.x.x\biorefineries\oilcane\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595BCB61-81D5-4C8E-8B2D-B1A6C5950B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="2112" windowWidth="20532" windowHeight="10596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>Element</t>
   </si>
@@ -94,6 +88,9 @@
     <t>Stream-pure glycerine</t>
   </si>
   <si>
+    <t>Saccharification</t>
+  </si>
+  <si>
     <t>cellulase</t>
   </si>
   <si>
@@ -109,6 +106,18 @@
     <t>Cofermentation</t>
   </si>
   <si>
+    <t>oilcane</t>
+  </si>
+  <si>
+    <t>oilsorghum</t>
+  </si>
+  <si>
+    <t>Oil retention [%]</t>
+  </si>
+  <si>
+    <t>Bagasse oil extraction efficiency [%]</t>
+  </si>
+  <si>
     <t>Capacity [ton/hr]</t>
   </si>
   <si>
@@ -130,7 +139,7 @@
     <t>Price [USD/kg]</t>
   </si>
   <si>
-    <t>Tau</t>
+    <t>Reaction time [hr]</t>
   </si>
   <si>
     <t>Cellulase loading [wt. % cellulose]</t>
@@ -163,18 +172,9 @@
     <t>Productivity [g/L]</t>
   </si>
   <si>
-    <t>Bagasse oil extraction efficiency [%]</t>
-  </si>
-  <si>
-    <t>oilcane</t>
-  </si>
-  <si>
     <t>Cane  PL content [% oil]</t>
   </si>
   <si>
-    <t>oilsorghum</t>
-  </si>
-  <si>
     <t>Sorghum  PL content [% oil]</t>
   </si>
   <si>
@@ -191,16 +191,13 @@
   </si>
   <si>
     <t>TAG to  FFA conversion [% oil]</t>
-  </si>
-  <si>
-    <t>Oil retention [%]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,11 +249,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -266,14 +260,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -320,7 +306,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,27 +338,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,24 +372,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -597,37 +547,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -674,7 +622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,775 +630,775 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>-2.283115780924631E-2</v>
+        <v>-0.02282848065713922</v>
       </c>
       <c r="E4">
-        <v>3.2521586068863441E-2</v>
+        <v>0.03252194914087796</v>
       </c>
       <c r="F4">
-        <v>-2.345721060228842E-2</v>
+        <v>-0.02345721060228842</v>
       </c>
       <c r="H4">
-        <v>2.3416565352662611E-2</v>
+        <v>0.02341656535266261</v>
       </c>
       <c r="I4">
-        <v>1.8247167801886711E-2</v>
+        <v>0.01824716780188671</v>
       </c>
       <c r="J4">
-        <v>-1.0011261443426111E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+        <v>-0.002045117860332284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>7.191296927651877E-3</v>
+        <v>0.007193248799729951</v>
       </c>
       <c r="E5">
-        <v>2.9407692696307702E-2</v>
+        <v>0.02940805941632237</v>
       </c>
       <c r="F5">
-        <v>-2.395886351835454E-2</v>
+        <v>-0.02395886351835454</v>
       </c>
       <c r="H5">
-        <v>2.3989847423593891E-2</v>
+        <v>0.02398984742359389</v>
       </c>
       <c r="I5">
-        <v>2.0999206727968261E-2</v>
+        <v>0.02099920672796826</v>
       </c>
       <c r="J5">
-        <v>9.4718183313619031E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+        <v>0.01881517031626738</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6">
-        <v>0.15198705171148211</v>
+        <v>0.1519892917755716</v>
       </c>
       <c r="E6">
-        <v>0.93822941634517643</v>
+        <v>0.9382297877691913</v>
       </c>
       <c r="F6">
-        <v>-0.99998048252721916</v>
+        <v>-0.9999804825272192</v>
       </c>
       <c r="H6">
-        <v>0.99999999164799958</v>
+        <v>0.9999999916479996</v>
       </c>
       <c r="I6">
-        <v>0.95869140954765619</v>
+        <v>0.9586914095476562</v>
       </c>
       <c r="J6">
-        <v>-2.1723984239358811E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.03717130597819318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7">
-        <v>0.94840309403212364</v>
+        <v>0.948402028624081</v>
       </c>
       <c r="E7">
-        <v>-1.0727441325097649E-2</v>
+        <v>-0.01072723041308921</v>
       </c>
       <c r="F7">
-        <v>4.9236818929472752E-3</v>
+        <v>0.004923681892947275</v>
       </c>
       <c r="H7">
-        <v>-4.8251625610065017E-3</v>
+        <v>-0.004825162561006502</v>
       </c>
       <c r="I7">
-        <v>2.488744899549796E-3</v>
+        <v>0.002488744899549796</v>
       </c>
       <c r="J7">
-        <v>7.0570776904830554E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>-0.007348018100251941</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>2.2518815172752601E-2</v>
+        <v>0.02251866032474641</v>
       </c>
       <c r="E8">
-        <v>1.356077353443094E-2</v>
+        <v>0.01356083689443347</v>
       </c>
       <c r="F8">
-        <v>-1.314891086195643E-2</v>
+        <v>-0.01314891086195643</v>
       </c>
       <c r="H8">
-        <v>1.3129953645198139E-2</v>
+        <v>0.01312995364519814</v>
       </c>
       <c r="I8">
-        <v>1.8082658451306331E-2</v>
+        <v>0.01808265845130633</v>
       </c>
       <c r="J8">
-        <v>1.109177598846261E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>-0.01008280875313502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C9">
-        <v>-4.6048153841926152E-3</v>
+        <v>-0.004603344664133786</v>
       </c>
       <c r="E9">
-        <v>-7.4371149214845951E-3</v>
+        <v>-0.007437610857504434</v>
       </c>
       <c r="F9">
-        <v>1.4176456119058239E-2</v>
+        <v>0.01417645611905824</v>
       </c>
       <c r="H9">
-        <v>-1.424939039397561E-2</v>
+        <v>-0.01424939039397561</v>
       </c>
       <c r="I9">
-        <v>-1.66405299776212E-2</v>
+        <v>-0.0166405299776212</v>
       </c>
       <c r="J9">
-        <v>-1.2202190182349139E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+        <v>-0.005956763129398836</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C10">
-        <v>4.7849356505974251E-2</v>
+        <v>0.04784763455390538</v>
       </c>
       <c r="E10">
-        <v>2.169796397191855E-2</v>
+        <v>0.0216985349799414</v>
       </c>
       <c r="F10">
-        <v>-1.8181956919278271E-2</v>
+        <v>-0.01818195691927827</v>
       </c>
       <c r="H10">
-        <v>1.8062413778496551E-2</v>
+        <v>0.01806241377849655</v>
       </c>
       <c r="I10">
-        <v>1.400161121606445E-2</v>
+        <v>0.01400161121606445</v>
       </c>
       <c r="J10">
-        <v>6.5672117246890743E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+        <v>-0.004188052275484431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>0.1444172317606893</v>
+        <v>0.1444196462567858</v>
       </c>
       <c r="E11">
-        <v>3.3303417972136719E-3</v>
+        <v>0.003330694405227776</v>
       </c>
       <c r="F11">
-        <v>-7.8890978195639127E-3</v>
+        <v>-0.007889097819563913</v>
       </c>
       <c r="H11">
-        <v>7.6865115074604591E-3</v>
+        <v>0.007686511507460459</v>
       </c>
       <c r="I11">
-        <v>0.28337295072691798</v>
+        <v>0.283372950726918</v>
       </c>
       <c r="J11">
-        <v>-5.2716968164144614E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+        <v>0.01621422609533115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12">
-        <v>-0.19376981219879241</v>
+        <v>-0.1937712858948514</v>
       </c>
       <c r="E12">
-        <v>1.269399737175989E-2</v>
+        <v>0.0126933899797356</v>
       </c>
       <c r="F12">
-        <v>-1.4465973602638941E-2</v>
+        <v>-0.01446597360263894</v>
       </c>
       <c r="H12">
-        <v>1.4446771585870859E-2</v>
+        <v>0.01444677158587086</v>
       </c>
       <c r="I12">
-        <v>1.842309193692368E-2</v>
+        <v>0.01842309193692368</v>
       </c>
       <c r="J12">
-        <v>-3.2217541858241281E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.006420499561071366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>2.2407812192312481E-2</v>
+        <v>0.02240433948817358</v>
       </c>
       <c r="E13">
-        <v>-1.322413396896536E-3</v>
+        <v>-0.001323309556932382</v>
       </c>
       <c r="F13">
-        <v>4.6666170186646797E-3</v>
+        <v>0.00466661701866468</v>
       </c>
       <c r="H13">
-        <v>-4.7307682532307296E-3</v>
+        <v>-0.00473076825323073</v>
       </c>
       <c r="I13">
-        <v>-4.8883509155340362E-3</v>
+        <v>-0.004888350915534036</v>
       </c>
       <c r="J13">
-        <v>1.3835630570942489E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.0148806108589639</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C14">
-        <v>5.9017442360697681E-5</v>
+        <v>5.877984235119369E-05</v>
       </c>
       <c r="E14">
-        <v>-5.4659778506391133E-3</v>
+        <v>-0.005466022202640888</v>
       </c>
       <c r="F14">
-        <v>1.9647408785896349E-4</v>
+        <v>0.0001964740878589635</v>
       </c>
       <c r="H14">
-        <v>-1.528324861132994E-4</v>
+        <v>-0.0001528324861132994</v>
       </c>
       <c r="I14">
-        <v>-9.953175374127014E-3</v>
+        <v>-0.009953175374127014</v>
       </c>
       <c r="J14">
-        <v>-6.8710997556671062E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>-0.009907834521313514</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C15">
-        <v>-1.7526312029052481E-2</v>
+        <v>-0.01752412428496497</v>
       </c>
       <c r="E15">
-        <v>-7.7588049823521981E-3</v>
+        <v>-0.007759412470376498</v>
       </c>
       <c r="F15">
-        <v>7.8148350005933977E-3</v>
+        <v>0.007814835000593398</v>
       </c>
       <c r="H15">
-        <v>-7.782896567315861E-3</v>
+        <v>-0.007782896567315861</v>
       </c>
       <c r="I15">
-        <v>-7.8913572756542909E-3</v>
+        <v>-0.007891357275654291</v>
       </c>
       <c r="J15">
-        <v>2.159517101128804E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>0.004984996424747783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C16">
-        <v>1.6201356168054251E-3</v>
+        <v>0.001623263680930547</v>
       </c>
       <c r="E16">
-        <v>7.8259593850383731E-3</v>
+        <v>0.007825677625027104</v>
       </c>
       <c r="F16">
-        <v>-4.0670516826820666E-3</v>
+        <v>-0.004067051682682067</v>
       </c>
       <c r="H16">
-        <v>4.0787643551505734E-3</v>
+        <v>0.004078764355150573</v>
       </c>
       <c r="I16">
-        <v>8.3034321081372833E-3</v>
+        <v>0.008303432108137283</v>
       </c>
       <c r="J16">
-        <v>-1.9568402032568832E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+        <v>0.02280240083207389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C17">
-        <v>1.36514549460582E-3</v>
+        <v>0.001363491990539679</v>
       </c>
       <c r="E17">
-        <v>7.9603203184128109E-6</v>
+        <v>8.517312340692491E-06</v>
       </c>
       <c r="F17">
-        <v>-6.2726679949067186E-3</v>
+        <v>-0.006272667994906719</v>
       </c>
       <c r="H17">
-        <v>6.5184617967384709E-3</v>
+        <v>0.006518461796738471</v>
       </c>
       <c r="I17">
-        <v>5.896042603841703E-3</v>
+        <v>0.005896042603841703</v>
       </c>
       <c r="J17">
-        <v>-4.3159552906311656E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-0.005541955651736855</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C18">
-        <v>1.526795734671829E-2</v>
+        <v>0.01526711955468478</v>
       </c>
       <c r="E18">
-        <v>2.7086696763467871E-3</v>
+        <v>0.002708350860334034</v>
       </c>
       <c r="F18">
-        <v>-1.605290944211638E-3</v>
+        <v>-0.001605290944211638</v>
       </c>
       <c r="H18">
-        <v>1.54255926170237E-3</v>
+        <v>0.00154255926170237</v>
       </c>
       <c r="I18">
-        <v>-2.3310106532404261E-4</v>
+        <v>-0.0002331010653240426</v>
       </c>
       <c r="J18">
-        <v>7.4538770285661948E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>-0.03527657102737577</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C19">
-        <v>5.9280896131235833E-3</v>
+        <v>0.005929336653173466</v>
       </c>
       <c r="E19">
-        <v>6.6039593041583708E-4</v>
+        <v>0.0006596974343878973</v>
       </c>
       <c r="F19">
-        <v>4.1364760054590397E-4</v>
+        <v>0.000413647600545904</v>
       </c>
       <c r="H19">
-        <v>-3.5964846238593852E-4</v>
+        <v>-0.0003596484623859385</v>
       </c>
       <c r="I19">
-        <v>2.8548615541944618E-3</v>
+        <v>0.002854861554194462</v>
       </c>
       <c r="J19">
-        <v>-9.8184213059300078E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
+        <v>0.01205301617796706</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C20">
-        <v>-1.8148440149937599E-2</v>
+        <v>-0.01814623416584936</v>
       </c>
       <c r="E20">
-        <v>-6.1563714782548566E-3</v>
+        <v>-0.006156975798279032</v>
       </c>
       <c r="F20">
-        <v>4.8682783707311343E-3</v>
+        <v>0.004868278370731134</v>
       </c>
       <c r="H20">
-        <v>-4.8067104002684153E-3</v>
+        <v>-0.004806710400268415</v>
       </c>
       <c r="I20">
-        <v>-2.0263788330551532E-3</v>
+        <v>-0.002026378833055153</v>
       </c>
       <c r="J20">
-        <v>3.5433773421575448E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+        <v>0.007259576762824828</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C21">
-        <v>-2.2813675152547001E-2</v>
+        <v>-0.02281394961655798</v>
       </c>
       <c r="E21">
-        <v>1.1380897703235899E-2</v>
+        <v>0.01138105648724226</v>
       </c>
       <c r="F21">
-        <v>-4.9493003579720134E-3</v>
+        <v>-0.004949300357972013</v>
       </c>
       <c r="H21">
-        <v>5.0526002021040071E-3</v>
+        <v>0.005052600202104007</v>
       </c>
       <c r="I21">
-        <v>3.556671886266875E-3</v>
+        <v>0.003556671886266875</v>
       </c>
       <c r="J21">
-        <v>8.1965690640256744E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+        <v>0.004871370891708491</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C22">
-        <v>-2.2149669909986791E-2</v>
+        <v>-0.02214724850188994</v>
       </c>
       <c r="E22">
-        <v>-1.159324654372986E-2</v>
+        <v>-0.01159287550371502</v>
       </c>
       <c r="F22">
-        <v>1.1057474746298991E-2</v>
+        <v>0.01105747474629899</v>
       </c>
       <c r="H22">
-        <v>-1.103848815353952E-2</v>
+        <v>-0.01103848815353952</v>
       </c>
       <c r="I22">
-        <v>-1.0868982290759289E-2</v>
+        <v>-0.01086898229075929</v>
       </c>
       <c r="J22">
-        <v>6.3666902292093654E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>0.008408733523535534</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C23">
-        <v>-4.6300915132036586E-3</v>
+        <v>-0.004626522137060884</v>
       </c>
       <c r="E23">
-        <v>-1.2301165932046641E-2</v>
+        <v>-0.01230164286006571</v>
       </c>
       <c r="F23">
-        <v>1.396085643043425E-2</v>
+        <v>0.01396085643043425</v>
       </c>
       <c r="H23">
-        <v>-1.4082891059315639E-2</v>
+        <v>-0.01408289105931564</v>
       </c>
       <c r="I23">
-        <v>-1.179273109570924E-2</v>
+        <v>-0.01179273109570924</v>
       </c>
       <c r="J23">
-        <v>-1.849373487128882E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+        <v>-0.007662212278717682</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C24">
-        <v>-9.812086472483458E-3</v>
+        <v>-0.009810745928429836</v>
       </c>
       <c r="E24">
-        <v>7.1067979162719157E-3</v>
+        <v>0.007106787644271504</v>
       </c>
       <c r="F24">
-        <v>-1.023005272920211E-2</v>
+        <v>-0.01023005272920211</v>
       </c>
       <c r="H24">
-        <v>1.027197593087904E-2</v>
+        <v>0.01027197593087904</v>
       </c>
       <c r="I24">
-        <v>1.3105829324233169E-2</v>
+        <v>0.01310582932423317</v>
       </c>
       <c r="J24">
-        <v>4.913271513563789E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>-0.02917054464679801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C25">
-        <v>4.6574181062967231E-3</v>
+        <v>0.004659246522369861</v>
       </c>
       <c r="E25">
-        <v>1.9628313329132532E-2</v>
+        <v>0.01962846270513851</v>
       </c>
       <c r="F25">
-        <v>-1.7051159818046391E-2</v>
+        <v>-0.01705115981804639</v>
       </c>
       <c r="H25">
-        <v>1.7054648938185951E-2</v>
+        <v>0.01705464893818595</v>
       </c>
       <c r="I25">
-        <v>1.9851648890065951E-2</v>
+        <v>0.01985164889006595</v>
       </c>
       <c r="J25">
-        <v>5.8476042502770857E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+        <v>0.007423663911901022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C26">
-        <v>2.198199620727985E-2</v>
+        <v>0.02198208155128326</v>
       </c>
       <c r="E26">
-        <v>5.9564232462569287E-3</v>
+        <v>0.005955619918224795</v>
       </c>
       <c r="F26">
-        <v>-1.390672644426905E-2</v>
+        <v>-0.01390672644426905</v>
       </c>
       <c r="H26">
-        <v>1.38342625693705E-2</v>
+        <v>0.0138342625693705</v>
       </c>
       <c r="I26">
-        <v>1.161479844859194E-2</v>
+        <v>0.01161479844859194</v>
       </c>
       <c r="J26">
-        <v>-1.2940584053835399E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.02320857139827741</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C27">
-        <v>2.228941845957674E-2</v>
+        <v>0.02229343423573736</v>
       </c>
       <c r="E27">
-        <v>-2.8772508382900332E-2</v>
+        <v>-0.02877268569490743</v>
       </c>
       <c r="F27">
-        <v>2.5703967140158681E-2</v>
+        <v>0.02570396714015868</v>
       </c>
       <c r="H27">
-        <v>-2.5679164195166561E-2</v>
+        <v>-0.02567916419516656</v>
       </c>
       <c r="I27">
-        <v>-2.17181802287272E-2</v>
+        <v>-0.0217181802287272</v>
       </c>
       <c r="J27">
-        <v>1.2179810615479611E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.02813557060668474</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C28">
-        <v>-1.376402301456092E-2</v>
+        <v>-0.01376714291868571</v>
       </c>
       <c r="E28">
-        <v>1.6876236099049442E-2</v>
+        <v>0.01687560902702436</v>
       </c>
       <c r="F28">
-        <v>-1.179589208783568E-2</v>
+        <v>-0.01179589208783568</v>
       </c>
       <c r="H28">
-        <v>1.1732409973296399E-2</v>
+        <v>0.0117324099732964</v>
       </c>
       <c r="I28">
-        <v>8.2587973863518949E-3</v>
+        <v>0.008258797386351895</v>
       </c>
       <c r="J28">
-        <v>-1.6712491605601312E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.005866782117671989</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C29">
-        <v>1.106015948240638E-2</v>
+        <v>0.01105898569035943</v>
       </c>
       <c r="E29">
-        <v>-5.5117984604719384E-3</v>
+        <v>-0.005511614332464572</v>
       </c>
       <c r="F29">
-        <v>6.3166174686646974E-3</v>
+        <v>0.006316617468664697</v>
       </c>
       <c r="H29">
-        <v>-6.3538307181532274E-3</v>
+        <v>-0.006353830718153227</v>
       </c>
       <c r="I29">
-        <v>-8.0306650892266029E-3</v>
+        <v>-0.008030665089226603</v>
       </c>
       <c r="J29">
-        <v>1.089234380240115E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-0.01448525091290828</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30">
-        <v>3.8272977210919079E-3</v>
+        <v>0.00382599826503993</v>
       </c>
       <c r="E30">
-        <v>5.0098979603959166E-3</v>
+        <v>0.005010308456412337</v>
       </c>
       <c r="F30">
-        <v>-2.1181993807279751E-3</v>
+        <v>-0.002118199380727975</v>
       </c>
       <c r="H30">
-        <v>2.1117693964707758E-3</v>
+        <v>0.002111769396470776</v>
       </c>
       <c r="I30">
-        <v>3.0671786186871439E-3</v>
+        <v>0.003067178618687144</v>
       </c>
       <c r="J30">
-        <v>-2.1808116186103E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.003722836878509105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C31">
-        <v>-7.5599982863999299E-3</v>
+        <v>-0.0075587925263517</v>
       </c>
       <c r="E31">
-        <v>1.726961963478478E-2</v>
+        <v>0.01726902241876089</v>
       </c>
       <c r="F31">
-        <v>-2.0975765159030602E-2</v>
+        <v>-0.0209757651590306</v>
       </c>
       <c r="H31">
-        <v>2.1012672168506889E-2</v>
+        <v>0.02101267216850689</v>
       </c>
       <c r="I31">
-        <v>1.505415967416639E-2</v>
+        <v>0.01505415967416639</v>
       </c>
       <c r="J31">
-        <v>1.263127517042416E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-0.002775566062005731</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C32">
-        <v>8.9167523246700929E-3</v>
+        <v>0.008915606756624268</v>
       </c>
       <c r="E32">
-        <v>3.5971343518853729E-3</v>
+        <v>0.003596433743857349</v>
       </c>
       <c r="F32">
-        <v>-2.4611565144462598E-3</v>
+        <v>-0.00246115651444626</v>
       </c>
       <c r="H32">
-        <v>2.4063489602539579E-3</v>
+        <v>0.002406348960253958</v>
       </c>
       <c r="I32">
-        <v>3.7544965021798602E-3</v>
+        <v>0.00375449650217986</v>
       </c>
       <c r="J32">
-        <v>7.8495657810936925E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.002286869203088693</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C33">
-        <v>6.1727913189116527E-3</v>
+        <v>0.006169412406776495</v>
       </c>
       <c r="E33">
-        <v>-1.873426922937076E-3</v>
+        <v>-0.001873167626926705</v>
       </c>
       <c r="F33">
-        <v>7.547397325895891E-3</v>
+        <v>0.007547397325895891</v>
       </c>
       <c r="H33">
-        <v>-7.6157373286294917E-3</v>
+        <v>-0.007615737328629492</v>
       </c>
       <c r="I33">
-        <v>-4.6081257523250298E-3</v>
+        <v>-0.00460812575232503</v>
       </c>
       <c r="J33">
-        <v>2.3809717127214031E-3</v>
+        <v>0.01459788492970327</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix up inconsistency in benchmark biorefinery; remove old results
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -638,10 +638,10 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>-0.02282848065713922</v>
+        <v>-0.02283115780924631</v>
       </c>
       <c r="E4">
-        <v>0.03252194914087796</v>
+        <v>0.03252158606886344</v>
       </c>
       <c r="F4">
         <v>-0.02345721060228842</v>
@@ -653,7 +653,7 @@
         <v>0.01824716780188671</v>
       </c>
       <c r="J4">
-        <v>-0.002045117860332284</v>
+        <v>-0.01001126144342611</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -662,10 +662,10 @@
         <v>33</v>
       </c>
       <c r="C5">
-        <v>0.007193248799729951</v>
+        <v>0.007191296927651877</v>
       </c>
       <c r="E5">
-        <v>0.02940805941632237</v>
+        <v>0.0294076926963077</v>
       </c>
       <c r="F5">
         <v>-0.02395886351835454</v>
@@ -677,7 +677,7 @@
         <v>0.02099920672796826</v>
       </c>
       <c r="J5">
-        <v>0.01881517031626738</v>
+        <v>0.009471818331361903</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -686,10 +686,10 @@
         <v>34</v>
       </c>
       <c r="C6">
-        <v>0.1519892917755716</v>
+        <v>0.1519870517114821</v>
       </c>
       <c r="E6">
-        <v>0.9382297877691913</v>
+        <v>0.9382294163451764</v>
       </c>
       <c r="F6">
         <v>-0.9999804825272192</v>
@@ -701,7 +701,7 @@
         <v>0.9586914095476562</v>
       </c>
       <c r="J6">
-        <v>0.03717130597819318</v>
+        <v>-0.002172398423935881</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -712,10 +712,10 @@
         <v>35</v>
       </c>
       <c r="C7">
-        <v>0.948402028624081</v>
+        <v>0.9484030940321236</v>
       </c>
       <c r="E7">
-        <v>-0.01072723041308921</v>
+        <v>-0.01072744132509765</v>
       </c>
       <c r="F7">
         <v>0.004923681892947275</v>
@@ -727,7 +727,7 @@
         <v>0.002488744899549796</v>
       </c>
       <c r="J7">
-        <v>-0.007348018100251941</v>
+        <v>0.007057077690483055</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -738,10 +738,10 @@
         <v>35</v>
       </c>
       <c r="C8">
-        <v>0.02251866032474641</v>
+        <v>0.0225188151727526</v>
       </c>
       <c r="E8">
-        <v>0.01356083689443347</v>
+        <v>0.01356077353443094</v>
       </c>
       <c r="F8">
         <v>-0.01314891086195643</v>
@@ -753,7 +753,7 @@
         <v>0.01808265845130633</v>
       </c>
       <c r="J8">
-        <v>-0.01008280875313502</v>
+        <v>0.01109177598846261</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -764,10 +764,10 @@
         <v>36</v>
       </c>
       <c r="C9">
-        <v>-0.004603344664133786</v>
+        <v>-0.004604815384192615</v>
       </c>
       <c r="E9">
-        <v>-0.007437610857504434</v>
+        <v>-0.007437114921484595</v>
       </c>
       <c r="F9">
         <v>0.01417645611905824</v>
@@ -779,7 +779,7 @@
         <v>-0.0166405299776212</v>
       </c>
       <c r="J9">
-        <v>-0.005956763129398836</v>
+        <v>-0.01220219018234914</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -790,10 +790,10 @@
         <v>37</v>
       </c>
       <c r="C10">
-        <v>0.04784763455390538</v>
+        <v>0.04784935650597425</v>
       </c>
       <c r="E10">
-        <v>0.0216985349799414</v>
+        <v>0.02169796397191855</v>
       </c>
       <c r="F10">
         <v>-0.01818195691927827</v>
@@ -805,7 +805,7 @@
         <v>0.01400161121606445</v>
       </c>
       <c r="J10">
-        <v>-0.004188052275484431</v>
+        <v>0.006567211724689074</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -814,10 +814,10 @@
         <v>38</v>
       </c>
       <c r="C11">
-        <v>0.1444196462567858</v>
+        <v>0.1444172317606893</v>
       </c>
       <c r="E11">
-        <v>0.003330694405227776</v>
+        <v>0.003330341797213672</v>
       </c>
       <c r="F11">
         <v>-0.007889097819563913</v>
@@ -829,7 +829,7 @@
         <v>0.283372950726918</v>
       </c>
       <c r="J11">
-        <v>0.01621422609533115</v>
+        <v>-0.005271696816414461</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -838,10 +838,10 @@
         <v>39</v>
       </c>
       <c r="C12">
-        <v>-0.1937712858948514</v>
+        <v>-0.1937698121987924</v>
       </c>
       <c r="E12">
-        <v>0.0126933899797356</v>
+        <v>0.01269399737175989</v>
       </c>
       <c r="F12">
         <v>-0.01446597360263894</v>
@@ -853,7 +853,7 @@
         <v>0.01842309193692368</v>
       </c>
       <c r="J12">
-        <v>0.006420499561071366</v>
+        <v>-0.003221754185824128</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -864,10 +864,10 @@
         <v>40</v>
       </c>
       <c r="C13">
-        <v>0.02240433948817358</v>
+        <v>0.02240781219231248</v>
       </c>
       <c r="E13">
-        <v>-0.001323309556932382</v>
+        <v>-0.001322413396896536</v>
       </c>
       <c r="F13">
         <v>0.00466661701866468</v>
@@ -879,7 +879,7 @@
         <v>-0.004888350915534036</v>
       </c>
       <c r="J13">
-        <v>0.0148806108589639</v>
+        <v>0.01383563057094249</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -890,10 +890,10 @@
         <v>40</v>
       </c>
       <c r="C14">
-        <v>5.877984235119369E-05</v>
+        <v>5.901744236069768E-05</v>
       </c>
       <c r="E14">
-        <v>-0.005466022202640888</v>
+        <v>-0.005465977850639113</v>
       </c>
       <c r="F14">
         <v>0.0001964740878589635</v>
@@ -905,7 +905,7 @@
         <v>-0.009953175374127014</v>
       </c>
       <c r="J14">
-        <v>-0.009907834521313514</v>
+        <v>-0.0006871099755667106</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -916,10 +916,10 @@
         <v>41</v>
       </c>
       <c r="C15">
-        <v>-0.01752412428496497</v>
+        <v>-0.01752631202905248</v>
       </c>
       <c r="E15">
-        <v>-0.007759412470376498</v>
+        <v>-0.007758804982352198</v>
       </c>
       <c r="F15">
         <v>0.007814835000593398</v>
@@ -931,7 +931,7 @@
         <v>-0.007891357275654291</v>
       </c>
       <c r="J15">
-        <v>0.004984996424747783</v>
+        <v>0.02159517101128804</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -942,10 +942,10 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>0.001623263680930547</v>
+        <v>0.001620135616805425</v>
       </c>
       <c r="E16">
-        <v>0.007825677625027104</v>
+        <v>0.007825959385038373</v>
       </c>
       <c r="F16">
         <v>-0.004067051682682067</v>
@@ -957,7 +957,7 @@
         <v>0.008303432108137283</v>
       </c>
       <c r="J16">
-        <v>0.02280240083207389</v>
+        <v>-0.01956840203256883</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -966,10 +966,10 @@
         <v>42</v>
       </c>
       <c r="C17">
-        <v>0.001363491990539679</v>
+        <v>0.00136514549460582</v>
       </c>
       <c r="E17">
-        <v>8.517312340692491E-06</v>
+        <v>7.960320318412811E-06</v>
       </c>
       <c r="F17">
         <v>-0.006272667994906719</v>
@@ -981,7 +981,7 @@
         <v>0.005896042603841703</v>
       </c>
       <c r="J17">
-        <v>-0.005541955651736855</v>
+        <v>-0.004315955290631166</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -992,10 +992,10 @@
         <v>43</v>
       </c>
       <c r="C18">
-        <v>0.01526711955468478</v>
+        <v>0.01526795734671829</v>
       </c>
       <c r="E18">
-        <v>0.002708350860334034</v>
+        <v>0.002708669676346787</v>
       </c>
       <c r="F18">
         <v>-0.001605290944211638</v>
@@ -1007,7 +1007,7 @@
         <v>-0.0002331010653240426</v>
       </c>
       <c r="J18">
-        <v>-0.03527657102737577</v>
+        <v>0.007453877028566195</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1018,10 +1018,10 @@
         <v>44</v>
       </c>
       <c r="C19">
-        <v>0.005929336653173466</v>
+        <v>0.005928089613123583</v>
       </c>
       <c r="E19">
-        <v>0.0006596974343878973</v>
+        <v>0.0006603959304158371</v>
       </c>
       <c r="F19">
         <v>0.000413647600545904</v>
@@ -1033,7 +1033,7 @@
         <v>0.002854861554194462</v>
       </c>
       <c r="J19">
-        <v>0.01205301617796706</v>
+        <v>-0.009818421305930008</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1042,10 +1042,10 @@
         <v>45</v>
       </c>
       <c r="C20">
-        <v>-0.01814623416584936</v>
+        <v>-0.0181484401499376</v>
       </c>
       <c r="E20">
-        <v>-0.006156975798279032</v>
+        <v>-0.006156371478254857</v>
       </c>
       <c r="F20">
         <v>0.004868278370731134</v>
@@ -1057,7 +1057,7 @@
         <v>-0.002026378833055153</v>
       </c>
       <c r="J20">
-        <v>0.007259576762824828</v>
+        <v>0.003543377342157545</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1066,10 +1066,10 @@
         <v>46</v>
       </c>
       <c r="C21">
-        <v>-0.02281394961655798</v>
+        <v>-0.022813675152547</v>
       </c>
       <c r="E21">
-        <v>0.01138105648724226</v>
+        <v>0.0113808977032359</v>
       </c>
       <c r="F21">
         <v>-0.004949300357972013</v>
@@ -1081,7 +1081,7 @@
         <v>0.003556671886266875</v>
       </c>
       <c r="J21">
-        <v>0.004871370891708491</v>
+        <v>0.008196569064025674</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1090,10 +1090,10 @@
         <v>47</v>
       </c>
       <c r="C22">
-        <v>-0.02214724850188994</v>
+        <v>-0.02214966990998679</v>
       </c>
       <c r="E22">
-        <v>-0.01159287550371502</v>
+        <v>-0.01159324654372986</v>
       </c>
       <c r="F22">
         <v>0.01105747474629899</v>
@@ -1105,7 +1105,7 @@
         <v>-0.01086898229075929</v>
       </c>
       <c r="J22">
-        <v>0.008408733523535534</v>
+        <v>0.006366690229209365</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1116,10 +1116,10 @@
         <v>48</v>
       </c>
       <c r="C23">
-        <v>-0.004626522137060884</v>
+        <v>-0.004630091513203659</v>
       </c>
       <c r="E23">
-        <v>-0.01230164286006571</v>
+        <v>-0.01230116593204664</v>
       </c>
       <c r="F23">
         <v>0.01396085643043425</v>
@@ -1131,7 +1131,7 @@
         <v>-0.01179273109570924</v>
       </c>
       <c r="J23">
-        <v>-0.007662212278717682</v>
+        <v>-0.01849373487128882</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1140,10 +1140,10 @@
         <v>49</v>
       </c>
       <c r="C24">
-        <v>-0.009810745928429836</v>
+        <v>-0.009812086472483458</v>
       </c>
       <c r="E24">
-        <v>0.007106787644271504</v>
+        <v>0.007106797916271916</v>
       </c>
       <c r="F24">
         <v>-0.01023005272920211</v>
@@ -1155,7 +1155,7 @@
         <v>0.01310582932423317</v>
       </c>
       <c r="J24">
-        <v>-0.02917054464679801</v>
+        <v>0.004913271513563789</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1166,10 +1166,10 @@
         <v>50</v>
       </c>
       <c r="C25">
-        <v>0.004659246522369861</v>
+        <v>0.004657418106296723</v>
       </c>
       <c r="E25">
-        <v>0.01962846270513851</v>
+        <v>0.01962831332913253</v>
       </c>
       <c r="F25">
         <v>-0.01705115981804639</v>
@@ -1181,7 +1181,7 @@
         <v>0.01985164889006595</v>
       </c>
       <c r="J25">
-        <v>0.007423663911901022</v>
+        <v>0.005847604250277086</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1190,10 +1190,10 @@
         <v>51</v>
       </c>
       <c r="C26">
-        <v>0.02198208155128326</v>
+        <v>0.02198199620727985</v>
       </c>
       <c r="E26">
-        <v>0.005955619918224795</v>
+        <v>0.005956423246256929</v>
       </c>
       <c r="F26">
         <v>-0.01390672644426905</v>
@@ -1205,7 +1205,7 @@
         <v>0.01161479844859194</v>
       </c>
       <c r="J26">
-        <v>0.02320857139827741</v>
+        <v>-0.0129405840538354</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1216,10 +1216,10 @@
         <v>52</v>
       </c>
       <c r="C27">
-        <v>0.02229343423573736</v>
+        <v>0.02228941845957674</v>
       </c>
       <c r="E27">
-        <v>-0.02877268569490743</v>
+        <v>-0.02877250838290033</v>
       </c>
       <c r="F27">
         <v>0.02570396714015868</v>
@@ -1231,7 +1231,7 @@
         <v>-0.0217181802287272</v>
       </c>
       <c r="J27">
-        <v>0.02813557060668474</v>
+        <v>0.001217981061547961</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1242,10 +1242,10 @@
         <v>53</v>
       </c>
       <c r="C28">
-        <v>-0.01376714291868571</v>
+        <v>-0.01376402301456092</v>
       </c>
       <c r="E28">
-        <v>0.01687560902702436</v>
+        <v>0.01687623609904944</v>
       </c>
       <c r="F28">
         <v>-0.01179589208783568</v>
@@ -1257,7 +1257,7 @@
         <v>0.008258797386351895</v>
       </c>
       <c r="J28">
-        <v>0.005866782117671989</v>
+        <v>-0.01671249160560131</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1268,10 +1268,10 @@
         <v>54</v>
       </c>
       <c r="C29">
-        <v>0.01105898569035943</v>
+        <v>0.01106015948240638</v>
       </c>
       <c r="E29">
-        <v>-0.005511614332464572</v>
+        <v>-0.005511798460471938</v>
       </c>
       <c r="F29">
         <v>0.006316617468664697</v>
@@ -1283,7 +1283,7 @@
         <v>-0.008030665089226603</v>
       </c>
       <c r="J29">
-        <v>-0.01448525091290828</v>
+        <v>0.01089234380240115</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1294,10 +1294,10 @@
         <v>55</v>
       </c>
       <c r="C30">
-        <v>0.00382599826503993</v>
+        <v>0.003827297721091908</v>
       </c>
       <c r="E30">
-        <v>0.005010308456412337</v>
+        <v>0.005009897960395917</v>
       </c>
       <c r="F30">
         <v>-0.002118199380727975</v>
@@ -1309,7 +1309,7 @@
         <v>0.003067178618687144</v>
       </c>
       <c r="J30">
-        <v>0.003722836878509105</v>
+        <v>-0.021808116186103</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1320,10 +1320,10 @@
         <v>56</v>
       </c>
       <c r="C31">
-        <v>-0.0075587925263517</v>
+        <v>-0.00755999828639993</v>
       </c>
       <c r="E31">
-        <v>0.01726902241876089</v>
+        <v>0.01726961963478478</v>
       </c>
       <c r="F31">
         <v>-0.0209757651590306</v>
@@ -1335,7 +1335,7 @@
         <v>0.01505415967416639</v>
       </c>
       <c r="J31">
-        <v>-0.002775566062005731</v>
+        <v>0.01263127517042416</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1346,10 +1346,10 @@
         <v>57</v>
       </c>
       <c r="C32">
-        <v>0.008915606756624268</v>
+        <v>0.008916752324670093</v>
       </c>
       <c r="E32">
-        <v>0.003596433743857349</v>
+        <v>0.003597134351885373</v>
       </c>
       <c r="F32">
         <v>-0.00246115651444626</v>
@@ -1361,7 +1361,7 @@
         <v>0.00375449650217986</v>
       </c>
       <c r="J32">
-        <v>0.002286869203088693</v>
+        <v>0.0007849565781093693</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1372,10 +1372,10 @@
         <v>58</v>
       </c>
       <c r="C33">
-        <v>0.006169412406776495</v>
+        <v>0.006172791318911653</v>
       </c>
       <c r="E33">
-        <v>-0.001873167626926705</v>
+        <v>-0.001873426922937076</v>
       </c>
       <c r="F33">
         <v>0.007547397325895891</v>
@@ -1387,7 +1387,7 @@
         <v>-0.00460812575232503</v>
       </c>
       <c r="J33">
-        <v>0.01459788492970327</v>
+        <v>0.002380971712721403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a few GWP values for uncertainty
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Element</t>
   </si>
@@ -25,6 +25,24 @@
     <t>Biorefinery</t>
   </si>
   <si>
+    <t>Biofuel displacement</t>
+  </si>
+  <si>
+    <t>Ethanol displacement</t>
+  </si>
+  <si>
+    <t>Biodiesel displacement</t>
+  </si>
+  <si>
+    <t>Biofuel allocation</t>
+  </si>
+  <si>
+    <t>Ethanol allocation</t>
+  </si>
+  <si>
+    <t>Biodiesel allocation</t>
+  </si>
+  <si>
     <t>MFPP [USD/ton]</t>
   </si>
   <si>
@@ -67,6 +85,15 @@
     <t>TCI derivative [10^6*USD]</t>
   </si>
   <si>
+    <t>GWP [kg*CO2*eq / GGE]</t>
+  </si>
+  <si>
+    <t>GWP [kg*CO2*eq / (ethanol*gal)]</t>
+  </si>
+  <si>
+    <t>GWP [kg*CO2*eq / (biodiesel*gal)]</t>
+  </si>
+  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -112,6 +139,9 @@
     <t>oilsorghum</t>
   </si>
   <si>
+    <t>Stream-sugarcane</t>
+  </si>
+  <si>
     <t>Oil retention [%]</t>
   </si>
   <si>
@@ -172,16 +202,16 @@
     <t>Productivity [g/L]</t>
   </si>
   <si>
-    <t>Cane  PL content [% oil]</t>
-  </si>
-  <si>
-    <t>Sorghum  PL content [% oil]</t>
-  </si>
-  <si>
-    <t>Cane  FFA content [% oil]</t>
-  </si>
-  <si>
-    <t>Sorghum  FFA content [% oil]</t>
+    <t>Cane PL content [% oil]</t>
+  </si>
+  <si>
+    <t>Sorghum PL content [% oil]</t>
+  </si>
+  <si>
+    <t>Cane FFA content [% oil]</t>
+  </si>
+  <si>
+    <t>Sorghum FFA content [% oil]</t>
   </si>
   <si>
     <t>Cane oil content [dry wt. %]</t>
@@ -190,7 +220,10 @@
     <t>Relative sorghum oil content [dry wt. %]</t>
   </si>
   <si>
-    <t>TAG to  FFA conversion [% oil]</t>
+    <t>TAG to FFA conversion [% oil]</t>
+  </si>
+  <si>
+    <t>GWP [kg*CO2-eq/kg]</t>
   </si>
 </sst>
 </file>
@@ -548,13 +581,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:22">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,820 +607,1254 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C4">
-        <v>-0.02283115780924631</v>
+        <v>-0.06604260426042603</v>
       </c>
       <c r="E4">
-        <v>0.03252158606886344</v>
+        <v>-0.02683468346834683</v>
       </c>
       <c r="F4">
-        <v>-0.02345721060228842</v>
+        <v>0.03665166516651665</v>
       </c>
       <c r="H4">
-        <v>0.02341656535266261</v>
+        <v>-0.03726372637263726</v>
       </c>
       <c r="I4">
-        <v>0.01824716780188671</v>
+        <v>-0.03924392439243924</v>
       </c>
       <c r="J4">
-        <v>-0.01001126144342611</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>-0.02216583578387608</v>
+      </c>
+      <c r="Q4">
+        <v>0.05554155415541554</v>
+      </c>
+      <c r="R4">
+        <v>0.05554155415541554</v>
+      </c>
+      <c r="T4">
+        <v>0.05796579657965795</v>
+      </c>
+      <c r="U4">
+        <v>0.05796579657965795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>0.007191296927651877</v>
+        <v>-0.1408460846084608</v>
       </c>
       <c r="E5">
-        <v>0.0294076926963077</v>
+        <v>-0.1469666966696669</v>
       </c>
       <c r="F5">
-        <v>-0.02395886351835454</v>
+        <v>0.1045424542454245</v>
       </c>
       <c r="H5">
-        <v>0.02398984742359389</v>
+        <v>-0.1050825082508251</v>
       </c>
       <c r="I5">
-        <v>0.02099920672796826</v>
+        <v>-0.1012421242124212</v>
       </c>
       <c r="J5">
-        <v>0.009471818331361903</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>0.03058164497986805</v>
+      </c>
+      <c r="Q5">
+        <v>-0.1188838883888389</v>
+      </c>
+      <c r="R5">
+        <v>-0.1188838883888389</v>
+      </c>
+      <c r="T5">
+        <v>-0.1162196219621962</v>
+      </c>
+      <c r="U5">
+        <v>-0.1162196219621962</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C6">
-        <v>0.1519870517114821</v>
+        <v>0.1576717671767177</v>
       </c>
       <c r="E6">
-        <v>0.9382294163451764</v>
+        <v>0.9746534653465345</v>
       </c>
       <c r="F6">
-        <v>-0.9999804825272192</v>
+        <v>-0.9999759975997599</v>
       </c>
       <c r="H6">
-        <v>0.9999999916479996</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="I6">
-        <v>0.9586914095476562</v>
+        <v>0.956111611161116</v>
       </c>
       <c r="J6">
-        <v>-0.002172398423935881</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>0.0858220313941023</v>
+      </c>
+      <c r="Q6">
+        <v>0.385058505850585</v>
+      </c>
+      <c r="R6">
+        <v>0.385058505850585</v>
+      </c>
+      <c r="T6">
+        <v>0.3195919591959195</v>
+      </c>
+      <c r="U6">
+        <v>0.3195919591959195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C7">
-        <v>0.9484030940321236</v>
+        <v>0.9537593759375936</v>
       </c>
       <c r="E7">
-        <v>-0.01072744132509765</v>
+        <v>0.03041104110411041</v>
       </c>
       <c r="F7">
-        <v>0.004923681892947275</v>
+        <v>-0.01006900690069007</v>
       </c>
       <c r="H7">
-        <v>-0.004825162561006502</v>
+        <v>0.01137713771377138</v>
       </c>
       <c r="I7">
-        <v>0.002488744899549796</v>
+        <v>0.009672967296729673</v>
       </c>
       <c r="J7">
-        <v>0.007057077690483055</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>0.1454114869431675</v>
+      </c>
+      <c r="Q7">
+        <v>0.07605160516051603</v>
+      </c>
+      <c r="R7">
+        <v>0.07605160516051603</v>
+      </c>
+      <c r="T7">
+        <v>0.07509150915091509</v>
+      </c>
+      <c r="U7">
+        <v>0.07509150915091509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>0.0225188151727526</v>
+        <v>-0.08213621362136211</v>
       </c>
       <c r="E8">
-        <v>0.01356077353443094</v>
+        <v>0.03974797479747975</v>
       </c>
       <c r="F8">
-        <v>-0.01314891086195643</v>
+        <v>-0.06273027302730272</v>
       </c>
       <c r="H8">
-        <v>0.01312995364519814</v>
+        <v>0.06263426342634262</v>
       </c>
       <c r="I8">
-        <v>0.01808265845130633</v>
+        <v>0.1098109810981098</v>
       </c>
       <c r="J8">
-        <v>0.01109177598846261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>-0.01097479186372401</v>
+      </c>
+      <c r="Q8">
+        <v>0.04832883288328833</v>
+      </c>
+      <c r="R8">
+        <v>0.04832883288328833</v>
+      </c>
+      <c r="T8">
+        <v>0.03831983198319831</v>
+      </c>
+      <c r="U8">
+        <v>0.03831983198319831</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>-0.004604815384192615</v>
+        <v>0.03217521752175218</v>
       </c>
       <c r="E9">
-        <v>-0.007437114921484595</v>
+        <v>-0.1171437143714371</v>
       </c>
       <c r="F9">
-        <v>0.01417645611905824</v>
+        <v>0.1023942394239424</v>
       </c>
       <c r="H9">
-        <v>-0.01424939039397561</v>
+        <v>-0.1036663666366636</v>
       </c>
       <c r="I9">
-        <v>-0.0166405299776212</v>
+        <v>-0.07396339633963396</v>
       </c>
       <c r="J9">
-        <v>-0.01220219018234914</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>-0.02093440046254963</v>
+      </c>
+      <c r="Q9">
+        <v>-0.1402460246024602</v>
+      </c>
+      <c r="R9">
+        <v>-0.1402460246024602</v>
+      </c>
+      <c r="T9">
+        <v>-0.1327572757275727</v>
+      </c>
+      <c r="U9">
+        <v>-0.1327572757275727</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C10">
-        <v>0.04784935650597425</v>
+        <v>0.1397539753975398</v>
       </c>
       <c r="E10">
-        <v>0.02169796397191855</v>
+        <v>0.08736873687368735</v>
       </c>
       <c r="F10">
-        <v>-0.01818195691927827</v>
+        <v>-0.07959195919591958</v>
       </c>
       <c r="H10">
-        <v>0.01806241377849655</v>
+        <v>0.0785118511851185</v>
       </c>
       <c r="I10">
-        <v>0.01400161121606445</v>
+        <v>0.09706570657065706</v>
       </c>
       <c r="J10">
-        <v>0.006567211724689074</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>0.03668475857239328</v>
+      </c>
+      <c r="Q10">
+        <v>0.02975097509750975</v>
+      </c>
+      <c r="R10">
+        <v>0.02975097509750975</v>
+      </c>
+      <c r="T10">
+        <v>0.0285028502850285</v>
+      </c>
+      <c r="U10">
+        <v>0.0285028502850285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C11">
-        <v>0.1444172317606893</v>
+        <v>0.08918091809180917</v>
       </c>
       <c r="E11">
-        <v>0.003330341797213672</v>
+        <v>-0.04456045604560455</v>
       </c>
       <c r="F11">
-        <v>-0.007889097819563913</v>
+        <v>0.04446444644464446</v>
       </c>
       <c r="H11">
-        <v>0.007686511507460459</v>
+        <v>-0.04451245124512451</v>
       </c>
       <c r="I11">
-        <v>0.283372950726918</v>
+        <v>0.2375037503750375</v>
       </c>
       <c r="J11">
-        <v>-0.005271696816414461</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>0.05812374716660838</v>
+      </c>
+      <c r="Q11">
+        <v>-0.06945094509450944</v>
+      </c>
+      <c r="R11">
+        <v>-0.06945094509450944</v>
+      </c>
+      <c r="T11">
+        <v>-0.06603060306030602</v>
+      </c>
+      <c r="U11">
+        <v>-0.06603060306030602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C12">
-        <v>-0.1937698121987924</v>
+        <v>-0.1439183918391839</v>
       </c>
       <c r="E12">
-        <v>0.01269399737175989</v>
+        <v>0.02556255625562556</v>
       </c>
       <c r="F12">
-        <v>-0.01446597360263894</v>
+        <v>-0.009900990099009899</v>
       </c>
       <c r="H12">
-        <v>0.01444677158587086</v>
+        <v>0.009384938493849384</v>
       </c>
       <c r="I12">
-        <v>0.01842309193692368</v>
+        <v>0.04852085208520851</v>
       </c>
       <c r="J12">
-        <v>-0.003221754185824128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>0.1326766436201818</v>
+      </c>
+      <c r="Q12">
+        <v>-0.1207440744074407</v>
+      </c>
+      <c r="R12">
+        <v>-0.1207440744074407</v>
+      </c>
+      <c r="T12">
+        <v>-0.1233483348334833</v>
+      </c>
+      <c r="U12">
+        <v>-0.1233483348334833</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>0.02240781219231248</v>
+        <v>0.1227122712271227</v>
       </c>
       <c r="E13">
-        <v>-0.001322413396896536</v>
+        <v>-0.005268526852685268</v>
       </c>
       <c r="F13">
-        <v>0.00466661701866468</v>
+        <v>-0.007236723672367236</v>
       </c>
       <c r="H13">
-        <v>-0.00473076825323073</v>
+        <v>0.0066006600660066</v>
       </c>
       <c r="I13">
-        <v>-0.004888350915534036</v>
+        <v>0.008148814881488147</v>
       </c>
       <c r="J13">
-        <v>0.01383563057094249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>0.05211073859759484</v>
+      </c>
+      <c r="Q13">
+        <v>-0.07633963396339634</v>
+      </c>
+      <c r="R13">
+        <v>-0.07633963396339634</v>
+      </c>
+      <c r="T13">
+        <v>-0.08379237923792378</v>
+      </c>
+      <c r="U13">
+        <v>-0.08379237923792378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C14">
-        <v>5.901744236069768E-05</v>
+        <v>-0.005292529252925292</v>
       </c>
       <c r="E14">
-        <v>-0.005465977850639113</v>
+        <v>0.1214041404140414</v>
       </c>
       <c r="F14">
-        <v>0.0001964740878589635</v>
+        <v>-0.1278487848784878</v>
       </c>
       <c r="H14">
-        <v>-0.0001528324861132994</v>
+        <v>0.1266846684668467</v>
       </c>
       <c r="I14">
-        <v>-0.009953175374127014</v>
+        <v>0.1162676267626763</v>
       </c>
       <c r="J14">
-        <v>-0.0006871099755667106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>-0.09062162564649173</v>
+      </c>
+      <c r="Q14">
+        <v>0.1981758175817582</v>
+      </c>
+      <c r="R14">
+        <v>0.1981758175817582</v>
+      </c>
+      <c r="T14">
+        <v>0.1923432343234323</v>
+      </c>
+      <c r="U14">
+        <v>0.1923432343234323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C15">
-        <v>-0.01752631202905248</v>
+        <v>0.03108310831083108</v>
       </c>
       <c r="E15">
-        <v>-0.007758804982352198</v>
+        <v>-0.06135013501350134</v>
       </c>
       <c r="F15">
-        <v>0.007814835000593398</v>
+        <v>0.08298829882988298</v>
       </c>
       <c r="H15">
-        <v>-0.007782896567315861</v>
+        <v>-0.08392439243924392</v>
       </c>
       <c r="I15">
-        <v>-0.007891357275654291</v>
+        <v>-0.04128412841284127</v>
       </c>
       <c r="J15">
-        <v>0.02159517101128804</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>0.003015514786857938</v>
+      </c>
+      <c r="Q15">
+        <v>-0.2860606060606061</v>
+      </c>
+      <c r="R15">
+        <v>-0.2860606060606061</v>
+      </c>
+      <c r="T15">
+        <v>-0.283072307230723</v>
+      </c>
+      <c r="U15">
+        <v>-0.283072307230723</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C16">
-        <v>0.001620135616805425</v>
+        <v>0.1163756375637564</v>
       </c>
       <c r="E16">
-        <v>0.007825959385038373</v>
+        <v>0.2263546354635463</v>
       </c>
       <c r="F16">
-        <v>-0.004067051682682067</v>
+        <v>-0.2246744674467446</v>
       </c>
       <c r="H16">
-        <v>0.004078764355150573</v>
+        <v>0.225010501050105</v>
       </c>
       <c r="I16">
-        <v>0.008303432108137283</v>
+        <v>0.2248784878487848</v>
       </c>
       <c r="J16">
-        <v>-0.01956840203256883</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>0.06715227052247985</v>
+      </c>
+      <c r="Q16">
+        <v>0.1121632163216321</v>
+      </c>
+      <c r="R16">
+        <v>0.1121632163216321</v>
+      </c>
+      <c r="T16">
+        <v>0.09034503450345033</v>
+      </c>
+      <c r="U16">
+        <v>0.09034503450345033</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C17">
-        <v>0.00136514549460582</v>
+        <v>0.1392499249924992</v>
       </c>
       <c r="E17">
-        <v>7.960320318412811E-06</v>
+        <v>0.1282808280828083</v>
       </c>
       <c r="F17">
-        <v>-0.006272667994906719</v>
+        <v>-0.1326732673267327</v>
       </c>
       <c r="H17">
-        <v>0.006518461796738471</v>
+        <v>0.1329132913291329</v>
       </c>
       <c r="I17">
-        <v>0.005896042603841703</v>
+        <v>0.09747374737473745</v>
       </c>
       <c r="J17">
-        <v>-0.004315955290631166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>0.07644510194731896</v>
+      </c>
+      <c r="Q17">
+        <v>0.08946894689468947</v>
+      </c>
+      <c r="R17">
+        <v>0.08946894689468947</v>
+      </c>
+      <c r="T17">
+        <v>0.08675667566756674</v>
+      </c>
+      <c r="U17">
+        <v>0.08675667566756674</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C18">
-        <v>0.01526795734671829</v>
+        <v>-0.1599159915991599</v>
       </c>
       <c r="E18">
-        <v>0.002708669676346787</v>
+        <v>-0.01333333333333333</v>
       </c>
       <c r="F18">
-        <v>-0.001605290944211638</v>
+        <v>-0.008712871287128712</v>
       </c>
       <c r="H18">
-        <v>0.00154255926170237</v>
+        <v>0.009876987698769876</v>
       </c>
       <c r="I18">
-        <v>-0.0002331010653240426</v>
+        <v>0.01243324332433243</v>
       </c>
       <c r="J18">
-        <v>0.007453877028566195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>-0.02670112196729788</v>
+      </c>
+      <c r="Q18">
+        <v>-0.1032463246324632</v>
+      </c>
+      <c r="R18">
+        <v>-0.1032463246324632</v>
+      </c>
+      <c r="T18">
+        <v>-0.107962796279628</v>
+      </c>
+      <c r="U18">
+        <v>-0.107962796279628</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C19">
-        <v>0.005928089613123583</v>
+        <v>-0.05548154815481547</v>
       </c>
       <c r="E19">
-        <v>0.0006603959304158371</v>
+        <v>-0.05245724572457245</v>
       </c>
       <c r="F19">
-        <v>0.000413647600545904</v>
+        <v>0.03287128712871287</v>
       </c>
       <c r="H19">
-        <v>-0.0003596484623859385</v>
+        <v>-0.03201920192019202</v>
       </c>
       <c r="I19">
-        <v>0.002854861554194462</v>
+        <v>0.01947794779477947</v>
       </c>
       <c r="J19">
-        <v>-0.009818421305930008</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>-0.03256996249869271</v>
+      </c>
+      <c r="Q19">
+        <v>0.02353435343534353</v>
+      </c>
+      <c r="R19">
+        <v>0.02353435343534353</v>
+      </c>
+      <c r="T19">
+        <v>0.01546954695469547</v>
+      </c>
+      <c r="U19">
+        <v>0.01546954695469547</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C20">
-        <v>-0.0181484401499376</v>
+        <v>-0.009108910891089108</v>
       </c>
       <c r="E20">
-        <v>-0.006156371478254857</v>
+        <v>0.07162316231623163</v>
       </c>
       <c r="F20">
-        <v>0.004868278370731134</v>
+        <v>-0.07403540354035403</v>
       </c>
       <c r="H20">
-        <v>-0.004806710400268415</v>
+        <v>0.07455145514551455</v>
       </c>
       <c r="I20">
-        <v>-0.002026378833055153</v>
+        <v>0.07039903990399039</v>
       </c>
       <c r="J20">
-        <v>0.003543377342157545</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>0.09724134137381732</v>
+      </c>
+      <c r="Q20">
+        <v>0.06622262226222622</v>
+      </c>
+      <c r="R20">
+        <v>0.06622262226222622</v>
+      </c>
+      <c r="T20">
+        <v>0.06665466546654665</v>
+      </c>
+      <c r="U20">
+        <v>0.06665466546654665</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C21">
-        <v>-0.022813675152547</v>
+        <v>-0.09054905490549055</v>
       </c>
       <c r="E21">
-        <v>0.0113808977032359</v>
+        <v>0.1561716171617162</v>
       </c>
       <c r="F21">
-        <v>-0.004949300357972013</v>
+        <v>-0.1542634263426343</v>
       </c>
       <c r="H21">
-        <v>0.005052600202104007</v>
+        <v>0.1544194419441944</v>
       </c>
       <c r="I21">
-        <v>0.003556671886266875</v>
+        <v>0.1648244824482448</v>
       </c>
       <c r="J21">
-        <v>0.008196569064025674</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>0.003622221945169993</v>
+      </c>
+      <c r="Q21">
+        <v>-0.01266126612661266</v>
+      </c>
+      <c r="R21">
+        <v>-0.01266126612661266</v>
+      </c>
+      <c r="T21">
+        <v>-0.02486648664866487</v>
+      </c>
+      <c r="U21">
+        <v>-0.02486648664866487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C22">
-        <v>-0.02214966990998679</v>
+        <v>-9.6009600960096E-05</v>
       </c>
       <c r="E22">
-        <v>-0.01159324654372986</v>
+        <v>-0.04351635163516351</v>
       </c>
       <c r="F22">
-        <v>0.01105747474629899</v>
+        <v>0.05843384338433843</v>
       </c>
       <c r="H22">
-        <v>-0.01103848815353952</v>
+        <v>-0.05785778577857785</v>
       </c>
       <c r="I22">
-        <v>-0.01086898229075929</v>
+        <v>-0.01126912691269127</v>
       </c>
       <c r="J22">
-        <v>0.006366690229209365</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>-0.1363889705888635</v>
+      </c>
+      <c r="Q22">
+        <v>-0.1145874587458746</v>
+      </c>
+      <c r="R22">
+        <v>-0.1145874587458746</v>
+      </c>
+      <c r="T22">
+        <v>-0.1138073807380738</v>
+      </c>
+      <c r="U22">
+        <v>-0.1138073807380738</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C23">
-        <v>-0.004630091513203659</v>
+        <v>0.1173957395739574</v>
       </c>
       <c r="E23">
-        <v>-0.01230116593204664</v>
+        <v>0.01300930093009301</v>
       </c>
       <c r="F23">
-        <v>0.01396085643043425</v>
+        <v>-0.02618661866186618</v>
       </c>
       <c r="H23">
-        <v>-0.01408289105931564</v>
+        <v>0.02562256225622562</v>
       </c>
       <c r="I23">
-        <v>-0.01179273109570924</v>
+        <v>0.03677167716771677</v>
       </c>
       <c r="J23">
-        <v>-0.01849373487128882</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>0.1552990115231838</v>
+      </c>
+      <c r="Q23">
+        <v>0.07606360636063604</v>
+      </c>
+      <c r="R23">
+        <v>0.07606360636063604</v>
+      </c>
+      <c r="T23">
+        <v>0.08091209120912089</v>
+      </c>
+      <c r="U23">
+        <v>0.08091209120912089</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C24">
-        <v>-0.009812086472483458</v>
+        <v>-0.01976597659765976</v>
       </c>
       <c r="E24">
-        <v>0.007106797916271916</v>
+        <v>-0.1635403540354035</v>
       </c>
       <c r="F24">
-        <v>-0.01023005272920211</v>
+        <v>0.1628202820282028</v>
       </c>
       <c r="H24">
-        <v>0.01027197593087904</v>
+        <v>-0.1625802580258026</v>
       </c>
       <c r="I24">
-        <v>0.01310582932423317</v>
+        <v>-0.1768616861686169</v>
       </c>
       <c r="J24">
-        <v>0.004913271513563789</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>-0.04174265389218289</v>
+      </c>
+      <c r="Q24">
+        <v>-0.02907890789078908</v>
+      </c>
+      <c r="R24">
+        <v>-0.02907890789078908</v>
+      </c>
+      <c r="T24">
+        <v>-0.02621062106210621</v>
+      </c>
+      <c r="U24">
+        <v>-0.02621062106210621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C25">
-        <v>0.004657418106296723</v>
+        <v>0.04985298529852985</v>
       </c>
       <c r="E25">
-        <v>0.01962831332913253</v>
+        <v>-0.02125412541254125</v>
       </c>
       <c r="F25">
-        <v>-0.01705115981804639</v>
+        <v>0.03380738073807381</v>
       </c>
       <c r="H25">
-        <v>0.01705464893818595</v>
+        <v>-0.03348334833483348</v>
       </c>
       <c r="I25">
-        <v>0.01985164889006595</v>
+        <v>-0.03613561356135613</v>
       </c>
       <c r="J25">
-        <v>0.005847604250277086</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>0.07168154970433421</v>
+      </c>
+      <c r="Q25">
+        <v>0.02307830783078308</v>
+      </c>
+      <c r="R25">
+        <v>0.02307830783078308</v>
+      </c>
+      <c r="T25">
+        <v>0.02634263426342634</v>
+      </c>
+      <c r="U25">
+        <v>0.02634263426342634</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C26">
-        <v>0.02198199620727985</v>
+        <v>0.07595559555955594</v>
       </c>
       <c r="E26">
-        <v>0.005956423246256929</v>
+        <v>0.0312991299129913</v>
       </c>
       <c r="F26">
-        <v>-0.01390672644426905</v>
+        <v>-0.02588658865886588</v>
       </c>
       <c r="H26">
-        <v>0.0138342625693705</v>
+        <v>0.02624662466246624</v>
       </c>
       <c r="I26">
-        <v>0.01161479844859194</v>
+        <v>0.03127512751275127</v>
       </c>
       <c r="J26">
-        <v>-0.0129405840538354</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>-0.1170884745526592</v>
+      </c>
+      <c r="Q26">
+        <v>0.002112211221122112</v>
+      </c>
+      <c r="R26">
+        <v>0.002112211221122112</v>
+      </c>
+      <c r="T26">
+        <v>0.009300930093009299</v>
+      </c>
+      <c r="U26">
+        <v>0.009300930093009299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C27">
-        <v>0.02228941845957674</v>
+        <v>-0.1043024302430243</v>
       </c>
       <c r="E27">
-        <v>-0.02877250838290033</v>
+        <v>-0.1461026102610261</v>
       </c>
       <c r="F27">
-        <v>0.02570396714015868</v>
+        <v>0.1484188418841884</v>
       </c>
       <c r="H27">
-        <v>-0.02567916419516656</v>
+        <v>-0.1480708070807081</v>
       </c>
       <c r="I27">
-        <v>-0.0217181802287272</v>
+        <v>-0.1595679567956796</v>
       </c>
       <c r="J27">
-        <v>0.001217981061547961</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>-0.007658926998493768</v>
+      </c>
+      <c r="Q27">
+        <v>-0.008568856885688569</v>
+      </c>
+      <c r="R27">
+        <v>-0.008568856885688569</v>
+      </c>
+      <c r="T27">
+        <v>0.003012301230123012</v>
+      </c>
+      <c r="U27">
+        <v>0.003012301230123012</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C28">
-        <v>-0.01376402301456092</v>
+        <v>0.1525832583258326</v>
       </c>
       <c r="E28">
-        <v>0.01687623609904944</v>
+        <v>0.1101710171017102</v>
       </c>
       <c r="F28">
-        <v>-0.01179589208783568</v>
+        <v>-0.09564956495649564</v>
       </c>
       <c r="H28">
-        <v>0.0117324099732964</v>
+        <v>0.09641764176417641</v>
       </c>
       <c r="I28">
-        <v>0.008258797386351895</v>
+        <v>0.07170717071707169</v>
       </c>
       <c r="J28">
-        <v>-0.01671249160560131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>0.09846076269200887</v>
+      </c>
+      <c r="Q28">
+        <v>0.01736573657365736</v>
+      </c>
+      <c r="R28">
+        <v>0.01736573657365736</v>
+      </c>
+      <c r="T28">
+        <v>0.01203720372037204</v>
+      </c>
+      <c r="U28">
+        <v>0.01203720372037204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C29">
-        <v>0.01106015948240638</v>
+        <v>-0.03871587158715871</v>
       </c>
       <c r="E29">
-        <v>-0.005511798460471938</v>
+        <v>-0.08841284128412841</v>
       </c>
       <c r="F29">
-        <v>0.006316617468664697</v>
+        <v>0.04622862286228623</v>
       </c>
       <c r="H29">
-        <v>-0.006353830718153227</v>
+        <v>-0.04607260726072606</v>
       </c>
       <c r="I29">
-        <v>-0.008030665089226603</v>
+        <v>-0.09708970897089708</v>
       </c>
       <c r="J29">
-        <v>0.01089234380240115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>-0.06079085586255445</v>
+      </c>
+      <c r="Q29">
+        <v>-0.01137713771377138</v>
+      </c>
+      <c r="R29">
+        <v>-0.01137713771377138</v>
+      </c>
+      <c r="T29">
+        <v>-0.004584458445844585</v>
+      </c>
+      <c r="U29">
+        <v>-0.004584458445844585</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C30">
-        <v>0.003827297721091908</v>
+        <v>-0.006636663666366636</v>
       </c>
       <c r="E30">
-        <v>0.005009897960395917</v>
+        <v>0.07914791479147913</v>
       </c>
       <c r="F30">
-        <v>-0.002118199380727975</v>
+        <v>-0.07059105910591058</v>
       </c>
       <c r="H30">
-        <v>0.002111769396470776</v>
+        <v>0.07042304230423042</v>
       </c>
       <c r="I30">
-        <v>0.003067178618687144</v>
+        <v>0.04447644764476447</v>
       </c>
       <c r="J30">
-        <v>-0.021808116186103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>0.02548170064910632</v>
+      </c>
+      <c r="Q30">
+        <v>0.01393339333933393</v>
+      </c>
+      <c r="R30">
+        <v>0.01393339333933393</v>
+      </c>
+      <c r="T30">
+        <v>0.01054905490549055</v>
+      </c>
+      <c r="U30">
+        <v>0.01054905490549055</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C31">
-        <v>-0.00755999828639993</v>
+        <v>-0.05066906690669067</v>
       </c>
       <c r="E31">
-        <v>0.01726961963478478</v>
+        <v>0.03894389438943893</v>
       </c>
       <c r="F31">
-        <v>-0.0209757651590306</v>
+        <v>-0.07699969996999699</v>
       </c>
       <c r="H31">
-        <v>0.02101267216850689</v>
+        <v>0.07746774677467745</v>
       </c>
       <c r="I31">
-        <v>0.01505415967416639</v>
+        <v>0.1172757275727573</v>
       </c>
       <c r="J31">
-        <v>0.01263127517042416</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>-0.0006247281630143935</v>
+      </c>
+      <c r="Q31">
+        <v>0.1258925892589259</v>
+      </c>
+      <c r="R31">
+        <v>0.1258925892589259</v>
+      </c>
+      <c r="T31">
+        <v>0.122976297629763</v>
+      </c>
+      <c r="U31">
+        <v>0.122976297629763</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C32">
-        <v>0.008916752324670093</v>
+        <v>-0.07854785478547853</v>
       </c>
       <c r="E32">
-        <v>0.003597134351885373</v>
+        <v>0.01951395139513951</v>
       </c>
       <c r="F32">
-        <v>-0.00246115651444626</v>
+        <v>-0.002712271227122712</v>
       </c>
       <c r="H32">
-        <v>0.002406348960253958</v>
+        <v>0.002112211221122112</v>
       </c>
       <c r="I32">
-        <v>0.00375449650217986</v>
+        <v>0.04094809480948094</v>
       </c>
       <c r="J32">
-        <v>0.0007849565781093693</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>-0.035267106202476</v>
+      </c>
+      <c r="Q32">
+        <v>-0.04021602160216022</v>
+      </c>
+      <c r="R32">
+        <v>-0.04021602160216022</v>
+      </c>
+      <c r="T32">
+        <v>-0.04664866486648664</v>
+      </c>
+      <c r="U32">
+        <v>-0.04664866486648664</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C33">
-        <v>0.006172791318911653</v>
+        <v>-0.06088208820882088</v>
       </c>
       <c r="E33">
-        <v>-0.001873426922937076</v>
+        <v>-0.2295589558955895</v>
       </c>
       <c r="F33">
-        <v>0.007547397325895891</v>
+        <v>0.2412241224122412</v>
       </c>
       <c r="H33">
-        <v>-0.007615737328629492</v>
+        <v>-0.2402040204020402</v>
       </c>
       <c r="I33">
-        <v>-0.00460812575232503</v>
+        <v>-0.1809780978097809</v>
       </c>
       <c r="J33">
-        <v>0.002380971712721403</v>
+        <v>0.1417352019838905</v>
+      </c>
+      <c r="Q33">
+        <v>-0.2486048604860486</v>
+      </c>
+      <c r="R33">
+        <v>-0.2486048604860486</v>
+      </c>
+      <c r="T33">
+        <v>-0.2358715871587159</v>
+      </c>
+      <c r="U33">
+        <v>-0.2358715871587159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34">
+        <v>0.1355775577557756</v>
+      </c>
+      <c r="E34">
+        <v>0.2594539453945394</v>
+      </c>
+      <c r="F34">
+        <v>-0.254977497749775</v>
+      </c>
+      <c r="H34">
+        <v>0.2555775577557756</v>
+      </c>
+      <c r="I34">
+        <v>0.2303030303030303</v>
+      </c>
+      <c r="J34">
+        <v>0.006998156826074696</v>
+      </c>
+      <c r="Q34">
+        <v>0.9895109510951094</v>
+      </c>
+      <c r="R34">
+        <v>0.9895109510951094</v>
+      </c>
+      <c r="T34">
+        <v>0.997143714371437</v>
+      </c>
+      <c r="U34">
+        <v>0.997143714371437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plot enhancements; unique flowsheet names for each configuration
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -624,7 +624,7 @@
       </c>
       <c r="N2" s="1" t="inlineStr">
         <is>
-          <t>Crude glycerol GWP [kg*CO2*eq / gal]</t>
+          <t>Crude glycerol GWP [kg*CO2*eq / kg]</t>
         </is>
       </c>
       <c r="O2" s="1" t="inlineStr">
@@ -712,37 +712,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.2142694269426942</v>
+        <v>0.05563909774436089</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>-0.1006060606060606</v>
+        <v>-0.1548872180451128</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.05488148814881488</v>
+        <v>-0.1759398496240602</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.06948694869486949</v>
+        <v>-0.1233082706766917</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09986198619861984</v>
+        <v>0.2661654135338345</v>
       </c>
       <c r="I4" t="n">
-        <v>0.06405040504050405</v>
+        <v>0.4135338345864661</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.1590212314955781</v>
+        <v>-0.3206626056029393</v>
       </c>
       <c r="K4" t="n">
-        <v>0.123000300030003</v>
+        <v>0.2917293233082707</v>
       </c>
       <c r="L4" t="n">
-        <v>0.123000300030003</v>
+        <v>0.2917293233082707</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.123000300030003</v>
+        <v>0.2917293233082707</v>
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
@@ -764,37 +764,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.08664866486648665</v>
+        <v>-0.1353383458646616</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.07689168916891688</v>
+        <v>-0.1488721804511278</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1146114611461146</v>
+        <v>-0.3714285714285714</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1372697269726973</v>
+        <v>-0.1774436090225564</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.1017341734173417</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.1119111911191119</v>
+        <v>0.2255639097744361</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.06434971870560277</v>
+        <v>0.1505458242267321</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0849204920492049</v>
+        <v>0.2511278195488721</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.0849204920492049</v>
+        <v>0.2511278195488721</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>-0.0849204920492049</v>
+        <v>0.2511278195488721</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -816,37 +816,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1722772277227723</v>
+        <v>-0.1263157894736842</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>-0.5007020702070206</v>
+        <v>-0.6631578947368421</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.9757335733573358</v>
+        <v>-0.9609022556390976</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.5129672967296729</v>
+        <v>-0.6360902255639098</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9561716171617161</v>
+        <v>0.9368421052631578</v>
       </c>
       <c r="J6" t="n">
-        <v>0.01649438323210914</v>
+        <v>-0.3266844385720086</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9836423642364235</v>
+        <v>0.9924812030075187</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9836423642364235</v>
+        <v>0.9924812030075187</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.9836423642364235</v>
+        <v>0.9924812030075187</v>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -872,37 +872,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.943090309030903</v>
+        <v>0.9203007518796992</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.1772457245724572</v>
+        <v>0.2992481203007519</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.05153315331533153</v>
+        <v>0.3759398496240601</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1625802580258026</v>
+        <v>0.2691729323308271</v>
       </c>
       <c r="H7" t="n">
-        <v>0.003672367236723672</v>
+        <v>-0.3864661654135338</v>
       </c>
       <c r="I7" t="n">
-        <v>0.004668466846684667</v>
+        <v>-0.2947368421052631</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2143068481264347</v>
+        <v>0.3703427275977609</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.04529252925292529</v>
+        <v>-0.4060150375939849</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.04529252925292529</v>
+        <v>-0.4060150375939849</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.04529252925292529</v>
+        <v>-0.4060150375939849</v>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
@@ -928,37 +928,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.09864986498649862</v>
+        <v>0.2496240601503759</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.07693969396939694</v>
+        <v>0.2736842105263158</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.03693969396939693</v>
+        <v>0.150375939849624</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06499849984998499</v>
+        <v>0.2330827067669173</v>
       </c>
       <c r="H8" t="n">
-        <v>0.02007800780078008</v>
+        <v>-0.2932330827067668</v>
       </c>
       <c r="I8" t="n">
-        <v>0.001404140414041404</v>
+        <v>-0.3849624060150376</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1346640850985633</v>
+        <v>0.08505839068810363</v>
       </c>
       <c r="K8" t="n">
-        <v>0.01359735973597359</v>
+        <v>-0.3293233082706767</v>
       </c>
       <c r="L8" t="n">
-        <v>0.01359735973597359</v>
+        <v>-0.3293233082706767</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>0.01359735973597359</v>
+        <v>-0.3293233082706767</v>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -984,37 +984,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.04628862886288628</v>
+        <v>-0.312781954887218</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>-0.1634443444344434</v>
+        <v>0.07368421052631578</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01285328532853285</v>
+        <v>0.2421052631578947</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.1663486348634863</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01807380738073807</v>
+        <v>-0.2526315789473684</v>
       </c>
       <c r="I9" t="n">
-        <v>0.04094809480948094</v>
+        <v>-0.3969924812030075</v>
       </c>
       <c r="J9" t="n">
-        <v>0.03130689199044167</v>
+        <v>0.2589388176699792</v>
       </c>
       <c r="K9" t="n">
-        <v>0.03842784278427842</v>
+        <v>-0.2421052631578947</v>
       </c>
       <c r="L9" t="n">
-        <v>0.03842784278427842</v>
+        <v>-0.2421052631578947</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.03842784278427842</v>
+        <v>-0.2421052631578947</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
@@ -1040,37 +1040,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.01092109210921092</v>
+        <v>0.1458646616541353</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>0.137065706570657</v>
+        <v>-0.3263157894736842</v>
       </c>
       <c r="F10" t="n">
-        <v>0.04940894089408941</v>
+        <v>-0.2842105263157895</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1606000600060006</v>
+        <v>-0.318796992481203</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.04614461446144614</v>
+        <v>0.2496240601503759</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.0417041704170417</v>
+        <v>0.1759398496240602</v>
       </c>
       <c r="J10" t="n">
-        <v>0.04408313129659467</v>
+        <v>0.1881822802834151</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0484008400840084</v>
+        <v>0.2240601503759398</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.0484008400840084</v>
+        <v>0.2240601503759398</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>-0.0484008400840084</v>
+        <v>0.2240601503759398</v>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
@@ -1092,37 +1092,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1472187218721872</v>
+        <v>0.3097744360902255</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>-0.05594959495949594</v>
+        <v>0.06616541353383458</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02771077107710771</v>
+        <v>0.3909774436090225</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.04553255325532552</v>
+        <v>0.06917293233082707</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.03181518151815181</v>
+        <v>-0.3172932330827067</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2451005100510051</v>
+        <v>-0.004511278195488721</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.04995767856571438</v>
+        <v>0.1031238895953115</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.03183918391839183</v>
+        <v>-0.2947368421052631</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.03183918391839183</v>
+        <v>-0.2947368421052631</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.03183918391839183</v>
+        <v>-0.2947368421052631</v>
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
@@ -1144,37 +1144,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.2177017701770177</v>
+        <v>-0.1323308270676692</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>-0.1722892289228923</v>
+        <v>0.05864661654135337</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1079387938793879</v>
+        <v>0.4812030075187969</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.1584518451845184</v>
+        <v>0.03909774436090225</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.08556855685568555</v>
+        <v>-0.4030075187969925</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.1068946894689469</v>
+        <v>-0.3714285714285714</v>
       </c>
       <c r="J12" t="n">
-        <v>0.01941363678302139</v>
+        <v>0.117425742896851</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.05772577257725772</v>
+        <v>-0.3684210526315789</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.05772577257725772</v>
+        <v>-0.3684210526315789</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>-0.05772577257725772</v>
+        <v>-0.3684210526315789</v>
       </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
@@ -1200,37 +1200,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.02475847584758476</v>
+        <v>-0.4135338345864661</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>0.07867986798679868</v>
+        <v>-0.193984962406015</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.02754275427542754</v>
+        <v>-0.3037593984962406</v>
       </c>
       <c r="G13" t="n">
-        <v>0.06207020702070207</v>
+        <v>-0.1819548872180451</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01018901890189019</v>
+        <v>0.3097744360902255</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.01854185418541854</v>
+        <v>0.2225563909774436</v>
       </c>
       <c r="J13" t="n">
-        <v>0.04097166352010796</v>
+        <v>0.1309748670772569</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.01957395739573957</v>
+        <v>0.3233082706766917</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.01957395739573957</v>
+        <v>0.3233082706766917</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>-0.01957395739573957</v>
+        <v>0.3233082706766917</v>
       </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
@@ -1256,37 +1256,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.009792979297929792</v>
+        <v>0.09624060150375939</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>-0.1476987698769877</v>
+        <v>-0.4</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0282028202820282</v>
+        <v>-0.2902255639097744</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.1452385238523852</v>
+        <v>-0.4330827067669173</v>
       </c>
       <c r="H14" t="n">
-        <v>0.03548754875487549</v>
+        <v>0.2481203007518797</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01683768376837684</v>
+        <v>0.1729323308270676</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.1416258440810886</v>
+        <v>0.3402335627524145</v>
       </c>
       <c r="K14" t="n">
-        <v>0.05102910291029103</v>
+        <v>0.2015037593984962</v>
       </c>
       <c r="L14" t="n">
-        <v>0.05102910291029103</v>
+        <v>0.2015037593984962</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>0.05102910291029103</v>
+        <v>0.2015037593984962</v>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
@@ -1312,37 +1312,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.09810981098109808</v>
+        <v>0.150375939849624</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>-0.05542154215421542</v>
+        <v>0.2195488721804511</v>
       </c>
       <c r="F15" t="n">
-        <v>0.04398439843984397</v>
+        <v>0.1518796992481203</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.04934893489348934</v>
+        <v>0.2345864661654135</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.03284728472847284</v>
+        <v>-0.08270676691729321</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.04474047404740474</v>
+        <v>-0.01052631578947368</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.04753097396783672</v>
+        <v>0.02333460275514347</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.02378637863786378</v>
+        <v>-0.07518796992481201</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.02378637863786378</v>
+        <v>-0.07518796992481201</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.02378637863786378</v>
+        <v>-0.07518796992481201</v>
       </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1368,37 +1368,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.0123972397239724</v>
+        <v>0.1308270676691729</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>0.005172517251725172</v>
+        <v>0.1022556390977443</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.02883888388838883</v>
+        <v>-0.007518796992481202</v>
       </c>
       <c r="G16" t="n">
-        <v>0.02143414341434143</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="H16" t="n">
-        <v>0.04448844884488448</v>
+        <v>-0.1203007518796992</v>
       </c>
       <c r="I16" t="n">
-        <v>0.03991599159915991</v>
+        <v>-0.263157894736842</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1195452349182214</v>
+        <v>0.1588258445592023</v>
       </c>
       <c r="K16" t="n">
-        <v>0.05237323732373236</v>
+        <v>-0.1548872180451128</v>
       </c>
       <c r="L16" t="n">
-        <v>0.05237323732373236</v>
+        <v>-0.1548872180451128</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.05237323732373236</v>
+        <v>-0.1548872180451128</v>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
@@ -1420,37 +1420,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.07038703870387038</v>
+        <v>-0.05864661654135337</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>0.08645664566456644</v>
+        <v>-0.3398496240601503</v>
       </c>
       <c r="F17" t="n">
-        <v>0.07135913591359135</v>
+        <v>-0.1969924812030075</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1094509450945094</v>
+        <v>-0.3203007518796992</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.05272127212721272</v>
+        <v>0.3172932330827067</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.0794119411941194</v>
+        <v>0.3248120300751879</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.1624390406940741</v>
+        <v>-0.124200304987054</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.04244824482448245</v>
+        <v>0.3533834586466165</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.04244824482448245</v>
+        <v>0.3533834586466165</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.04244824482448245</v>
+        <v>0.3533834586466165</v>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
@@ -1476,37 +1476,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.02318631863186318</v>
+        <v>0.1639097744360902</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
-        <v>0.09156915691569155</v>
+        <v>0.004511278195488721</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.0126972697269727</v>
+        <v>0.1007518796992481</v>
       </c>
       <c r="G18" t="n">
-        <v>0.07222322232223222</v>
+        <v>0.003007518796992481</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.02072607260726072</v>
+        <v>-0.1112781954887218</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.04709270927092709</v>
+        <v>-0.1819548872180451</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.05012586601309205</v>
+        <v>0.2627024632756475</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.03653165316531653</v>
+        <v>-0.1473684210526316</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.03653165316531653</v>
+        <v>-0.1473684210526316</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.03653165316531653</v>
+        <v>-0.1473684210526316</v>
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
@@ -1532,37 +1532,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.154983498349835</v>
+        <v>0.1007518796992481</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>0.06012601260126012</v>
+        <v>0.1488721804511278</v>
       </c>
       <c r="F19" t="n">
-        <v>0.01197719771977197</v>
+        <v>-0.09473684210526315</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03583558355835583</v>
+        <v>0.1744360902255639</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.01914191419141914</v>
+        <v>0.05413533834586466</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001716171617161716</v>
+        <v>-0.004511278195488721</v>
       </c>
       <c r="J19" t="n">
-        <v>0.03569177901135925</v>
+        <v>-0.0474219346314206</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.02901890189018901</v>
+        <v>0.05864661654135337</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.02901890189018901</v>
+        <v>0.05864661654135337</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>-0.02901890189018901</v>
+        <v>0.05864661654135337</v>
       </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
@@ -1584,37 +1584,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.009876987698769876</v>
+        <v>-0.2406015037593985</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>0.07399939993999401</v>
+        <v>-0.2360902255639098</v>
       </c>
       <c r="F20" t="n">
-        <v>0.004308430843084308</v>
+        <v>-0.1894736842105263</v>
       </c>
       <c r="G20" t="n">
-        <v>0.07295529552955295</v>
+        <v>-0.1984962406015038</v>
       </c>
       <c r="H20" t="n">
-        <v>0.01422142214221422</v>
+        <v>0.2706766917293233</v>
       </c>
       <c r="I20" t="n">
-        <v>0.02013801380138014</v>
+        <v>0.03759398496240601</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.1100786843086788</v>
+        <v>-0.3778700188090975</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0138013801380138</v>
+        <v>0.2887218045112782</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0138013801380138</v>
+        <v>0.2887218045112782</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0.0138013801380138</v>
+        <v>0.2887218045112782</v>
       </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
@@ -1636,37 +1636,37 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.04484848484848484</v>
+        <v>0.38796992481203</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>-0.02312631263126312</v>
+        <v>-0.1714285714285714</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.08493249324932492</v>
+        <v>-0.1909774436090226</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.009708970897089709</v>
+        <v>-0.1428571428571428</v>
       </c>
       <c r="H21" t="n">
-        <v>0.08284428442844284</v>
+        <v>0.2766917293233083</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1197239723972397</v>
+        <v>0.3398496240601503</v>
       </c>
       <c r="J21" t="n">
-        <v>0.09630533370735828</v>
+        <v>0.05344376760048989</v>
       </c>
       <c r="K21" t="n">
-        <v>0.08669666966696668</v>
+        <v>0.3142857142857143</v>
       </c>
       <c r="L21" t="n">
-        <v>0.08669666966696668</v>
+        <v>0.3142857142857143</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0.08669666966696668</v>
+        <v>0.3142857142857143</v>
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -1688,37 +1688,37 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.02149414941494149</v>
+        <v>-0.07368421052631578</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>0.1367176717671767</v>
+        <v>0.06015037593984961</v>
       </c>
       <c r="F22" t="n">
-        <v>0.096009600960096</v>
+        <v>0.1699248120300751</v>
       </c>
       <c r="G22" t="n">
-        <v>0.1266606660666066</v>
+        <v>0.04511278195488722</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.1008460846084608</v>
+        <v>-0.1984962406015038</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.1012901290129013</v>
+        <v>-0.1849624060150376</v>
       </c>
       <c r="J22" t="n">
-        <v>0.08160695214546058</v>
+        <v>-0.1565676571958013</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.1178397839783978</v>
+        <v>-0.1909774436090226</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.1178397839783978</v>
+        <v>-0.1909774436090226</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>-0.1178397839783978</v>
+        <v>-0.1909774436090226</v>
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -1744,37 +1744,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.06064206420642063</v>
+        <v>0.009022556390977442</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>0.05971797179717971</v>
+        <v>0.02556390977443609</v>
       </c>
       <c r="F23" t="n">
-        <v>0.06269426942694269</v>
+        <v>-0.3097744360902255</v>
       </c>
       <c r="G23" t="n">
-        <v>0.07109510951095108</v>
+        <v>0.03609022556390977</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.03285928592859286</v>
+        <v>0.2</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.08976897689768974</v>
+        <v>0.08872180451127819</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.0786096115654087</v>
+        <v>0.08656384893037093</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.03353135313531352</v>
+        <v>0.1593984962406015</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.03353135313531352</v>
+        <v>0.1593984962406015</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>-0.03353135313531352</v>
+        <v>0.1593984962406015</v>
       </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
@@ -1796,37 +1796,37 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.01510951095109511</v>
+        <v>-0.2661654135338345</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>0.01696969696969697</v>
+        <v>-0.06015037593984961</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1010861086108611</v>
+        <v>-0.04962406015037594</v>
       </c>
       <c r="G24" t="n">
-        <v>0.02417041704170417</v>
+        <v>-0.05563909774436089</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.09218121812181217</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.07839183918391837</v>
+        <v>-0.02556390977443609</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.05102086350092318</v>
+        <v>-0.3710954567188945</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.08784878487848785</v>
+        <v>0.08421052631578946</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.08784878487848785</v>
+        <v>0.08421052631578946</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>-0.08784878487848785</v>
+        <v>0.08421052631578946</v>
       </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
@@ -1852,37 +1852,37 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.05132913291329132</v>
+        <v>-0.03308270676691729</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>-0.1608880888088809</v>
+        <v>0.4300751879699248</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.2331473147314731</v>
+        <v>0.6300751879699248</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.1615841584158416</v>
+        <v>0.431578947368421</v>
       </c>
       <c r="H25" t="n">
-        <v>0.2555295529552955</v>
+        <v>-0.6270676691729322</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2316951695169517</v>
+        <v>-0.6285714285714286</v>
       </c>
       <c r="J25" t="n">
-        <v>0.1357993503683625</v>
+        <v>0.2830261495462563</v>
       </c>
       <c r="K25" t="n">
-        <v>0.2676027602760275</v>
+        <v>-0.6330827067669172</v>
       </c>
       <c r="L25" t="n">
-        <v>0.2676027602760275</v>
+        <v>-0.6330827067669172</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.2676027602760275</v>
+        <v>-0.6330827067669172</v>
       </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
@@ -1904,37 +1904,37 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-0.08942094209420941</v>
+        <v>0.07518796992481201</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>-0.1163756375637564</v>
+        <v>0.1338345864661654</v>
       </c>
       <c r="F26" t="n">
-        <v>0.02543054305430542</v>
+        <v>0.05112781954887217</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.1291449144914491</v>
+        <v>0.1308270676691729</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.04523252325232523</v>
+        <v>-0.04962406015037594</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.06897089708970895</v>
+        <v>-0.0706766917293233</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.03594406018242574</v>
+        <v>0.2310878401880337</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.04656465646564656</v>
+        <v>-0.05714285714285714</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.04656465646564656</v>
+        <v>-0.05714285714285714</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>-0.04656465646564656</v>
+        <v>-0.05714285714285714</v>
       </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
@@ -1960,37 +1960,37 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-0.07533153315331532</v>
+        <v>0.3293233082706767</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>-0.0497089708970897</v>
+        <v>0.1894736842105263</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.09916591659165916</v>
+        <v>0.3834586466165413</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.03732373237323732</v>
+        <v>0.1759398496240602</v>
       </c>
       <c r="H27" t="n">
-        <v>0.1097389738973897</v>
+        <v>-0.4105263157894736</v>
       </c>
       <c r="I27" t="n">
-        <v>0.1291689168916892</v>
+        <v>-0.4406015037593984</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.009208262743926915</v>
+        <v>0.08581111980923728</v>
       </c>
       <c r="K27" t="n">
-        <v>0.1137473747374737</v>
+        <v>-0.3969924812030075</v>
       </c>
       <c r="L27" t="n">
-        <v>0.1137473747374737</v>
+        <v>-0.3969924812030075</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>0.1137473747374737</v>
+        <v>-0.3969924812030075</v>
       </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
@@ -2016,37 +2016,37 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.208016801680168</v>
+        <v>0.1007518796992481</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>0.03657965796579658</v>
+        <v>0.08721804511278194</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0586978697869787</v>
+        <v>0.06315789473684209</v>
       </c>
       <c r="G28" t="n">
-        <v>0.06135013501350134</v>
+        <v>0.1233082706766917</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.067998799879988</v>
+        <v>-0.02706766917293233</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.05515751575157515</v>
+        <v>0.1398496240601504</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.01671663093042962</v>
+        <v>-0.1859240929200141</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.06637863786378637</v>
+        <v>-0.01954887218045112</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.06637863786378637</v>
+        <v>-0.01954887218045112</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.06637863786378637</v>
+        <v>-0.01954887218045112</v>
       </c>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
@@ -2072,37 +2072,37 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.06007800780078007</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>0.03504350435043504</v>
+        <v>-0.1774436090225564</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1424662466246625</v>
+        <v>-0.07969924812030074</v>
       </c>
       <c r="G29" t="n">
-        <v>0.06954695469546954</v>
+        <v>-0.1759398496240602</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.1164116411641164</v>
+        <v>0.07218045112781954</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.1674407440744074</v>
+        <v>0.2135338345864662</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.05932211536792056</v>
+        <v>0.03387281045101471</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.1005460546054605</v>
+        <v>0.07368421052631578</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.1005460546054605</v>
+        <v>0.07368421052631578</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>-0.1005460546054605</v>
+        <v>0.07368421052631578</v>
       </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
@@ -2128,37 +2128,37 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.1958475847584758</v>
+        <v>-0.5624060150375939</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>0.06255025502550254</v>
+        <v>0.118796992481203</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.02995499549954995</v>
+        <v>0.3774436090225564</v>
       </c>
       <c r="G30" t="n">
-        <v>0.05417341734173416</v>
+        <v>0.1233082706766917</v>
       </c>
       <c r="H30" t="n">
-        <v>0.01424542454245424</v>
+        <v>-0.3548872180451128</v>
       </c>
       <c r="I30" t="n">
-        <v>0.03482748274827482</v>
+        <v>-0.5263157894736841</v>
       </c>
       <c r="J30" t="n">
-        <v>0.1745965904616593</v>
+        <v>-0.1354912418040589</v>
       </c>
       <c r="K30" t="n">
-        <v>0.008628862886288629</v>
+        <v>-0.3203007518796992</v>
       </c>
       <c r="L30" t="n">
-        <v>0.008628862886288629</v>
+        <v>-0.3203007518796992</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>0.008628862886288629</v>
+        <v>-0.3203007518796992</v>
       </c>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
@@ -2184,37 +2184,37 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.000624062406240624</v>
+        <v>0.112781954887218</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>-0.06022202220222022</v>
+        <v>-0.2721804511278195</v>
       </c>
       <c r="F31" t="n">
-        <v>0.03945994599459946</v>
+        <v>0.1263157894736842</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.04014401440144014</v>
+        <v>-0.2977443609022556</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.03247524752475248</v>
+        <v>-0.1593984962406015</v>
       </c>
       <c r="I31" t="n">
-        <v>0.015997599759976</v>
+        <v>-0.09924812030075188</v>
       </c>
       <c r="J31" t="n">
-        <v>0.04130803841486327</v>
+        <v>0.5058339694018198</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.01903390339033903</v>
+        <v>-0.162406015037594</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.01903390339033903</v>
+        <v>-0.162406015037594</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.01903390339033903</v>
+        <v>-0.162406015037594</v>
       </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
@@ -2240,37 +2240,37 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.008616861686168617</v>
+        <v>-0.07669172932330826</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>-0.05164116411641164</v>
+        <v>-0.05714285714285714</v>
       </c>
       <c r="F32" t="n">
-        <v>0.1492589258925892</v>
+        <v>0.3488721804511278</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.04978097809780978</v>
+        <v>-0.08872180451127819</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.1241884188418842</v>
+        <v>-0.356390977443609</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.1639483948394839</v>
+        <v>-0.3894736842105262</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.006505250196785941</v>
+        <v>0.4538956600435972</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.1159675967596759</v>
+        <v>-0.3368421052631578</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.1159675967596759</v>
+        <v>-0.3368421052631578</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>-0.1159675967596759</v>
+        <v>-0.3368421052631578</v>
       </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
@@ -2296,37 +2296,37 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.02912691269126912</v>
+        <v>0.5729323308270676</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>0.1338973897389739</v>
+        <v>-0.2496240601503759</v>
       </c>
       <c r="F33" t="n">
-        <v>0.004692469246924692</v>
+        <v>0.01804511278195488</v>
       </c>
       <c r="G33" t="n">
-        <v>0.1126672667266727</v>
+        <v>-0.263157894736842</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.03152715271527153</v>
+        <v>0.04060150375939849</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.03914791479147915</v>
+        <v>0.09172932330827067</v>
       </c>
       <c r="J33" t="n">
-        <v>0.1546904047256033</v>
+        <v>0.2544224429431772</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.04937293729372937</v>
+        <v>0.04210526315789473</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.04937293729372937</v>
+        <v>0.04210526315789473</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>-0.04937293729372937</v>
+        <v>0.04210526315789473</v>
       </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
@@ -2352,37 +2352,37 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.1161596159615961</v>
+        <v>-0.1007518796992481</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>0.02269426942694269</v>
+        <v>-0.2601503759398496</v>
       </c>
       <c r="F34" t="n">
-        <v>0.07075907590759076</v>
+        <v>-0.5518796992481202</v>
       </c>
       <c r="G34" t="n">
-        <v>0.06719471947194719</v>
+        <v>-0.2345864661654135</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.07822382238223821</v>
+        <v>0.5097744360902255</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.0833123312331233</v>
+        <v>0.4406015037593984</v>
       </c>
       <c r="J34" t="n">
-        <v>0.01281227947344821</v>
+        <v>-0.2702297544869841</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.07236723672367236</v>
+        <v>0.5037593984962406</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.07236723672367236</v>
+        <v>0.5037593984962406</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>-0.07236723672367236</v>
+        <v>0.5037593984962406</v>
       </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
@@ -2408,37 +2408,37 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.0395079507950795</v>
+        <v>0.03609022556390977</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>-0.1086588658865886</v>
+        <v>-0.3263157894736842</v>
       </c>
       <c r="F35" t="n">
-        <v>0.053009300930093</v>
+        <v>-0.2781954887218045</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.09082508250825082</v>
+        <v>-0.3609022556390977</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.01656165616561656</v>
+        <v>0.2135338345864662</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01956195619561956</v>
+        <v>0.1984962406015038</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.148203174612465</v>
+        <v>-0.0587128714484255</v>
       </c>
       <c r="K35" t="n">
-        <v>0.02381038103810381</v>
+        <v>0.1864661654135338</v>
       </c>
       <c r="L35" t="n">
-        <v>0.02381038103810381</v>
+        <v>0.1864661654135338</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>0.02381038103810381</v>
+        <v>0.1864661654135338</v>
       </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2464,37 +2464,37 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.00066006600660066</v>
+        <v>-0.118796992481203</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>0.1148394839483948</v>
+        <v>-0.07969924812030074</v>
       </c>
       <c r="F36" t="n">
-        <v>0.06101410141014101</v>
+        <v>-0.1834586466165413</v>
       </c>
       <c r="G36" t="n">
-        <v>0.09200120012001199</v>
+        <v>-0.05112781954887217</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.08973297329732971</v>
+        <v>0.2225563909774436</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.07501950195019501</v>
+        <v>0.1263157894736842</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.02357627610561849</v>
+        <v>-0.1369967000463262</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.1158355835583558</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.1158355835583558</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>-0.1158355835583558</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2520,37 +2520,37 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.09422142214221421</v>
+        <v>-0.237593984962406</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>0.05423342334233423</v>
+        <v>-0.06917293233082707</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.02459045904590459</v>
+        <v>-0.1819548872180451</v>
       </c>
       <c r="G37" t="n">
-        <v>0.05065706570657066</v>
+        <v>-0.05864661654135337</v>
       </c>
       <c r="H37" t="n">
-        <v>0.001272127212721272</v>
+        <v>0.1458646616541353</v>
       </c>
       <c r="I37" t="n">
-        <v>0.03245124512451245</v>
+        <v>0.08120300751879699</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.09408285672415347</v>
+        <v>0.2137750704019596</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.00192019201920192</v>
+        <v>0.1022556390977443</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.00192019201920192</v>
+        <v>0.1022556390977443</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.00192019201920192</v>
+        <v>0.1022556390977443</v>
       </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>

</xml_diff>

<commit_message>
add lca option for spearman plots; continue running simulations
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -629,7 +629,7 @@
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>Electricity GWP [kg*CO2*eq / kWhr]</t>
+          <t>Electricity GWP [kg*CO2*eq / MWhr]</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="Z2" s="1" t="inlineStr">
         <is>
-          <t>Electricity GWP derivative [kg*CO2*eq / kWhr]</t>
+          <t>Electricity GWP derivative [kg*CO2*eq / MWhr]</t>
         </is>
       </c>
     </row>
@@ -712,37 +712,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.05563909774436089</v>
+        <v>-0.02582761082510443</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>-0.1548872180451128</v>
+        <v>0.006278448059137922</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1759398496240602</v>
+        <v>0.005803265320130611</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.1233082706766917</v>
+        <v>0.005166825806673031</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2661654135338345</v>
+        <v>-0.007810884600435383</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4135338345864661</v>
+        <v>-0.006983176887327074</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.3206626056029393</v>
+        <v>0.01034820081595253</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2917293233082707</v>
+        <v>-0.00942725576909023</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2917293233082707</v>
+        <v>-0.00942725576909023</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.2917293233082707</v>
+        <v>-0.00942725576909023</v>
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
@@ -764,37 +764,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.1353383458646616</v>
+        <v>0.009941885197675407</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>-0.1488721804511278</v>
+        <v>-0.01076371550254862</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.3714285714285714</v>
+        <v>-0.002943337845733513</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.1774436090225564</v>
+        <v>-0.01042122185684887</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.005611729184469167</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2255639097744361</v>
+        <v>-0.0005059528522381141</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1505458242267321</v>
+        <v>0.01439178879278135</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2511278195488721</v>
+        <v>0.008641389945655597</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2511278195488721</v>
+        <v>0.008641389945655597</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.2511278195488721</v>
+        <v>0.008641389945655597</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -816,37 +816,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.1263157894736842</v>
+        <v>0.158945951061838</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>-0.6631578947368421</v>
+        <v>-0.4252339828013593</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.9609022556390976</v>
+        <v>-0.9727317469732697</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.6360902255639098</v>
+        <v>-0.4361537471741498</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0.9999930934717236</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9368421052631578</v>
+        <v>0.9579628848145153</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.3266844385720086</v>
+        <v>-0.01835997333905618</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9924812030075187</v>
+        <v>0.9802030376081213</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9924812030075187</v>
+        <v>0.9802030376081213</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.9924812030075187</v>
+        <v>0.9802030376081213</v>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -872,37 +872,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9203007518796992</v>
+        <v>0.9482859892914394</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.2992481203007519</v>
+        <v>0.002671719466868778</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3759398496240601</v>
+        <v>-0.006566324614652984</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2691729323308271</v>
+        <v>0.004238152585526103</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.3864661654135338</v>
+        <v>0.005660149378405975</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.2947368421052631</v>
+        <v>0.001493300027732001</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3703427275977609</v>
+        <v>-0.01887500478741833</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.4060150375939849</v>
+        <v>0.005702059044082361</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.4060150375939849</v>
+        <v>0.005702059044082361</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.4060150375939849</v>
+        <v>0.005702059044082361</v>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
@@ -928,37 +928,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.2496240601503759</v>
+        <v>-0.01275827580633103</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.2736842105263158</v>
+        <v>0.001623828064953122</v>
       </c>
       <c r="F8" t="n">
-        <v>0.150375939849624</v>
+        <v>0.01358628371145135</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2330827067669173</v>
+        <v>-0.001084707979388319</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.2932330827067668</v>
+        <v>-0.01304992429799697</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.3849624060150376</v>
+        <v>-0.009443602841744113</v>
       </c>
       <c r="J8" t="n">
-        <v>0.08505839068810363</v>
+        <v>0.007431583434837585</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.3293233082706767</v>
+        <v>-0.01153103393324135</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.3293233082706767</v>
+        <v>-0.01153103393324135</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>-0.3293233082706767</v>
+        <v>-0.01153103393324135</v>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -984,37 +984,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.312781954887218</v>
+        <v>0.01983799989751999</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>0.07368421052631578</v>
+        <v>-0.0136505576340223</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2421052631578947</v>
+        <v>-0.02406639168265566</v>
       </c>
       <c r="G9" t="n">
-        <v>0.05263157894736842</v>
+        <v>-0.01554824058992962</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.2526315789473684</v>
+        <v>0.02699373976774959</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.3969924812030075</v>
+        <v>0.02935640968625638</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2589388176699792</v>
+        <v>-0.00249073472405112</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.2421052631578947</v>
+        <v>0.02667502052300081</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.2421052631578947</v>
+        <v>0.02667502052300081</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>-0.2421052631578947</v>
+        <v>0.02667502052300081</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
@@ -1040,37 +1040,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.1458646616541353</v>
+        <v>0.02683866232154649</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>-0.3263157894736842</v>
+        <v>0.00660486554419462</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.2842105263157895</v>
+        <v>-0.001898852811954112</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.318796992481203</v>
+        <v>0.0008686074587442983</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2496240601503759</v>
+        <v>-0.001876327467053099</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1759398496240602</v>
+        <v>-0.0009429528377181134</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1881822802834151</v>
+        <v>-0.02529717439324946</v>
       </c>
       <c r="K10" t="n">
-        <v>0.2240601503759398</v>
+        <v>-0.002920339988813599</v>
       </c>
       <c r="L10" t="n">
-        <v>0.2240601503759398</v>
+        <v>-0.002920339988813599</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>0.2240601503759398</v>
+        <v>-0.002920339988813599</v>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
@@ -1092,37 +1092,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.3097744360902255</v>
+        <v>0.1137545369661815</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>0.06616541353383458</v>
+        <v>-0.00762312904092516</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3909774436090225</v>
+        <v>0.006939077557563101</v>
       </c>
       <c r="G11" t="n">
-        <v>0.06917293233082707</v>
+        <v>-0.008018200832728032</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.3172932330827067</v>
+        <v>-0.005576928127077125</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.004511278195488721</v>
+        <v>0.2739322870212915</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1031238895953115</v>
+        <v>-0.007289651238349656</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.2947368421052631</v>
+        <v>-0.002553755334150213</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.2947368421052631</v>
+        <v>-0.002553755334150213</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.2947368421052631</v>
+        <v>-0.002553755334150213</v>
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
@@ -1144,37 +1144,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.1323308270676692</v>
+        <v>-0.2321533771901351</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.05864661654135337</v>
+        <v>-0.002522963908918556</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4812030075187969</v>
+        <v>-0.01039102553564102</v>
       </c>
       <c r="G12" t="n">
-        <v>0.03909774436090225</v>
+        <v>-0.008845866209834647</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.4030075187969925</v>
+        <v>0.007154029918161196</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.3714285714285714</v>
+        <v>0.00596510827060433</v>
       </c>
       <c r="J12" t="n">
-        <v>0.117425742896851</v>
+        <v>0.005757202250523404</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.3684210526315789</v>
+        <v>0.004525499701019987</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.3684210526315789</v>
+        <v>0.004525499701019987</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>-0.3684210526315789</v>
+        <v>0.004525499701019987</v>
       </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
@@ -1200,37 +1200,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.4135338345864661</v>
+        <v>0.01056698269467931</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>-0.193984962406015</v>
+        <v>0.02040668990426759</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.3037593984962406</v>
+        <v>-0.01779460784778431</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1819548872180451</v>
+        <v>0.01958194235127769</v>
       </c>
       <c r="H13" t="n">
-        <v>0.3097744360902255</v>
+        <v>0.01394767476590699</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2225563909774436</v>
+        <v>0.008566614198664566</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1309748670772569</v>
+        <v>-0.006673082067163705</v>
       </c>
       <c r="K13" t="n">
-        <v>0.3233082706766917</v>
+        <v>0.01025061641002466</v>
       </c>
       <c r="L13" t="n">
-        <v>0.3233082706766917</v>
+        <v>0.01025061641002466</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>0.3233082706766917</v>
+        <v>0.01025061641002466</v>
       </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
@@ -1256,37 +1256,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.09624060150375939</v>
+        <v>-0.004903858948154358</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>-0.4</v>
+        <v>0.008945898405835935</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.2902255639097744</v>
+        <v>0.003007147128285884</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.4330827067669173</v>
+        <v>0.01225993345039734</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2481203007518797</v>
+        <v>-0.003247164897886596</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1729323308270676</v>
+        <v>-0.007119685916787436</v>
       </c>
       <c r="J14" t="n">
-        <v>0.3402335627524145</v>
+        <v>-0.01391352199389795</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2015037593984962</v>
+        <v>-0.00433883201355328</v>
       </c>
       <c r="L14" t="n">
-        <v>0.2015037593984962</v>
+        <v>-0.00433883201355328</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>0.2015037593984962</v>
+        <v>-0.00433883201355328</v>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
@@ -1312,37 +1312,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.150375939849624</v>
+        <v>0.006596756999870279</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>0.2195488721804511</v>
+        <v>0.01075373860614954</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1518796992481203</v>
+        <v>0.01240032184001287</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2345864661654135</v>
+        <v>0.01594537974181519</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.08270676691729321</v>
+        <v>-0.01226752810670112</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.01052631578947368</v>
+        <v>-0.01063130442525218</v>
       </c>
       <c r="J15" t="n">
-        <v>0.02333460275514347</v>
+        <v>0.007173397252697429</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.07518796992481201</v>
+        <v>-0.01096236312649452</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.07518796992481201</v>
+        <v>-0.01096236312649452</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.07518796992481201</v>
+        <v>-0.01096236312649452</v>
       </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1368,37 +1368,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.1308270676691729</v>
+        <v>0.02327230931489237</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>0.1022556390977443</v>
+        <v>0.007150765822030632</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.007518796992481202</v>
+        <v>-0.01200855734434229</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05263157894736842</v>
+        <v>0.001330667957226718</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.1203007518796992</v>
+        <v>0.009131315309252611</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.263157894736842</v>
+        <v>0.01187364479494579</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1588258445592023</v>
+        <v>-0.01514818011141934</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.1548872180451128</v>
+        <v>0.007138775613551023</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.1548872180451128</v>
+        <v>0.007138775613551023</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>-0.1548872180451128</v>
+        <v>0.007138775613551023</v>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
@@ -1420,37 +1420,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.05864661654135337</v>
+        <v>-0.001097359435894377</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>-0.3398496240601503</v>
+        <v>-0.01232639924505597</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.1969924812030075</v>
+        <v>0.01436509583860383</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.3203007518796992</v>
+        <v>-0.01240728184029127</v>
       </c>
       <c r="H17" t="n">
-        <v>0.3172932330827067</v>
+        <v>-0.007947437693897507</v>
       </c>
       <c r="I17" t="n">
-        <v>0.3248120300751879</v>
+        <v>-0.006570467302818691</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.124200304987054</v>
+        <v>0.0005686332642127915</v>
       </c>
       <c r="K17" t="n">
-        <v>0.3533834586466165</v>
+        <v>-0.005129341165173646</v>
       </c>
       <c r="L17" t="n">
-        <v>0.3533834586466165</v>
+        <v>-0.005129341165173646</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>0.3533834586466165</v>
+        <v>-0.005129341165173646</v>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
@@ -1476,37 +1476,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.1639097744360902</v>
+        <v>-0.0195531300621252</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
-        <v>0.004511278195488721</v>
+        <v>0.003402976552119061</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1007518796992481</v>
+        <v>0.009063783434551336</v>
       </c>
       <c r="G18" t="n">
-        <v>0.003007518796992481</v>
+        <v>0.005157989294319571</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.1112781954887218</v>
+        <v>-0.007303009156120366</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.1819548872180451</v>
+        <v>-0.004741255389650215</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2627024632756475</v>
+        <v>-0.01372789824304994</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.1473684210526316</v>
+        <v>-0.004396976431879056</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.1473684210526316</v>
+        <v>-0.004396976431879056</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.1473684210526316</v>
+        <v>-0.004396976431879056</v>
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
@@ -1532,37 +1532,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.1007518796992481</v>
+        <v>-0.01570813618032544</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>0.1488721804511278</v>
+        <v>0.004782966719318668</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.09473684210526315</v>
+        <v>0.005556496734259868</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1744360902255639</v>
+        <v>0.005297462227898488</v>
       </c>
       <c r="H19" t="n">
-        <v>0.05413533834586466</v>
+        <v>-0.006599684135987364</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.004511278195488721</v>
+        <v>-0.005024797256991891</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.0474219346314206</v>
+        <v>0.01025525899862456</v>
       </c>
       <c r="K19" t="n">
-        <v>0.05864661654135337</v>
+        <v>-0.008072723458908937</v>
       </c>
       <c r="L19" t="n">
-        <v>0.05864661654135337</v>
+        <v>-0.008072723458908937</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>0.05864661654135337</v>
+        <v>-0.008072723458908937</v>
       </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
@@ -1584,37 +1584,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.2406015037593985</v>
+        <v>0.009954047438161896</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>-0.2360902255639098</v>
+        <v>-0.005740128613605145</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.1894736842105263</v>
+        <v>0.009853405450136216</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.1984962406015038</v>
+        <v>-0.006633944617357784</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2706766917293233</v>
+        <v>-0.009825943305037731</v>
       </c>
       <c r="I20" t="n">
-        <v>0.03759398496240601</v>
+        <v>-0.006169556118782244</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.3778700188090975</v>
+        <v>-0.02638021511572415</v>
       </c>
       <c r="K20" t="n">
-        <v>0.2887218045112782</v>
+        <v>-0.008039878113595123</v>
       </c>
       <c r="L20" t="n">
-        <v>0.2887218045112782</v>
+        <v>-0.008039878113595123</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0.2887218045112782</v>
+        <v>-0.008039878113595123</v>
       </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
@@ -1636,37 +1636,37 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.38796992481203</v>
+        <v>-0.005299660531986421</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>-0.1714285714285714</v>
+        <v>0.01684457270578291</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.1909774436090226</v>
+        <v>0.00472676726107069</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.1428571428571428</v>
+        <v>0.007750133494005339</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2766917293233083</v>
+        <v>-0.00993502330940093</v>
       </c>
       <c r="I21" t="n">
-        <v>0.3398496240601503</v>
+        <v>-0.01017601365504055</v>
       </c>
       <c r="J21" t="n">
-        <v>0.05344376760048989</v>
+        <v>0.01340334183802703</v>
       </c>
       <c r="K21" t="n">
-        <v>0.3142857142857143</v>
+        <v>-0.01373533178141327</v>
       </c>
       <c r="L21" t="n">
-        <v>0.3142857142857143</v>
+        <v>-0.01373533178141327</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0.3142857142857143</v>
+        <v>-0.01373533178141327</v>
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -1688,37 +1688,37 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.07368421052631578</v>
+        <v>0.008285138731405548</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>0.06015037593984961</v>
+        <v>0.01152155633286225</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1699248120300751</v>
+        <v>0.01842706585708263</v>
       </c>
       <c r="G22" t="n">
-        <v>0.04511278195488722</v>
+        <v>0.01118482662339306</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.1984962406015038</v>
+        <v>-0.01983321813732872</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.1849624060150376</v>
+        <v>-0.01713025143721005</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.1565676571958013</v>
+        <v>0.008798088518457391</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.1909774436090226</v>
+        <v>-0.02011370365254814</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.1909774436090226</v>
+        <v>-0.02011370365254814</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>-0.1909774436090226</v>
+        <v>-0.02011370365254814</v>
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -1744,37 +1744,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.009022556390977442</v>
+        <v>0.006438271457530858</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>0.02556390977443609</v>
+        <v>0.01267765404310616</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.3097744360902255</v>
+        <v>0.007333373093334924</v>
       </c>
       <c r="G23" t="n">
-        <v>0.03609022556390977</v>
+        <v>0.01559422065576883</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2</v>
+        <v>-0.008720419068816761</v>
       </c>
       <c r="I23" t="n">
-        <v>0.08872180451127819</v>
+        <v>-0.01255258629410345</v>
       </c>
       <c r="J23" t="n">
-        <v>0.08656384893037093</v>
+        <v>-0.001803373655059443</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1593984962406015</v>
+        <v>-0.01007884110715364</v>
       </c>
       <c r="L23" t="n">
-        <v>0.1593984962406015</v>
+        <v>-0.01007884110715364</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>0.1593984962406015</v>
+        <v>-0.01007884110715364</v>
       </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
@@ -1796,37 +1796,37 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.2661654135338345</v>
+        <v>0.002236150553446022</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>-0.06015037593984961</v>
+        <v>0.002128765717150628</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.04962406015037594</v>
+        <v>-0.02478904111956164</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.05563909774436089</v>
+        <v>-0.004357932558317301</v>
       </c>
       <c r="H24" t="n">
-        <v>0.05263157894736842</v>
+        <v>0.02180615127224605</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.02556390977443609</v>
+        <v>0.02253726483749059</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.3710954567188945</v>
+        <v>-0.003294412552329649</v>
       </c>
       <c r="K24" t="n">
-        <v>0.08421052631578946</v>
+        <v>0.01742802338512094</v>
       </c>
       <c r="L24" t="n">
-        <v>0.08421052631578946</v>
+        <v>0.01742802338512094</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>0.08421052631578946</v>
+        <v>0.01742802338512094</v>
       </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
@@ -1852,37 +1852,37 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.03308270676691729</v>
+        <v>0.02462534383301375</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>0.4300751879699248</v>
+        <v>0.001950136110005444</v>
       </c>
       <c r="F25" t="n">
-        <v>0.6300751879699248</v>
+        <v>-0.01453228224529129</v>
       </c>
       <c r="G25" t="n">
-        <v>0.431578947368421</v>
+        <v>-0.005694928067797122</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.6270676691729322</v>
+        <v>0.01150377857215114</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.6285714285714286</v>
+        <v>0.0109187299727492</v>
       </c>
       <c r="J25" t="n">
-        <v>0.2830261495462563</v>
+        <v>-0.0003524729978338365</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.6330827067669172</v>
+        <v>0.008624320664972826</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.6330827067669172</v>
+        <v>0.008624320664972826</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>-0.6330827067669172</v>
+        <v>0.008624320664972826</v>
       </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
@@ -1904,37 +1904,37 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.07518796992481201</v>
+        <v>-0.01263183919327357</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>0.1338345864661654</v>
+        <v>0.001630648577225943</v>
       </c>
       <c r="F26" t="n">
-        <v>0.05112781954887217</v>
+        <v>0.001692465859698634</v>
       </c>
       <c r="G26" t="n">
-        <v>0.1308270676691729</v>
+        <v>0.0006880273235210929</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.04962406015037594</v>
+        <v>-0.005132423245296929</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.0706766917293233</v>
+        <v>-0.01001658673666347</v>
       </c>
       <c r="J26" t="n">
-        <v>0.2310878401880337</v>
+        <v>-0.006734521653986454</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.05714285714285714</v>
+        <v>-0.007382744167309766</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.05714285714285714</v>
+        <v>-0.007382744167309766</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>-0.05714285714285714</v>
+        <v>-0.007382744167309766</v>
       </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
@@ -1960,37 +1960,37 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.3293233082706767</v>
+        <v>0.01614806109392244</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>0.1894736842105263</v>
+        <v>-0.007162598974503958</v>
       </c>
       <c r="F27" t="n">
-        <v>0.3834586466165413</v>
+        <v>-0.02587930337117213</v>
       </c>
       <c r="G27" t="n">
-        <v>0.1759398496240602</v>
+        <v>-0.01326847397073896</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.4105263157894736</v>
+        <v>0.02219433141577325</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.4406015037593984</v>
+        <v>0.01890344744413789</v>
       </c>
       <c r="J27" t="n">
-        <v>0.08581111980923728</v>
+        <v>-0.006334450871893878</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.3969924812030075</v>
+        <v>0.01770171142806845</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.3969924812030075</v>
+        <v>0.01770171142806845</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-0.3969924812030075</v>
+        <v>0.01770171142806845</v>
       </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
@@ -2016,37 +2016,37 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.1007518796992481</v>
+        <v>-0.004579835223193408</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>0.08721804511278194</v>
+        <v>-0.0008652481306099251</v>
       </c>
       <c r="F28" t="n">
-        <v>0.06315789473684209</v>
+        <v>0.01041233196849328</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1233082706766917</v>
+        <v>0.0009345449653817984</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.02706766917293233</v>
+        <v>-0.008224093576963741</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1398496240601504</v>
+        <v>-0.008152086854083472</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.1859240929200141</v>
+        <v>0.004393436969495094</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.01954887218045112</v>
+        <v>-0.00741030327241213</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.01954887218045112</v>
+        <v>-0.00741030327241213</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.01954887218045112</v>
+        <v>-0.00741030327241213</v>
       </c>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
@@ -2072,37 +2072,37 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.05263157894736842</v>
+        <v>-0.005317255220690208</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>-0.1774436090225564</v>
+        <v>-0.009863765962550638</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.07969924812030074</v>
+        <v>-0.01403417316936693</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.1759398496240602</v>
+        <v>-0.0102721149388846</v>
       </c>
       <c r="H29" t="n">
-        <v>0.07218045112781954</v>
+        <v>0.01744044146561766</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2135338345864662</v>
+        <v>0.01661224492048979</v>
       </c>
       <c r="J29" t="n">
-        <v>0.03387281045101471</v>
+        <v>0.01016596626502864</v>
       </c>
       <c r="K29" t="n">
-        <v>0.07368421052631578</v>
+        <v>0.01954443524577741</v>
       </c>
       <c r="L29" t="n">
-        <v>0.07368421052631578</v>
+        <v>0.01954443524577741</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>0.07368421052631578</v>
+        <v>0.01954443524577741</v>
       </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
@@ -2128,37 +2128,37 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.5624060150375939</v>
+        <v>-0.005232737201309488</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>0.118796992481203</v>
+        <v>-0.01442198390487935</v>
       </c>
       <c r="F30" t="n">
-        <v>0.3774436090225564</v>
+        <v>0.0210508850660354</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1233082706766917</v>
+        <v>-0.01542084906483396</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.3548872180451128</v>
+        <v>-0.0172842700033708</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.5263157894736841</v>
+        <v>-0.01542497485699899</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.1354912418040589</v>
+        <v>0.01604107253044489</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.3203007518796992</v>
+        <v>-0.01323846043353842</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.3203007518796992</v>
+        <v>-0.01323846043353842</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>-0.3203007518796992</v>
+        <v>-0.01323846043353842</v>
       </c>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
@@ -2184,37 +2184,37 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.112781954887218</v>
+        <v>0.0169838624713545</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>-0.2721804511278195</v>
+        <v>0.007916122780644911</v>
       </c>
       <c r="F31" t="n">
-        <v>0.1263157894736842</v>
+        <v>0.01978643445545738</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.2977443609022556</v>
+        <v>0.01040825283233011</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.1593984962406015</v>
+        <v>-0.02045910091436403</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.09924812030075188</v>
+        <v>-0.02025557121022284</v>
       </c>
       <c r="J31" t="n">
-        <v>0.5058339694018198</v>
+        <v>-0.01254322739035051</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.162406015037594</v>
+        <v>-0.01845828438633138</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.162406015037594</v>
+        <v>-0.01845828438633138</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.162406015037594</v>
+        <v>-0.01845828438633138</v>
       </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
@@ -2240,37 +2240,37 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-0.07669172932330826</v>
+        <v>0.006301445532057821</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>-0.05714285714285714</v>
+        <v>-0.003315691716627668</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3488721804511278</v>
+        <v>0.005914909868596395</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.08872180451127819</v>
+        <v>-0.002260650330426013</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.356390977443609</v>
+        <v>-0.007688326387533055</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.3894736842105262</v>
+        <v>-0.01117334454293378</v>
       </c>
       <c r="J32" t="n">
-        <v>0.4538956600435972</v>
+        <v>-0.0003907793235924373</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.3368421052631578</v>
+        <v>-0.00731939126877565</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.3368421052631578</v>
+        <v>-0.00731939126877565</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>-0.3368421052631578</v>
+        <v>-0.00731939126877565</v>
       </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
@@ -2296,37 +2296,37 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.5729323308270676</v>
+        <v>-0.0292310951212438</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>-0.2496240601503759</v>
+        <v>-0.01696712247068489</v>
       </c>
       <c r="F33" t="n">
-        <v>0.01804511278195488</v>
+        <v>-0.002417175552687022</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.263157894736842</v>
+        <v>-0.01250048690001948</v>
       </c>
       <c r="H33" t="n">
-        <v>0.04060150375939849</v>
+        <v>0.004958662278346491</v>
       </c>
       <c r="I33" t="n">
-        <v>0.09172932330827067</v>
+        <v>-0.001813062024522481</v>
       </c>
       <c r="J33" t="n">
-        <v>0.2544224429431772</v>
+        <v>0.02388824177708749</v>
       </c>
       <c r="K33" t="n">
-        <v>0.04210526315789473</v>
+        <v>0.008004164576166583</v>
       </c>
       <c r="L33" t="n">
-        <v>0.04210526315789473</v>
+        <v>0.008004164576166583</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>0.04210526315789473</v>
+        <v>0.008004164576166583</v>
       </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
@@ -2352,37 +2352,37 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.1007518796992481</v>
+        <v>-0.01115912233436489</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>-0.2601503759398496</v>
+        <v>-0.003242170113686804</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.5518796992481202</v>
+        <v>-0.007625020529000821</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.2345864661654135</v>
+        <v>-0.003237786945511478</v>
       </c>
       <c r="H34" t="n">
-        <v>0.5097744360902255</v>
+        <v>0.0100304025772161</v>
       </c>
       <c r="I34" t="n">
-        <v>0.4406015037593984</v>
+        <v>0.01138237082329483</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.2702297544869841</v>
+        <v>0.01951226615617973</v>
       </c>
       <c r="K34" t="n">
-        <v>0.5037593984962406</v>
+        <v>0.01119891375995655</v>
       </c>
       <c r="L34" t="n">
-        <v>0.5037593984962406</v>
+        <v>0.01119891375995655</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>0.5037593984962406</v>
+        <v>0.01119891375995655</v>
       </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
@@ -2408,37 +2408,37 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.03609022556390977</v>
+        <v>0.01647357397094296</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>-0.3263157894736842</v>
+        <v>-0.01733444901337796</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.2781954887218045</v>
+        <v>-0.01397609652704386</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.3609022556390977</v>
+        <v>-0.01556440843057634</v>
       </c>
       <c r="H35" t="n">
-        <v>0.2135338345864662</v>
+        <v>0.01631877070075083</v>
       </c>
       <c r="I35" t="n">
-        <v>0.1984962406015038</v>
+        <v>0.02218259157530366</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.0587128714484255</v>
+        <v>-0.0008964938581932726</v>
       </c>
       <c r="K35" t="n">
-        <v>0.1864661654135338</v>
+        <v>0.01776789171871567</v>
       </c>
       <c r="L35" t="n">
-        <v>0.1864661654135338</v>
+        <v>0.01776789171871567</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>0.1864661654135338</v>
+        <v>0.01776789171871567</v>
       </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2464,37 +2464,37 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.118796992481203</v>
+        <v>0.02270689089227564</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>-0.07969924812030074</v>
+        <v>0.01671489705259588</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.1834586466165413</v>
+        <v>-0.002266160058646402</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.05112781954887217</v>
+        <v>0.01695646935025878</v>
       </c>
       <c r="H36" t="n">
-        <v>0.2225563909774436</v>
+        <v>-0.001575617727024709</v>
       </c>
       <c r="I36" t="n">
-        <v>0.1263157894736842</v>
+        <v>-0.002515635364625415</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.1369967000463262</v>
+        <v>0.01867862767761825</v>
       </c>
       <c r="K36" t="n">
-        <v>0.2105263157894737</v>
+        <v>-0.004288278891531155</v>
       </c>
       <c r="L36" t="n">
-        <v>0.2105263157894737</v>
+        <v>-0.004288278891531155</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>0.2105263157894737</v>
+        <v>-0.004288278891531155</v>
       </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2520,37 +2520,37 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.237593984962406</v>
+        <v>0.01713575943743037</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>-0.06917293233082707</v>
+        <v>0.01111542822061713</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.1819548872180451</v>
+        <v>0.01133387037335481</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.05864661654135337</v>
+        <v>0.01659936882397475</v>
       </c>
       <c r="H37" t="n">
-        <v>0.1458646616541353</v>
+        <v>-0.0126059276402371</v>
       </c>
       <c r="I37" t="n">
-        <v>0.08120300751879699</v>
+        <v>-0.01464582970583318</v>
       </c>
       <c r="J37" t="n">
-        <v>0.2137750704019596</v>
+        <v>-0.004851411458547401</v>
       </c>
       <c r="K37" t="n">
-        <v>0.1022556390977443</v>
+        <v>-0.01142060829682433</v>
       </c>
       <c r="L37" t="n">
-        <v>0.1022556390977443</v>
+        <v>-0.01142060829682433</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>0.1022556390977443</v>
+        <v>-0.01142060829682433</v>
       </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>

</xml_diff>

<commit_message>
create new ozonolysis project
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -712,37 +712,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.02582761082510443</v>
+        <v>-0.02583181370527254</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.006278448059137922</v>
+        <v>0.005323675988947039</v>
       </c>
       <c r="F4" t="n">
-        <v>0.005803265320130611</v>
+        <v>0.005973432046937281</v>
       </c>
       <c r="G4" t="n">
-        <v>0.005166825806673031</v>
+        <v>0.004021858816874352</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.007810884600435383</v>
+        <v>-0.0078151175286047</v>
       </c>
       <c r="I4" t="n">
         <v>-0.006983176887327074</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01034820081595253</v>
+        <v>0.006564829073468265</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.00942725576909023</v>
+        <v>-0.00928604053144162</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.00942725576909023</v>
+        <v>-0.00928604053144162</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>-0.00942725576909023</v>
+        <v>-0.00928604053144162</v>
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
@@ -764,37 +764,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.009941885197675407</v>
+        <v>0.009945150349806012</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>-0.01076371550254862</v>
+        <v>-0.01013012430920497</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.002943337845733513</v>
+        <v>-0.003058251290330051</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.01042122185684887</v>
+        <v>-0.00966167577846703</v>
       </c>
       <c r="H5" t="n">
-        <v>0.005611729184469167</v>
+        <v>0.005615015840600633</v>
       </c>
       <c r="I5" t="n">
         <v>-0.0005059528522381141</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01439178879278135</v>
+        <v>0.01313037540911028</v>
       </c>
       <c r="K5" t="n">
-        <v>0.008641389945655597</v>
+        <v>0.008536039253441569</v>
       </c>
       <c r="L5" t="n">
-        <v>0.008641389945655597</v>
+        <v>0.008536039253441569</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.008641389945655597</v>
+        <v>0.008536039253441569</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -816,37 +816,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.158945951061838</v>
+        <v>0.1589457267098291</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>-0.4252339828013593</v>
+        <v>-0.4252679545147181</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.9727317469732697</v>
+        <v>-0.9727239851809593</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.4361537471741498</v>
+        <v>-0.4361857322634293</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9999930934717236</v>
+        <v>0.9999930974077238</v>
       </c>
       <c r="I6" t="n">
         <v>0.9579628848145153</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.01835997333905618</v>
+        <v>-0.01851083778164393</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9802030376081213</v>
+        <v>0.9801911761356469</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9802030376081213</v>
+        <v>0.9801911761356469</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.9802030376081213</v>
+        <v>0.9801911761356469</v>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -872,37 +872,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9482859892914394</v>
+        <v>0.948285655595426</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.002671719466868778</v>
+        <v>0.003304628676185146</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.006566324614652984</v>
+        <v>-0.006678755595150223</v>
       </c>
       <c r="G7" t="n">
-        <v>0.004238152585526103</v>
+        <v>0.005008803752352149</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005660149378405975</v>
+        <v>0.005661723394468935</v>
       </c>
       <c r="I7" t="n">
         <v>0.001493300027732001</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.01887500478741833</v>
+        <v>-0.01913561304691967</v>
       </c>
       <c r="K7" t="n">
-        <v>0.005702059044082361</v>
+        <v>0.005601806144072245</v>
       </c>
       <c r="L7" t="n">
-        <v>0.005702059044082361</v>
+        <v>0.005601806144072245</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>0.005702059044082361</v>
+        <v>0.005601806144072245</v>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
@@ -928,37 +928,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.01275827580633103</v>
+        <v>-0.01275851935834077</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.001623828064953122</v>
+        <v>0.001558442366337694</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01358628371145135</v>
+        <v>0.01360067545602702</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.001084707979388319</v>
+        <v>-0.001164979630599185</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.01304992429799697</v>
+        <v>-0.01304960077798403</v>
       </c>
       <c r="I8" t="n">
         <v>-0.009443602841744113</v>
       </c>
       <c r="J8" t="n">
-        <v>0.007431583434837585</v>
+        <v>0.01130422178425811</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.01153103393324135</v>
+        <v>-0.01151717854068714</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.01153103393324135</v>
+        <v>-0.01151717854068714</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>-0.01153103393324135</v>
+        <v>-0.01151717854068714</v>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -984,37 +984,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.01983799989751999</v>
+        <v>0.01983731772149271</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>-0.0136505576340223</v>
+        <v>-0.01379490035979601</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.02406639168265566</v>
+        <v>-0.02404344681773787</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.01554824058992962</v>
+        <v>-0.01571890565275623</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02699373976774959</v>
+        <v>0.02699259179970367</v>
       </c>
       <c r="I9" t="n">
         <v>0.02935640968625638</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.00249073472405112</v>
+        <v>-0.001152404203615604</v>
       </c>
       <c r="K9" t="n">
-        <v>0.02667502052300081</v>
+        <v>0.02669652529186101</v>
       </c>
       <c r="L9" t="n">
-        <v>0.02667502052300081</v>
+        <v>0.02669652529186101</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.02667502052300081</v>
+        <v>0.02669652529186101</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
@@ -1040,37 +1040,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.02683866232154649</v>
+        <v>0.02683496449739858</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>0.00660486554419462</v>
+        <v>0.00586770100270804</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.001898852811954112</v>
+        <v>-0.001767465190698607</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0008686074587442983</v>
+        <v>-2.187456087498243e-05</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.001876327467053099</v>
+        <v>-0.001878628587145143</v>
       </c>
       <c r="I10" t="n">
         <v>-0.0009429528377181134</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.02529717439324946</v>
+        <v>-0.02401487927802731</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.002920339988813599</v>
+        <v>-0.002806700272268011</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.002920339988813599</v>
+        <v>-0.002806700272268011</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>-0.002920339988813599</v>
+        <v>-0.002806700272268011</v>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
@@ -1092,37 +1092,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1137545369661815</v>
+        <v>0.1137550884862035</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>-0.00762312904092516</v>
+        <v>-0.007432408617296344</v>
       </c>
       <c r="F11" t="n">
-        <v>0.006939077557563101</v>
+        <v>0.006909197076367883</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.008018200832728032</v>
+        <v>-0.007790475575619021</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.005576928127077125</v>
+        <v>-0.005576402239056089</v>
       </c>
       <c r="I11" t="n">
         <v>0.2739322870212915</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.007289651238349656</v>
+        <v>-0.006201012892862459</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.002553755334150213</v>
+        <v>-0.002584748839389953</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.002553755334150213</v>
+        <v>-0.002584748839389953</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.002553755334150213</v>
+        <v>-0.002584748839389953</v>
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
@@ -1144,37 +1144,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.2321533771901351</v>
+        <v>-0.2321558205822328</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>-0.002522963908918556</v>
+        <v>-0.003226856193074247</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.01039102553564102</v>
+        <v>-0.01026742015469681</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.008845866209834647</v>
+        <v>-0.009694647075785882</v>
       </c>
       <c r="H12" t="n">
-        <v>0.007154029918161196</v>
+        <v>0.007151423806056952</v>
       </c>
       <c r="I12" t="n">
         <v>0.00596510827060433</v>
       </c>
       <c r="J12" t="n">
-        <v>0.005757202250523404</v>
+        <v>0.007696889331922898</v>
       </c>
       <c r="K12" t="n">
-        <v>0.004525499701019987</v>
+        <v>0.004637113145484525</v>
       </c>
       <c r="L12" t="n">
-        <v>0.004525499701019987</v>
+        <v>0.004637113145484525</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>0.004525499701019987</v>
+        <v>0.004637113145484525</v>
       </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
@@ -1200,37 +1200,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01056698269467931</v>
+        <v>0.01056586823063473</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>0.02040668990426759</v>
+        <v>0.02011383171655327</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.01779460784778431</v>
+        <v>-0.01774917728596709</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01958194235127769</v>
+        <v>0.01924058409762336</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01394767476590699</v>
+        <v>0.01394649396585976</v>
       </c>
       <c r="I13" t="n">
         <v>0.008566614198664566</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.006673082067163705</v>
+        <v>-0.007275914358668754</v>
       </c>
       <c r="K13" t="n">
-        <v>0.01025061641002466</v>
+        <v>0.01028816066752643</v>
       </c>
       <c r="L13" t="n">
-        <v>0.01025061641002466</v>
+        <v>0.01028816066752643</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>0.01025061641002466</v>
+        <v>0.01028816066752643</v>
       </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
@@ -1256,37 +1256,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.004903858948154358</v>
+        <v>-0.004906139044245562</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>0.008945898405835935</v>
+        <v>0.008200154344006172</v>
       </c>
       <c r="F14" t="n">
-        <v>0.003007147128285884</v>
+        <v>0.00314459849378394</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01225993345039734</v>
+        <v>0.01135978490239139</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.003247164897886596</v>
+        <v>-0.003250306498012259</v>
       </c>
       <c r="I14" t="n">
         <v>-0.007119685916787436</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.01391352199389795</v>
+        <v>-0.01175720248075576</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.00433883201355328</v>
+        <v>-0.004220812776832511</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.00433883201355328</v>
+        <v>-0.004220812776832511</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>-0.00433883201355328</v>
+        <v>-0.004220812776832511</v>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
@@ -1312,37 +1312,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.006596756999870279</v>
+        <v>0.006593593607743743</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>0.01075373860614954</v>
+        <v>0.01010293374811735</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01240032184001287</v>
+        <v>0.01251147314045892</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01594537974181519</v>
+        <v>0.0151634876465395</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.01226752810670112</v>
+        <v>-0.0122690350187614</v>
       </c>
       <c r="I15" t="n">
         <v>-0.01063130442525218</v>
       </c>
       <c r="J15" t="n">
-        <v>0.007173397252697429</v>
+        <v>0.006851217969517403</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.01096236312649452</v>
+        <v>-0.01086407697856308</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.01096236312649452</v>
+        <v>-0.01086407697856308</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.01096236312649452</v>
+        <v>-0.01086407697856308</v>
       </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1368,37 +1368,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.02327230931489237</v>
+        <v>0.02326990873879635</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>0.007150765822030632</v>
+        <v>0.006334121917364876</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.01200855734434229</v>
+        <v>-0.01186326527453061</v>
       </c>
       <c r="G16" t="n">
-        <v>0.001330667957226718</v>
+        <v>0.0003409260616370424</v>
       </c>
       <c r="H16" t="n">
-        <v>0.009131315309252611</v>
+        <v>0.009128238125129523</v>
       </c>
       <c r="I16" t="n">
         <v>0.01187364479494579</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.01514818011141934</v>
+        <v>-0.01522211223591942</v>
       </c>
       <c r="K16" t="n">
-        <v>0.007138775613551023</v>
+        <v>0.007267366562694662</v>
       </c>
       <c r="L16" t="n">
-        <v>0.007138775613551023</v>
+        <v>0.007267366562694662</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.007138775613551023</v>
+        <v>0.007267366562694662</v>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
@@ -1420,37 +1420,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.001097359435894377</v>
+        <v>-0.001096021483840859</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>-0.01232639924505597</v>
+        <v>-0.01186594108263764</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01436509583860383</v>
+        <v>0.01427674223506969</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.01240728184029127</v>
+        <v>-0.01184315317772612</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.007947437693897507</v>
+        <v>-0.007946154077846162</v>
       </c>
       <c r="I17" t="n">
         <v>-0.006570467302818691</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0005686332642127915</v>
+        <v>7.948560702341064e-05</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.005129341165173646</v>
+        <v>-0.005199365583974622</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.005129341165173646</v>
+        <v>-0.005199365583974622</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.005129341165173646</v>
+        <v>-0.005199365583974622</v>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
@@ -1476,37 +1476,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.0195531300621252</v>
+        <v>-0.01955374791814991</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
-        <v>0.003402976552119061</v>
+        <v>0.003212637824505512</v>
       </c>
       <c r="F18" t="n">
-        <v>0.009063783434551336</v>
+        <v>0.009095317707812706</v>
       </c>
       <c r="G18" t="n">
-        <v>0.005157989294319571</v>
+        <v>0.004934812421392497</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.007303009156120366</v>
+        <v>-0.007303982500159299</v>
       </c>
       <c r="I18" t="n">
         <v>-0.004741255389650215</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.01372789824304994</v>
+        <v>-0.0114945739148243</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.004396976431879056</v>
+        <v>-0.004365985806639432</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.004396976431879056</v>
+        <v>-0.004365985806639432</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.004396976431879056</v>
+        <v>-0.004365985806639432</v>
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
@@ -1532,37 +1532,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.01570813618032544</v>
+        <v>-0.01571077157243086</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>0.004782966719318668</v>
+        <v>0.004267814858712593</v>
       </c>
       <c r="F19" t="n">
-        <v>0.005556496734259868</v>
+        <v>0.005647702497908099</v>
       </c>
       <c r="G19" t="n">
-        <v>0.005297462227898488</v>
+        <v>0.004673611482944459</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.006599684135987364</v>
+        <v>-0.006601831368073253</v>
       </c>
       <c r="I19" t="n">
         <v>-0.005024797256991891</v>
       </c>
       <c r="J19" t="n">
-        <v>0.01025525899862456</v>
+        <v>0.009447927202545062</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.008072723458908937</v>
+        <v>-0.007990128223605128</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.008072723458908937</v>
+        <v>-0.007990128223605128</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>-0.008072723458908937</v>
+        <v>-0.007990128223605128</v>
       </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
@@ -1584,37 +1584,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.009954047438161896</v>
+        <v>0.009956271758250869</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>-0.005740128613605145</v>
+        <v>-0.005006833544273341</v>
       </c>
       <c r="F20" t="n">
-        <v>0.009853405450136216</v>
+        <v>0.009721509124860365</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.006633944617357784</v>
+        <v>-0.005748933157957325</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.009825943305037731</v>
+        <v>-0.009823572872942913</v>
       </c>
       <c r="I20" t="n">
         <v>-0.006169556118782244</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.02638021511572415</v>
+        <v>-0.0253186096626263</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.008039878113595123</v>
+        <v>-0.008158050470322017</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.008039878113595123</v>
+        <v>-0.008158050470322017</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>-0.008039878113595123</v>
+        <v>-0.008158050470322017</v>
       </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
@@ -1636,37 +1636,37 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.005299660531986421</v>
+        <v>-0.005300213492008539</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>0.01684457270578291</v>
+        <v>0.01680334867213394</v>
       </c>
       <c r="F21" t="n">
-        <v>0.00472676726107069</v>
+        <v>0.004735222077408883</v>
       </c>
       <c r="G21" t="n">
-        <v>0.007750133494005339</v>
+        <v>0.007697500819900032</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.00993502330940093</v>
+        <v>-0.009935331277413249</v>
       </c>
       <c r="I21" t="n">
         <v>-0.01017601365504055</v>
       </c>
       <c r="J21" t="n">
-        <v>0.01340334183802703</v>
+        <v>0.01305152829702044</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.01373533178141327</v>
+        <v>-0.01372975360519014</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.01373533178141327</v>
+        <v>-0.01372975360519014</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-0.01373533178141327</v>
+        <v>-0.01372975360519014</v>
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -1688,37 +1688,37 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.008285138731405548</v>
+        <v>0.008283845611353825</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>0.01152155633286225</v>
+        <v>0.01116295158251806</v>
       </c>
       <c r="F22" t="n">
-        <v>0.01842706585708263</v>
+        <v>0.01849504883580195</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01118482662339306</v>
+        <v>0.0107526649421066</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.01983321813732872</v>
+        <v>-0.0198344550013782</v>
       </c>
       <c r="I22" t="n">
         <v>-0.01713025143721005</v>
       </c>
       <c r="J22" t="n">
-        <v>0.008798088518457391</v>
+        <v>0.007590651152202</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.02011370365254814</v>
+        <v>-0.02005689689827587</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.02011370365254814</v>
+        <v>-0.02005689689827587</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>-0.02011370365254814</v>
+        <v>-0.02005689689827587</v>
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -1744,37 +1744,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.006438271457530858</v>
+        <v>0.006441263105650522</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>0.01267765404310616</v>
+        <v>0.0130137524565501</v>
       </c>
       <c r="F23" t="n">
-        <v>0.007333373093334924</v>
+        <v>0.007272629858905193</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01559422065576883</v>
+        <v>0.01600876086435043</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.008720419068816761</v>
+        <v>-0.00871884399675376</v>
       </c>
       <c r="I23" t="n">
         <v>-0.01255258629410345</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.001803373655059443</v>
+        <v>-0.00317587135008713</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.01007884110715364</v>
+        <v>-0.01013380398935216</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.01007884110715364</v>
+        <v>-0.01013380398935216</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>-0.01007884110715364</v>
+        <v>-0.01013380398935216</v>
       </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
@@ -1796,37 +1796,37 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.002236150553446022</v>
+        <v>0.002234838521393541</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>0.002128765717150628</v>
+        <v>0.002021694128867765</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.02478904111956164</v>
+        <v>-0.02476419910256796</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.004357932558317301</v>
+        <v>-0.004495211123808444</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02180615127224605</v>
+        <v>0.02180537040821481</v>
       </c>
       <c r="I24" t="n">
         <v>0.02253726483749059</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.003294412552329649</v>
+        <v>-0.00130007673734563</v>
       </c>
       <c r="K24" t="n">
-        <v>0.01742802338512094</v>
+        <v>0.0174503299460132</v>
       </c>
       <c r="L24" t="n">
-        <v>0.01742802338512094</v>
+        <v>0.0174503299460132</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>0.01742802338512094</v>
+        <v>0.0174503299460132</v>
       </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
@@ -1852,37 +1852,37 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.02462534383301375</v>
+        <v>0.02462292808891712</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>0.001950136110005444</v>
+        <v>0.0009841143753645748</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.01453228224529129</v>
+        <v>-0.01435726396629056</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.005694928067797122</v>
+        <v>-0.006858083602323342</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01150377857215114</v>
+        <v>0.01150002564400102</v>
       </c>
       <c r="I25" t="n">
         <v>0.0109187299727492</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.0003524729978338365</v>
+        <v>0.002240979422174362</v>
       </c>
       <c r="K25" t="n">
-        <v>0.008624320664972826</v>
+        <v>0.008770965662838625</v>
       </c>
       <c r="L25" t="n">
-        <v>0.008624320664972826</v>
+        <v>0.008770965662838625</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.008624320664972826</v>
+        <v>0.008770965662838625</v>
       </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
@@ -1904,37 +1904,37 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-0.01263183919327357</v>
+        <v>-0.01263190322527613</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>0.001630648577225943</v>
+        <v>0.001490879291635171</v>
       </c>
       <c r="F26" t="n">
-        <v>0.001692465859698634</v>
+        <v>0.001714591844583674</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0006880273235210929</v>
+        <v>0.0005169198926767957</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.005132423245296929</v>
+        <v>-0.00513286100531444</v>
       </c>
       <c r="I26" t="n">
         <v>-0.01001658673666347</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.006734521653986454</v>
+        <v>-0.00586887031631364</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.007382744167309766</v>
+        <v>-0.007364472390578894</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.007382744167309766</v>
+        <v>-0.007364472390578894</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>-0.007382744167309766</v>
+        <v>-0.007364472390578894</v>
       </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
@@ -1960,37 +1960,37 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.01614806109392244</v>
+        <v>0.01614552784582111</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>-0.007162598974503958</v>
+        <v>-0.007641888689675546</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.02587930337117213</v>
+        <v>-0.02579559875982395</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.01326847397073896</v>
+        <v>-0.01384898100195924</v>
       </c>
       <c r="H27" t="n">
-        <v>0.02219433141577325</v>
+        <v>0.02219243589569744</v>
       </c>
       <c r="I27" t="n">
         <v>0.01890344744413789</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.006334450871893878</v>
+        <v>-0.006236589269584303</v>
       </c>
       <c r="K27" t="n">
-        <v>0.01770171142806845</v>
+        <v>0.01777407776696311</v>
       </c>
       <c r="L27" t="n">
-        <v>0.01770171142806845</v>
+        <v>0.01777407776696311</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>0.01770171142806845</v>
+        <v>0.01777407776696311</v>
       </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
@@ -2016,37 +2016,37 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.004579835223193408</v>
+        <v>-0.004582101207284047</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>-0.0008652481306099251</v>
+        <v>-0.001277891091115644</v>
       </c>
       <c r="F28" t="n">
-        <v>0.01041233196849328</v>
+        <v>0.01048654093146164</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0009345449653817984</v>
+        <v>0.0004306996972279878</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.008224093576963741</v>
+        <v>-0.00822583578503343</v>
       </c>
       <c r="I28" t="n">
         <v>-0.008152086854083472</v>
       </c>
       <c r="J28" t="n">
-        <v>0.004393436969495094</v>
+        <v>0.005047839700050126</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.00741030327241213</v>
+        <v>-0.00734137075765483</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.00741030327241213</v>
+        <v>-0.00734137075765483</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.00741030327241213</v>
+        <v>-0.00734137075765483</v>
       </c>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
@@ -2072,37 +2072,37 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.005317255220690208</v>
+        <v>-0.00531415451656618</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>-0.009863765962550638</v>
+        <v>-0.009483023323320931</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.01403417316936693</v>
+        <v>-0.01410470120418805</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.0102721149388846</v>
+        <v>-0.009823971176958846</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01744044146561766</v>
+        <v>0.01744225068169002</v>
       </c>
       <c r="I29" t="n">
         <v>0.01661224492048979</v>
       </c>
       <c r="J29" t="n">
-        <v>0.01016596626502864</v>
+        <v>0.009506652406639417</v>
       </c>
       <c r="K29" t="n">
-        <v>0.01954443524577741</v>
+        <v>0.01948544957941798</v>
       </c>
       <c r="L29" t="n">
-        <v>0.01954443524577741</v>
+        <v>0.01948544957941798</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>0.01954443524577741</v>
+        <v>0.01948544957941798</v>
       </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
@@ -2128,37 +2128,37 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.005232737201309488</v>
+        <v>-0.005234805137392206</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>-0.01442198390487935</v>
+        <v>-0.01503540924141637</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0210508850660354</v>
+        <v>0.02116549313461972</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.01542084906483396</v>
+        <v>-0.01616924061476962</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.0172842700033708</v>
+        <v>-0.01728756049950242</v>
       </c>
       <c r="I30" t="n">
         <v>-0.01542497485699899</v>
       </c>
       <c r="J30" t="n">
-        <v>0.01604107253044489</v>
+        <v>0.01566352778829018</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.01323846043353842</v>
+        <v>-0.0131317674692707</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.01323846043353842</v>
+        <v>-0.0131317674692707</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>-0.01323846043353842</v>
+        <v>-0.0131317674692707</v>
       </c>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
@@ -2184,37 +2184,37 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.0169838624713545</v>
+        <v>0.01698458189538327</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>0.007916122780644911</v>
+        <v>0.007866128858645153</v>
       </c>
       <c r="F31" t="n">
-        <v>0.01978643445545738</v>
+        <v>0.01979747407189896</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01040825283233011</v>
+        <v>0.01033770281350811</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.02045910091436403</v>
+        <v>-0.02045879611435184</v>
       </c>
       <c r="I31" t="n">
         <v>-0.02025557121022284</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.01254322739035051</v>
+        <v>-0.01287680051306386</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.01845828438633138</v>
+        <v>-0.01845362233814489</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.01845828438633138</v>
+        <v>-0.01845362233814489</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.01845828438633138</v>
+        <v>-0.01845362233814489</v>
       </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
@@ -2240,37 +2240,37 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.006301445532057821</v>
+        <v>0.006300207804008312</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>-0.003315691716627668</v>
+        <v>-0.003358240070329603</v>
       </c>
       <c r="F32" t="n">
-        <v>0.005914909868596395</v>
+        <v>0.005920060748802428</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.002260650330426013</v>
+        <v>-0.002313754652550186</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.007688326387533055</v>
+        <v>-0.007688387347535493</v>
       </c>
       <c r="I32" t="n">
         <v>-0.01117334454293378</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.0003907793235924373</v>
+        <v>0.002330390421893428</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.00731939126877565</v>
+        <v>-0.007312721092508842</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.00731939126877565</v>
+        <v>-0.007312721092508842</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>-0.00731939126877565</v>
+        <v>-0.007312721092508842</v>
       </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
@@ -2296,37 +2296,37 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.0292310951212438</v>
+        <v>-0.02923019310520772</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>-0.01696712247068489</v>
+        <v>-0.01652959650118386</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.002417175552687022</v>
+        <v>-0.002491824291672971</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.01250048690001948</v>
+        <v>-0.01198059772722391</v>
       </c>
       <c r="H33" t="n">
-        <v>0.004958662278346491</v>
+        <v>0.004960326822413073</v>
       </c>
       <c r="I33" t="n">
         <v>-0.001813062024522481</v>
       </c>
       <c r="J33" t="n">
-        <v>0.02388824177708749</v>
+        <v>0.02349167283205113</v>
       </c>
       <c r="K33" t="n">
-        <v>0.008004164576166583</v>
+        <v>0.007939010237560409</v>
       </c>
       <c r="L33" t="n">
-        <v>0.008004164576166583</v>
+        <v>0.007939010237560409</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>0.008004164576166583</v>
+        <v>0.007939010237560409</v>
       </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
@@ -2352,37 +2352,37 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.01115912233436489</v>
+        <v>-0.01115823980632959</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>-0.003242170113686804</v>
+        <v>-0.003319750116790004</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.007625020529000821</v>
+        <v>-0.007611254224450168</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.003237786945511478</v>
+        <v>-0.003330203173208127</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0100304025772161</v>
+        <v>0.01003024984120999</v>
       </c>
       <c r="I34" t="n">
         <v>0.01138237082329483</v>
       </c>
       <c r="J34" t="n">
-        <v>0.01951226615617973</v>
+        <v>0.01949998583334653</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01119891375995655</v>
+        <v>0.01121485801659432</v>
       </c>
       <c r="L34" t="n">
-        <v>0.01119891375995655</v>
+        <v>0.01121485801659432</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>0.01119891375995655</v>
+        <v>0.01121485801659432</v>
       </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
@@ -2408,37 +2408,37 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01647357397094296</v>
+        <v>0.01647461105898444</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>-0.01733444901337796</v>
+        <v>-0.01711472084458883</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.01397609652704386</v>
+        <v>-0.01401762622470505</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.01556440843057634</v>
+        <v>-0.01529951696398068</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01631877070075083</v>
+        <v>0.01631998020479921</v>
       </c>
       <c r="I35" t="n">
         <v>0.02218259157530366</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.0008964938581932726</v>
+        <v>-0.0005847199143155518</v>
       </c>
       <c r="K35" t="n">
-        <v>0.01776789171871567</v>
+        <v>0.01772926678917067</v>
       </c>
       <c r="L35" t="n">
-        <v>0.01776789171871567</v>
+        <v>0.01772926678917067</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>0.01776789171871567</v>
+        <v>0.01772926678917067</v>
       </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2464,37 +2464,37 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.02270689089227564</v>
+        <v>0.02270644958025798</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>0.01671489705259588</v>
+        <v>0.01656757045470282</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.002266160058646402</v>
+        <v>-0.002234137049365482</v>
       </c>
       <c r="G36" t="n">
-        <v>0.01695646935025878</v>
+        <v>0.01677957398318296</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.001575617727024709</v>
+        <v>-0.001576489407059576</v>
       </c>
       <c r="I36" t="n">
         <v>-0.002515635364625415</v>
       </c>
       <c r="J36" t="n">
-        <v>0.01867862767761825</v>
+        <v>0.01558235757093167</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.004288278891531155</v>
+        <v>-0.004262439338497573</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.004288278891531155</v>
+        <v>-0.004262439338497573</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>-0.004288278891531155</v>
+        <v>-0.004262439338497573</v>
       </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2520,37 +2520,37 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.01713575943743037</v>
+        <v>0.01713563434942537</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>0.01111542822061713</v>
+        <v>0.01103650623346025</v>
       </c>
       <c r="F37" t="n">
-        <v>0.01133387037335481</v>
+        <v>0.01134849069393963</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01659936882397475</v>
+        <v>0.01650855454834218</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.0126059276402371</v>
+        <v>-0.01260722920828916</v>
       </c>
       <c r="I37" t="n">
         <v>-0.01464582970583318</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.004851411458547401</v>
+        <v>-0.005527097916335087</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.01142060829682433</v>
+        <v>-0.01141044045641762</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.01142060829682433</v>
+        <v>-0.01141044045641762</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.01142060829682433</v>
+        <v>-0.01141044045641762</v>
       </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>

</xml_diff>

<commit_message>
work on actag contour graph style; continue running oilcane model
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -712,37 +712,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.02583181370527254</v>
+        <v>-0.02658737885549515</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.005323675988947039</v>
+        <v>0.005465991194639646</v>
       </c>
       <c r="F4" t="n">
-        <v>0.005973432046937281</v>
+        <v>-0.01063662023346481</v>
       </c>
       <c r="G4" t="n">
-        <v>0.004021858816874352</v>
+        <v>0.04256176682247067</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0078151175286047</v>
+        <v>-0.007805750712230028</v>
       </c>
       <c r="I4" t="n">
         <v>-0.006983176887327074</v>
       </c>
       <c r="J4" t="n">
-        <v>0.006564829073468265</v>
+        <v>-0.005555156068918668</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.00928604053144162</v>
+        <v>0.03173725470949018</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.00928604053144162</v>
+        <v>0.03173725470949018</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>-0.00928604053144162</v>
+        <v>0.03173725470949018</v>
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
@@ -764,37 +764,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.009945150349806012</v>
+        <v>0.01021047688841907</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>-0.01013012430920497</v>
+        <v>-0.01013502376540095</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.003058251290330051</v>
+        <v>0.01090468670818747</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.00966167577846703</v>
+        <v>-0.00523009451320378</v>
       </c>
       <c r="H5" t="n">
-        <v>0.005615015840600633</v>
+        <v>0.005649591297983651</v>
       </c>
       <c r="I5" t="n">
         <v>-0.0005059528522381141</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01313037540911028</v>
+        <v>0.0244145690650492</v>
       </c>
       <c r="K5" t="n">
-        <v>0.008536039253441569</v>
+        <v>0.009640727809629112</v>
       </c>
       <c r="L5" t="n">
-        <v>0.008536039253441569</v>
+        <v>0.009640727809629112</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.008536039253441569</v>
+        <v>0.009640727809629112</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -816,37 +816,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1589457267098291</v>
+        <v>0.1898265375450615</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>-0.4252679545147181</v>
+        <v>-0.4253799642471985</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.9727239851809593</v>
+        <v>0.8335373874534955</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.4361857322634293</v>
+        <v>0.3258798638191945</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9999930974077238</v>
+        <v>0.9999932175037286</v>
       </c>
       <c r="I6" t="n">
         <v>0.9579628848145153</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.01851083778164393</v>
+        <v>0.007026714779913105</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9801911761356469</v>
+        <v>-0.4333832774953311</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9801911761356469</v>
+        <v>-0.4333832774953311</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.9801911761356469</v>
+        <v>-0.4333832774953311</v>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -872,37 +872,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.948285655595426</v>
+        <v>0.9426671344106852</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.003304628676185146</v>
+        <v>0.002995317431812697</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.006678755595150223</v>
+        <v>0.003223472384938895</v>
       </c>
       <c r="G7" t="n">
-        <v>0.005008803752352149</v>
+        <v>-0.009856131562245261</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005661723394468935</v>
+        <v>0.005664523330580932</v>
       </c>
       <c r="I7" t="n">
         <v>0.001493300027732001</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.01913561304691967</v>
+        <v>-0.009728802489008368</v>
       </c>
       <c r="K7" t="n">
-        <v>0.005601806144072245</v>
+        <v>-0.005593015903720636</v>
       </c>
       <c r="L7" t="n">
-        <v>0.005601806144072245</v>
+        <v>-0.005593015903720636</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>0.005601806144072245</v>
+        <v>-0.005593015903720636</v>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
@@ -928,37 +928,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.01275851935834077</v>
+        <v>-0.01313509166140367</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.001558442366337694</v>
+        <v>0.001354536150181446</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01360067545602702</v>
+        <v>-0.007606005616240224</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.001164979630599185</v>
+        <v>-0.0288083400963336</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.01304960077798403</v>
+        <v>-0.01306648861865954</v>
       </c>
       <c r="I8" t="n">
         <v>-0.009443602841744113</v>
       </c>
       <c r="J8" t="n">
-        <v>0.01130422178425811</v>
+        <v>0.01585730368087417</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.01151717854068714</v>
+        <v>0.01131375962055038</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.01151717854068714</v>
+        <v>0.01131375962055038</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>-0.01151717854068714</v>
+        <v>0.01131375962055038</v>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -984,37 +984,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.01983731772149271</v>
+        <v>0.02045771093030843</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>-0.01379490035979601</v>
+        <v>-0.01361019971240798</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.02404344681773787</v>
+        <v>0.02089843955593758</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.01571890565275623</v>
+        <v>-0.009879947051197879</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02699259179970367</v>
+        <v>0.02695556805422272</v>
       </c>
       <c r="I9" t="n">
         <v>0.02935640968625638</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.001152404203615604</v>
+        <v>-0.01511229979866384</v>
       </c>
       <c r="K9" t="n">
-        <v>0.02669652529186101</v>
+        <v>-0.0002645018025800721</v>
       </c>
       <c r="L9" t="n">
-        <v>0.02669652529186101</v>
+        <v>-0.0002645018025800721</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.02669652529186101</v>
+        <v>-0.0002645018025800721</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
@@ -1040,37 +1040,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.02683496449739858</v>
+        <v>0.02999642414385696</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>0.00586770100270804</v>
+        <v>0.005756988422279535</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.001767465190698607</v>
+        <v>-0.005379545975181838</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.187456087498243e-05</v>
+        <v>-0.006492012067680481</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.001878628587145143</v>
+        <v>-0.001882962315318492</v>
       </c>
       <c r="I10" t="n">
         <v>-0.0009429528377181134</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.02401487927802731</v>
+        <v>0.01335783306135146</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.002806700272268011</v>
+        <v>-0.002089564979582599</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.002806700272268011</v>
+        <v>-0.002089564979582599</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>-0.002806700272268011</v>
+        <v>-0.002089564979582599</v>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
@@ -1092,37 +1092,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1137550884862035</v>
+        <v>0.1123469959498798</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>-0.007432408617296344</v>
+        <v>-0.007713633908545355</v>
       </c>
       <c r="F11" t="n">
-        <v>0.006909197076367883</v>
+        <v>0.002453693474147739</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.007790475575619021</v>
+        <v>-0.01776083571843343</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.005576402239056089</v>
+        <v>-0.005572430814897231</v>
       </c>
       <c r="I11" t="n">
         <v>0.2739322870212915</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.006201012892862459</v>
+        <v>0.0250161915335958</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.002584748839389953</v>
+        <v>0.01980312108012484</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.002584748839389953</v>
+        <v>0.01980312108012484</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.002584748839389953</v>
+        <v>0.01980312108012484</v>
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
@@ -1144,37 +1144,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.2321558205822328</v>
+        <v>-0.2301963123758525</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>-0.003226856193074247</v>
+        <v>-0.002983256375330254</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.01026742015469681</v>
+        <v>0.002545738853829554</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.009694647075785882</v>
+        <v>0.01394744830189793</v>
       </c>
       <c r="H12" t="n">
-        <v>0.007151423806056952</v>
+        <v>0.007194415583776623</v>
       </c>
       <c r="I12" t="n">
         <v>0.00596510827060433</v>
       </c>
       <c r="J12" t="n">
-        <v>0.007696889331922898</v>
+        <v>-0.004179991492478003</v>
       </c>
       <c r="K12" t="n">
-        <v>0.004637113145484525</v>
+        <v>-0.01292686093307444</v>
       </c>
       <c r="L12" t="n">
-        <v>0.004637113145484525</v>
+        <v>-0.01292686093307444</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>0.004637113145484525</v>
+        <v>-0.01292686093307444</v>
       </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
@@ -1200,37 +1200,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01056586823063473</v>
+        <v>0.01080141489605659</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>0.02011383171655327</v>
+        <v>0.01996635593465423</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.01774917728596709</v>
+        <v>0.003818433848737354</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01924058409762336</v>
+        <v>0.03070264452410577</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01394649396585976</v>
+        <v>0.01397413169496526</v>
       </c>
       <c r="I13" t="n">
         <v>0.008566614198664566</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.007275914358668754</v>
+        <v>-0.007947490557074603</v>
       </c>
       <c r="K13" t="n">
-        <v>0.01028816066752643</v>
+        <v>-0.03490118789204751</v>
       </c>
       <c r="L13" t="n">
-        <v>0.01028816066752643</v>
+        <v>-0.03490118789204751</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>0.01028816066752643</v>
+        <v>-0.03490118789204751</v>
       </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
@@ -1256,37 +1256,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.004906139044245562</v>
+        <v>-0.005271760818870433</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>0.008200154344006172</v>
+        <v>0.00833421527736861</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00314459849378394</v>
+        <v>-0.004312245004489799</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01135978490239139</v>
+        <v>0.01820064063202562</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.003250306498012259</v>
+        <v>-0.0032442650257706</v>
       </c>
       <c r="I14" t="n">
         <v>-0.007119685916787436</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.01175720248075576</v>
+        <v>-0.01816328662100451</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.004220812776832511</v>
+        <v>-0.008689076411563053</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.004220812776832511</v>
+        <v>-0.008689076411563053</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>-0.004220812776832511</v>
+        <v>-0.008689076411563053</v>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
@@ -1312,37 +1312,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.006593593607743743</v>
+        <v>0.006335240893409635</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>0.01010293374811735</v>
+        <v>0.01024268200970728</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01251147314045892</v>
+        <v>-0.007798515863940633</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0151634876465395</v>
+        <v>0.01462896768915871</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.0122690350187614</v>
+        <v>-0.0122924876276995</v>
       </c>
       <c r="I15" t="n">
         <v>-0.01063130442525218</v>
       </c>
       <c r="J15" t="n">
-        <v>0.006851217969517403</v>
+        <v>0.02597828933294155</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.01086407697856308</v>
+        <v>-0.00323509174540367</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.01086407697856308</v>
+        <v>-0.00323509174540367</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.01086407697856308</v>
+        <v>-0.00323509174540367</v>
       </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1368,37 +1368,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.02326990873879635</v>
+        <v>0.02334623958984958</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>0.006334121917364876</v>
+        <v>0.006423257248930289</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.01186326527453061</v>
+        <v>0.003686763315470533</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0003409260616370424</v>
+        <v>-0.001225655377026215</v>
       </c>
       <c r="H16" t="n">
-        <v>0.009128238125129523</v>
+        <v>0.009106960780278429</v>
       </c>
       <c r="I16" t="n">
         <v>0.01187364479494579</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.01522211223591942</v>
+        <v>0.007087023224312781</v>
       </c>
       <c r="K16" t="n">
-        <v>0.007267366562694662</v>
+        <v>-0.01867843658713746</v>
       </c>
       <c r="L16" t="n">
-        <v>0.007267366562694662</v>
+        <v>-0.01867843658713746</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.007267366562694662</v>
+        <v>-0.01867843658713746</v>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
@@ -1420,37 +1420,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.001096021483840859</v>
+        <v>-0.001135276461411058</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>-0.01186594108263764</v>
+        <v>-0.01153963015758521</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01427674223506969</v>
+        <v>0.006041890801675631</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.01184315317772612</v>
+        <v>-0.01297424835896993</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.007946154077846162</v>
+        <v>-0.00791644476465779</v>
       </c>
       <c r="I17" t="n">
         <v>-0.006570467302818691</v>
       </c>
       <c r="J17" t="n">
-        <v>7.948560702341064e-05</v>
+        <v>-0.01915670001997974</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.005199365583974622</v>
+        <v>0.01084217678568707</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.005199365583974622</v>
+        <v>0.01084217678568707</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.005199365583974622</v>
+        <v>0.01084217678568707</v>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
@@ -1476,37 +1476,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.01955374791814991</v>
+        <v>-0.01989691836387673</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
-        <v>0.003212637824505512</v>
+        <v>0.003639089425563576</v>
       </c>
       <c r="F18" t="n">
-        <v>0.009095317707812706</v>
+        <v>-0.000267592426703697</v>
       </c>
       <c r="G18" t="n">
-        <v>0.004934812421392497</v>
+        <v>-0.01052097238883889</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.007303982500159299</v>
+        <v>-0.007381185319247411</v>
       </c>
       <c r="I18" t="n">
         <v>-0.004741255389650215</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.0114945739148243</v>
+        <v>-0.02729983306254776</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.004365985806639432</v>
+        <v>0.005782498119299924</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.004365985806639432</v>
+        <v>0.005782498119299924</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.004365985806639432</v>
+        <v>0.005782498119299924</v>
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
@@ -1532,37 +1532,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.01571077157243086</v>
+        <v>-0.01545339853813594</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>0.004267814858712593</v>
+        <v>0.004322925292917011</v>
       </c>
       <c r="F19" t="n">
-        <v>0.005647702497908099</v>
+        <v>-0.009711448708457946</v>
       </c>
       <c r="G19" t="n">
-        <v>0.004673611482944459</v>
+        <v>0.006890932979637318</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.006601831368073253</v>
+        <v>-0.006571173478846938</v>
       </c>
       <c r="I19" t="n">
         <v>-0.005024797256991891</v>
       </c>
       <c r="J19" t="n">
-        <v>0.009447927202545062</v>
+        <v>0.006451798757356922</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.007990128223605128</v>
+        <v>0.0007931293757251749</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.007990128223605128</v>
+        <v>0.0007931293757251749</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>-0.007990128223605128</v>
+        <v>0.0007931293757251749</v>
       </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
@@ -1584,37 +1584,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.009956271758250869</v>
+        <v>0.009796079143843164</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>-0.005006833544273341</v>
+        <v>-0.004774373854974953</v>
       </c>
       <c r="F20" t="n">
-        <v>0.009721509124860365</v>
+        <v>-0.001218417936736717</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.005748933157957325</v>
+        <v>-0.01659785567191422</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.009823572872942913</v>
+        <v>-0.00980594525623781</v>
       </c>
       <c r="I20" t="n">
         <v>-0.006169556118782244</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.0253186096626263</v>
+        <v>0.005239006579315293</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.008158050470322017</v>
+        <v>0.002764813934592557</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.008158050470322017</v>
+        <v>0.002764813934592557</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>-0.008158050470322017</v>
+        <v>0.002764813934592557</v>
       </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
@@ -1636,37 +1636,37 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.005300213492008539</v>
+        <v>-0.00570230902809236</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>0.01680334867213394</v>
+        <v>0.01654423390976936</v>
       </c>
       <c r="F21" t="n">
-        <v>0.004735222077408883</v>
+        <v>-0.02003432412937296</v>
       </c>
       <c r="G21" t="n">
-        <v>0.007697500819900032</v>
+        <v>-0.01258124901524996</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.009935331277413249</v>
+        <v>-0.009949458637978345</v>
       </c>
       <c r="I21" t="n">
         <v>-0.01017601365504055</v>
       </c>
       <c r="J21" t="n">
-        <v>0.01305152829702044</v>
+        <v>-0.02343897902993137</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.01372975360519014</v>
+        <v>-0.007859911034396439</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.01372975360519014</v>
+        <v>-0.007859911034396439</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-0.01372975360519014</v>
+        <v>-0.007859911034396439</v>
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -1688,37 +1688,37 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.008283845611353825</v>
+        <v>0.007205545152221804</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>0.01116295158251806</v>
+        <v>0.01158410407936416</v>
       </c>
       <c r="F22" t="n">
-        <v>0.01849504883580195</v>
+        <v>-0.01994049046161962</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0107526649421066</v>
+        <v>-0.02717386879895475</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.0198344550013782</v>
+        <v>-0.01987639317905572</v>
       </c>
       <c r="I22" t="n">
         <v>-0.01713025143721005</v>
       </c>
       <c r="J22" t="n">
-        <v>0.007590651152202</v>
+        <v>0.0004640778625561794</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.02005689689827587</v>
+        <v>0.009169012494760499</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.02005689689827587</v>
+        <v>0.009169012494760499</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>-0.02005689689827587</v>
+        <v>0.009169012494760499</v>
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -1744,37 +1744,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.006441263105650522</v>
+        <v>0.006136369301454772</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>0.0130137524565501</v>
+        <v>0.01284851081794043</v>
       </c>
       <c r="F23" t="n">
-        <v>0.007272629858905193</v>
+        <v>-0.01275608134224325</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01600876086435043</v>
+        <v>0.01634454324578173</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.00871884399675376</v>
+        <v>-0.008755867358234692</v>
       </c>
       <c r="I23" t="n">
         <v>-0.01255258629410345</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.00317587135008713</v>
+        <v>0.003824189430728897</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.01013380398935216</v>
+        <v>-0.007450953898038154</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.01013380398935216</v>
+        <v>-0.007450953898038154</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>-0.01013380398935216</v>
+        <v>-0.007450953898038154</v>
       </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
@@ -1796,37 +1796,37 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.002234838521393541</v>
+        <v>0.003185699455427978</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>0.002021694128867765</v>
+        <v>0.002374643134985725</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.02476419910256796</v>
+        <v>0.006416828896673154</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.004495211123808444</v>
+        <v>0.005575577311023092</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02180537040821481</v>
+        <v>0.02185127319405093</v>
       </c>
       <c r="I24" t="n">
         <v>0.02253726483749059</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.00130007673734563</v>
+        <v>-0.01309152295407683</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0174503299460132</v>
+        <v>-0.01159524737580989</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0174503299460132</v>
+        <v>-0.01159524737580989</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>0.0174503299460132</v>
+        <v>-0.01159524737580989</v>
       </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
@@ -1852,37 +1852,37 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.02462292808891712</v>
+        <v>0.02515687943827517</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>0.0009841143753645748</v>
+        <v>0.0007909506556380262</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.01435726396629056</v>
+        <v>0.004485315347412614</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.006858083602323342</v>
+        <v>0.002973895318955812</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01150002564400102</v>
+        <v>0.01147743617109744</v>
       </c>
       <c r="I25" t="n">
         <v>0.0109187299727492</v>
       </c>
       <c r="J25" t="n">
-        <v>0.002240979422174362</v>
+        <v>0.0003448332356581201</v>
       </c>
       <c r="K25" t="n">
-        <v>0.008770965662838625</v>
+        <v>-0.01303921952956878</v>
       </c>
       <c r="L25" t="n">
-        <v>0.008770965662838625</v>
+        <v>-0.01303921952956878</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.008770965662838625</v>
+        <v>-0.01303921952956878</v>
       </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
@@ -1904,37 +1904,37 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-0.01263190322527613</v>
+        <v>-0.01290339862813594</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>0.001490879291635171</v>
+        <v>0.001803960936158437</v>
       </c>
       <c r="F26" t="n">
-        <v>0.001714591844583674</v>
+        <v>-0.005087429963497197</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0005169198926767957</v>
+        <v>-0.01422859861714394</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.00513286100531444</v>
+        <v>-0.005165468366618734</v>
       </c>
       <c r="I26" t="n">
         <v>-0.01001658673666347</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.00586887031631364</v>
+        <v>-0.02199675722573285</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.007364472390578894</v>
+        <v>0.00397648623905945</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.007364472390578894</v>
+        <v>0.00397648623905945</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>-0.007364472390578894</v>
+        <v>0.00397648623905945</v>
       </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
@@ -1960,37 +1960,37 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.01614552784582111</v>
+        <v>0.0164600126264005</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>-0.007641888689675546</v>
+        <v>-0.007252641698105667</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.02579559875982395</v>
+        <v>0.01292652234106089</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.01384898100195924</v>
+        <v>0.02516431444657257</v>
       </c>
       <c r="H27" t="n">
-        <v>0.02219243589569744</v>
+        <v>0.02216083797443352</v>
       </c>
       <c r="I27" t="n">
         <v>0.01890344744413789</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.006236589269584303</v>
+        <v>0.01182696312872424</v>
       </c>
       <c r="K27" t="n">
-        <v>0.01777407776696311</v>
+        <v>-0.02319023699160948</v>
       </c>
       <c r="L27" t="n">
-        <v>0.01777407776696311</v>
+        <v>-0.02319023699160948</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>0.01777407776696311</v>
+        <v>-0.02319023699160948</v>
       </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
@@ -2016,37 +2016,37 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.004582101207284047</v>
+        <v>-0.004742163741686549</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>-0.001277891091115644</v>
+        <v>-0.001196453423858137</v>
       </c>
       <c r="F28" t="n">
-        <v>0.01048654093146164</v>
+        <v>-0.004674141402965656</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0004306996972279878</v>
+        <v>-0.005745953989838158</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.00822583578503343</v>
+        <v>-0.008281227595249102</v>
       </c>
       <c r="I28" t="n">
         <v>-0.008152086854083472</v>
       </c>
       <c r="J28" t="n">
-        <v>0.005047839700050126</v>
+        <v>0.02201875937753802</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.00734137075765483</v>
+        <v>0.009894203147768125</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.00734137075765483</v>
+        <v>0.009894203147768125</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.00734137075765483</v>
+        <v>0.009894203147768125</v>
       </c>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
@@ -2072,37 +2072,37 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.00531415451656618</v>
+        <v>-0.004829002561160102</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>-0.009483023323320931</v>
+        <v>-0.009635420641416825</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.01410470120418805</v>
+        <v>0.01546226529049061</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.009823971176958846</v>
+        <v>-0.02003520944140837</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01744225068169002</v>
+        <v>0.01746085615443424</v>
       </c>
       <c r="I29" t="n">
         <v>0.01661224492048979</v>
       </c>
       <c r="J29" t="n">
-        <v>0.009506652406639417</v>
+        <v>-0.01061326536252559</v>
       </c>
       <c r="K29" t="n">
-        <v>0.01948544957941798</v>
+        <v>0.008761500062460001</v>
       </c>
       <c r="L29" t="n">
-        <v>0.01948544957941798</v>
+        <v>0.008761500062460001</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>0.01948544957941798</v>
+        <v>0.008761500062460001</v>
       </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
@@ -2128,37 +2128,37 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.005234805137392206</v>
+        <v>-0.005650332322013292</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>-0.01503540924141637</v>
+        <v>-0.01517796156711846</v>
       </c>
       <c r="F30" t="n">
-        <v>0.02116549313461972</v>
+        <v>-0.003768562902742516</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.01616924061476962</v>
+        <v>-0.01611525165261006</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.01728756049950242</v>
+        <v>-0.01728617531544701</v>
       </c>
       <c r="I30" t="n">
         <v>-0.01542497485699899</v>
       </c>
       <c r="J30" t="n">
-        <v>0.01566352778829018</v>
+        <v>0.003241245582398439</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.0131317674692707</v>
+        <v>0.02517635707105428</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.0131317674692707</v>
+        <v>0.02517635707105428</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>-0.0131317674692707</v>
+        <v>0.02517635707105428</v>
       </c>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
@@ -2184,37 +2184,37 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01698458189538327</v>
+        <v>0.01624372730574909</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>0.007866128858645153</v>
+        <v>0.00750373201214928</v>
       </c>
       <c r="F31" t="n">
-        <v>0.01979747407189896</v>
+        <v>-0.01408857483554299</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01033770281350811</v>
+        <v>-0.01487549089901963</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.02045879611435184</v>
+        <v>-0.02046772593870904</v>
       </c>
       <c r="I31" t="n">
         <v>-0.02025557121022284</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.01287680051306386</v>
+        <v>-0.001123116618161756</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.01845362233814489</v>
+        <v>0.006570363430814536</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.01845362233814489</v>
+        <v>0.006570363430814536</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.01845362233814489</v>
+        <v>0.006570363430814536</v>
       </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
@@ -2240,37 +2240,37 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.006300207804008312</v>
+        <v>0.005779685895187434</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>-0.003358240070329603</v>
+        <v>-0.003752471958098878</v>
       </c>
       <c r="F32" t="n">
-        <v>0.005920060748802428</v>
+        <v>-0.002625132201005288</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.002313754652550186</v>
+        <v>-0.01447027776281111</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.007688387347535493</v>
+        <v>-0.007723920980956838</v>
       </c>
       <c r="I32" t="n">
         <v>-0.01117334454293378</v>
       </c>
       <c r="J32" t="n">
-        <v>0.002330390421893428</v>
+        <v>-0.0004864400211933896</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.007312721092508842</v>
+        <v>0.00930496203619848</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.007312721092508842</v>
+        <v>0.00930496203619848</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>-0.007312721092508842</v>
+        <v>0.00930496203619848</v>
       </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
@@ -2296,37 +2296,37 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.02923019310520772</v>
+        <v>-0.02880934934437397</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>-0.01652959650118386</v>
+        <v>-0.01674910818996432</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.002491824291672971</v>
+        <v>0.01002812824112513</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.01198059772722391</v>
+        <v>0.01410188062807522</v>
       </c>
       <c r="H33" t="n">
-        <v>0.004960326822413073</v>
+        <v>0.004923553060942122</v>
       </c>
       <c r="I33" t="n">
         <v>-0.001813062024522481</v>
       </c>
       <c r="J33" t="n">
-        <v>0.02349167283205113</v>
+        <v>-0.007722500166711017</v>
       </c>
       <c r="K33" t="n">
-        <v>0.007939010237560409</v>
+        <v>0.01046894288275771</v>
       </c>
       <c r="L33" t="n">
-        <v>0.007939010237560409</v>
+        <v>0.01046894288275771</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>0.007939010237560409</v>
+        <v>0.01046894288275771</v>
       </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
@@ -2352,37 +2352,37 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.01115823980632959</v>
+        <v>-0.01080156446406258</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>-0.003319750116790004</v>
+        <v>-0.00331645174865807</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.007611254224450168</v>
+        <v>0.008141933509677339</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.003330203173208127</v>
+        <v>0.004613862616554504</v>
       </c>
       <c r="H34" t="n">
-        <v>0.01003024984120999</v>
+        <v>0.00998423627136945</v>
       </c>
       <c r="I34" t="n">
         <v>0.01138237082329483</v>
       </c>
       <c r="J34" t="n">
-        <v>0.01949998583334653</v>
+        <v>-0.02112237127770925</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01121485801659432</v>
+        <v>0.001624897408995896</v>
       </c>
       <c r="L34" t="n">
-        <v>0.01121485801659432</v>
+        <v>0.001624897408995896</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>0.01121485801659432</v>
+        <v>0.001624897408995896</v>
       </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
@@ -2408,37 +2408,37 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01647461105898444</v>
+        <v>0.0169848050953922</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>-0.01711472084458883</v>
+        <v>-0.01677903974316159</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.01401762622470505</v>
+        <v>0.02338045360721814</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.01529951696398068</v>
+        <v>0.0179972724958909</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01631998020479921</v>
+        <v>0.01635089095803564</v>
       </c>
       <c r="I35" t="n">
         <v>0.02218259157530366</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.0005847199143155518</v>
+        <v>-0.009541144701469696</v>
       </c>
       <c r="K35" t="n">
-        <v>0.01772926678917067</v>
+        <v>-0.008561160918446435</v>
       </c>
       <c r="L35" t="n">
-        <v>0.01772926678917067</v>
+        <v>-0.008561160918446435</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>0.01772926678917067</v>
+        <v>-0.008561160918446435</v>
       </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2464,37 +2464,37 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.02270644958025798</v>
+        <v>0.02243902947356118</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>0.01656757045470282</v>
+        <v>0.01653045157321806</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.002234137049365482</v>
+        <v>-0.01027687625107505</v>
       </c>
       <c r="G36" t="n">
-        <v>0.01677957398318296</v>
+        <v>0.02402203900888156</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.001576489407059576</v>
+        <v>-0.001596459807858392</v>
       </c>
       <c r="I36" t="n">
         <v>-0.002515635364625415</v>
       </c>
       <c r="J36" t="n">
-        <v>0.01558235757093167</v>
+        <v>0.004738371838367395</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.004262439338497573</v>
+        <v>-0.01570889275635571</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.004262439338497573</v>
+        <v>-0.01570889275635571</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>-0.004262439338497573</v>
+        <v>-0.01570889275635571</v>
       </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2520,37 +2520,37 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.01713563434942537</v>
+        <v>0.01631056519642261</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>0.01103650623346025</v>
+        <v>0.01129508137980325</v>
       </c>
       <c r="F37" t="n">
-        <v>0.01134849069393963</v>
+        <v>-0.01110811273232451</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01650855454834218</v>
+        <v>-0.0006551590342063613</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.01260722920828916</v>
+        <v>-0.01261031656841266</v>
       </c>
       <c r="I37" t="n">
         <v>-0.01464582970583318</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.005527097916335087</v>
+        <v>-0.0008313077398965218</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.01141044045641762</v>
+        <v>0.008987598215503927</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.01141044045641762</v>
+        <v>0.008987598215503927</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.01141044045641762</v>
+        <v>0.008987598215503927</v>
       </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>

</xml_diff>

<commit_message>
rerun monte carlo and minor changes
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,57 +505,54 @@
           <t>Economic allocation</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Ethanol</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Biodiesel</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Crude glycerol</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Electricity</t>
-        </is>
-      </c>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Biorefinery</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="n"/>
+          <t>Displacement allocation</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Energy allocation</t>
+        </is>
+      </c>
       <c r="R1" s="1" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
-      <c r="U1" s="1" t="n"/>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Biorefinery</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="n"/>
+      <c r="W1" s="1" t="n"/>
+      <c r="X1" s="1" t="n"/>
+      <c r="Y1" s="1" t="n"/>
+      <c r="Z1" s="1" t="n"/>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Economic allocation</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Ethanol</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Biodiesel</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Crude glycerol</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Electricity</t>
         </is>
@@ -574,34 +571,34 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
+          <t>Feedstock consumption [ton/yr]</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
           <t>Biodiesel production [Gal/ton]</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Ethanol production [Gal/ton]</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>Electricity production [kWhr/ton]</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>Natural gas consumption [cf/ton]</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>TCI [10^6*USD]</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>Feedstock consumption [ton/yr]</t>
-        </is>
-      </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
           <t>Heat exchanger network error [%]</t>
@@ -634,55 +631,80 @@
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
+          <t>Ethanol GWP [kg*CO2*eq / ga;]</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>Biofuel GWP [kg*CO2*eq / GGE]</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>Ethanol GWP [kg*CO2*eq / gal]</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>Biodiesel GWP [kg*CO2*eq / gal]</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
+        <is>
+          <t>Crude-glycerol GWP [kg*CO2*eq / kg]</t>
+        </is>
+      </c>
+      <c r="U2" s="1" t="inlineStr">
+        <is>
           <t>MFPP derivative [USD/ton]</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>Biodiesel production derivative [Gal/ton]</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>Ethanol production derivative [Gal/ton]</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>Electricity production derivative [kWhr/ton]</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
         <is>
           <t>Natural gas consumption derivative [cf/ton]</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>TCI derivative [10^6*USD]</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>GWP derivative [kg*CO2*eq / USD]</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>Ethanol GWP derivative [kg*CO2*eq / gal]</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
         <is>
           <t>Biodiesel GWP derivative [kg*CO2*eq / gal]</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="AD2" s="1" t="inlineStr">
         <is>
           <t>Crude glycerol GWP derivative [kg*CO2*eq / kg]</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
+      <c r="AE2" s="1" t="inlineStr">
         <is>
           <t>Electricity GWP derivative [kg*CO2*eq / MWhr]</t>
         </is>
@@ -712,41 +734,47 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.02658737885549515</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
-        <v>0.005465991194639646</v>
-      </c>
+        <v>-0.2131653165316531</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.06405040504050405</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>-0.01063662023346481</v>
+        <v>-0.1006540654065406</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04256176682247067</v>
+        <v>0.1287728772877288</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.007805750712230028</v>
+        <v>-0.07247524752475247</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.006983176887327074</v>
+        <v>0.09986198619861984</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.005555156068918668</v>
+        <v>0.02558791056991953</v>
       </c>
       <c r="K4" t="n">
-        <v>0.03173725470949018</v>
+        <v>0.09035703570357034</v>
       </c>
       <c r="L4" t="n">
-        <v>0.03173725470949018</v>
+        <v>0.09035703570357034</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.03173725470949018</v>
-      </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
+        <v>0.09035703570357034</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-0.1204320432043204</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.08774077407740774</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.08774077407740774</v>
+      </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
@@ -755,6 +783,11 @@
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
@@ -764,41 +797,47 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01021047688841907</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
-        <v>-0.01013502376540095</v>
-      </c>
+        <v>-0.08357635763576358</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.1119111911191119</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>0.01090468670818747</v>
+        <v>0.07633963396339634</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.00523009451320378</v>
+        <v>-0.05106510651065106</v>
       </c>
       <c r="H5" t="n">
-        <v>0.005649591297983651</v>
+        <v>0.115991599159916</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0005059528522381141</v>
+        <v>-0.1017341734173417</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0244145690650492</v>
+        <v>-0.03945978886527606</v>
       </c>
       <c r="K5" t="n">
-        <v>0.009640727809629112</v>
+        <v>-0.01334533453345334</v>
       </c>
       <c r="L5" t="n">
-        <v>0.009640727809629112</v>
+        <v>-0.01334533453345334</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.009640727809629112</v>
-      </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
+        <v>-0.01334533453345334</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.04554455445544554</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.0008160816081608161</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-0.0008160816081608161</v>
+      </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
@@ -807,6 +846,11 @@
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -816,41 +860,47 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1898265375450615</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>-0.4253799642471985</v>
-      </c>
+        <v>0.2035523552355235</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.9561716171617161</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>0.8335373874534955</v>
+        <v>-0.5004020402040203</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3258798638191945</v>
+        <v>0.882172217221722</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9999932175037286</v>
+        <v>0.1453225322532253</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9579628848145153</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>0.007026714779913105</v>
+        <v>0.07117894953890079</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.4333832774953311</v>
+        <v>-0.2689228922892289</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.4333832774953311</v>
+        <v>-0.2689228922892289</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>-0.4333832774953311</v>
-      </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
+        <v>-0.2689228922892289</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-0.8558175817581758</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-0.3336093609360936</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-0.3336093609360936</v>
+      </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
@@ -859,6 +909,11 @@
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -872,41 +927,47 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9426671344106852</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>0.002995317431812697</v>
-      </c>
+        <v>0.9358535853585358</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.004668466846684667</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>0.003223472384938895</v>
+        <v>0.176957695769577</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.009856131562245261</v>
+        <v>-0.1025502550255025</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005664523330580932</v>
+        <v>0.1825262526252625</v>
       </c>
       <c r="I7" t="n">
-        <v>0.001493300027732001</v>
+        <v>0.003672367236723672</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.009728802489008368</v>
+        <v>0.04981865902089943</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.005593015903720636</v>
+        <v>-0.2047284728472847</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.005593015903720636</v>
+        <v>-0.2047284728472847</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.005593015903720636</v>
-      </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
+        <v>-0.2047284728472847</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.1096309630963096</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-0.192019201920192</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-0.192019201920192</v>
+      </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
@@ -915,6 +976,11 @@
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -928,41 +994,47 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.01313509166140367</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>0.001354536150181446</v>
-      </c>
+        <v>0.1004620462046204</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001404140414041404</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>-0.007606005616240224</v>
+        <v>0.07725172517251723</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0288083400963336</v>
+        <v>-0.04573657365736573</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.01306648861865954</v>
+        <v>-0.005160516051605159</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.009443602841744113</v>
+        <v>0.02007800780078008</v>
       </c>
       <c r="J8" t="n">
-        <v>0.01585730368087417</v>
+        <v>-0.1279695785601937</v>
       </c>
       <c r="K8" t="n">
-        <v>0.01131375962055038</v>
+        <v>-0.02879087908790879</v>
       </c>
       <c r="L8" t="n">
-        <v>0.01131375962055038</v>
+        <v>-0.02879087908790879</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>0.01131375962055038</v>
-      </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
+        <v>-0.02879087908790879</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.04218421842184217</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-0.02868286828682868</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-0.02868286828682868</v>
+      </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
@@ -971,6 +1043,11 @@
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -984,41 +1061,47 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.02045771093030843</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>-0.01361019971240798</v>
-      </c>
+        <v>0.04688868886888688</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.04094809480948094</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.02089843955593758</v>
+        <v>-0.1627722772277228</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.009879947051197879</v>
+        <v>0.05824182418241824</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02695556805422272</v>
+        <v>-0.0147014701470147</v>
       </c>
       <c r="I9" t="n">
-        <v>0.02935640968625638</v>
+        <v>0.01807380738073807</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.01511229979866384</v>
+        <v>-0.05473687041652583</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0002645018025800721</v>
+        <v>0.08858085808580857</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0002645018025800721</v>
+        <v>0.08858085808580857</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>-0.0002645018025800721</v>
-      </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
+        <v>0.08858085808580857</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-0.06817881788178817</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.06862286228622862</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.06862286228622862</v>
+      </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
@@ -1027,6 +1110,11 @@
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1040,41 +1128,47 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.02999642414385696</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>0.005756988422279535</v>
-      </c>
+        <v>-0.01358535853585358</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.0417041704170417</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>-0.005379545975181838</v>
+        <v>0.1364296429642964</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.006492012067680481</v>
+        <v>-0.08016801680168015</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.001882962315318492</v>
+        <v>0.04796879687968796</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.0009429528377181134</v>
+        <v>-0.04614461446144614</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01335783306135146</v>
+        <v>0.02970743806369208</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.002089564979582599</v>
+        <v>-0.03193519351935194</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.002089564979582599</v>
+        <v>-0.03193519351935194</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>-0.002089564979582599</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
+        <v>-0.03193519351935194</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.08183618361836184</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-0.009864986498649865</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-0.009864986498649865</v>
+      </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
@@ -1083,6 +1177,11 @@
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
@@ -1092,41 +1191,47 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1123469959498798</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
-        <v>-0.007713633908545355</v>
-      </c>
+        <v>0.1529432943294329</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.2451005100510051</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.002453693474147739</v>
+        <v>-0.05587758775877587</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.01776083571843343</v>
+        <v>-0.00072007200720072</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.005572430814897231</v>
+        <v>0.01514551455145514</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2739322870212915</v>
+        <v>-0.03181518151815181</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0250161915335958</v>
+        <v>-0.1647270534718288</v>
       </c>
       <c r="K11" t="n">
-        <v>0.01980312108012484</v>
+        <v>0.08705670567056706</v>
       </c>
       <c r="L11" t="n">
-        <v>0.01980312108012484</v>
+        <v>0.08705670567056706</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>0.01980312108012484</v>
-      </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
+        <v>0.08705670567056706</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-0.000132013201320132</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.08004800480048005</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.08004800480048005</v>
+      </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
@@ -1135,6 +1240,11 @@
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -1144,41 +1254,47 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.2301963123758525</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>-0.002983256375330254</v>
-      </c>
+        <v>-0.2197299729972997</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.1068946894689469</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>0.002545738853829554</v>
+        <v>-0.1727572757275727</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01394744830189793</v>
+        <v>0.04026402640264026</v>
       </c>
       <c r="H12" t="n">
-        <v>0.007194415583776623</v>
+        <v>-0.01135313531353135</v>
       </c>
       <c r="I12" t="n">
-        <v>0.00596510827060433</v>
+        <v>-0.08556855685568555</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.004179991492478003</v>
+        <v>-0.08029475527584935</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.01292686093307444</v>
+        <v>0.1258685868586859</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.01292686093307444</v>
+        <v>0.1258685868586859</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>-0.01292686093307444</v>
-      </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
+        <v>0.1258685868586859</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-0.05492949294929492</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.1192439243924392</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.1192439243924392</v>
+      </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
@@ -1187,6 +1303,11 @@
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1200,41 +1321,47 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01080141489605659</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>0.01996635593465423</v>
-      </c>
+        <v>0.01965796579657966</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.01854185418541854</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>0.003818433848737354</v>
+        <v>0.07818781878187818</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03070264452410577</v>
+        <v>-0.06311431143114311</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01397413169496526</v>
+        <v>0.0473087308730873</v>
       </c>
       <c r="I13" t="n">
-        <v>0.008566614198664566</v>
+        <v>0.01018901890189019</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.007947490557074603</v>
+        <v>-0.1581153919985875</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.03490118789204751</v>
+        <v>-0.07997599759975996</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.03490118789204751</v>
+        <v>-0.07997599759975996</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>-0.03490118789204751</v>
-      </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
+        <v>-0.07997599759975996</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.07789978997899788</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-0.06403840384038403</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-0.06403840384038403</v>
+      </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
@@ -1243,6 +1370,11 @@
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1256,41 +1388,47 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.005271760818870433</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.00833421527736861</v>
-      </c>
+        <v>0.007908790879087909</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.01683768376837684</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>-0.004312245004489799</v>
+        <v>-0.1486588658865887</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01820064063202562</v>
+        <v>0.1184518451845184</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.0032442650257706</v>
+        <v>-0.09050105010501049</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.007119685916787436</v>
+        <v>0.03548754875487549</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.01816328662100451</v>
+        <v>-0.03695564460156884</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.008689076411563053</v>
+        <v>0.09185718571857185</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.008689076411563053</v>
+        <v>0.09185718571857185</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>-0.008689076411563053</v>
-      </c>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
+        <v>0.09185718571857185</v>
+      </c>
+      <c r="P14" t="n">
+        <v>-0.1248364836483648</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.09918991899189919</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.09918991899189919</v>
+      </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
@@ -1299,6 +1437,11 @@
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1312,41 +1455,47 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.006335240893409635</v>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>0.01024268200970728</v>
-      </c>
+        <v>-0.0984098409840984</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.04474047404740474</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>-0.007798515863940633</v>
+        <v>-0.05635763576357636</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01462896768915871</v>
+        <v>0.005100510051005099</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.0122924876276995</v>
+        <v>0.03242724272427242</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.01063130442525218</v>
+        <v>-0.03284728472847284</v>
       </c>
       <c r="J15" t="n">
-        <v>0.02597828933294155</v>
+        <v>0.04846750204407899</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.00323509174540367</v>
+        <v>0.03493549354935493</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.00323509174540367</v>
+        <v>0.03493549354935493</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.00323509174540367</v>
-      </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
+        <v>0.03493549354935493</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-0.01742574257425742</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.0436003600360036</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0436003600360036</v>
+      </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
@@ -1355,6 +1504,11 @@
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1368,41 +1522,47 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.02334623958984958</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>0.006423257248930289</v>
-      </c>
+        <v>0.00984098409840984</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.03991599159915991</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>0.003686763315470533</v>
+        <v>0.004344434443444344</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.001225655377026215</v>
+        <v>0.04878487848784878</v>
       </c>
       <c r="H16" t="n">
-        <v>0.009106960780278429</v>
+        <v>0.1074467446744674</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01187364479494579</v>
+        <v>0.04448844884488448</v>
       </c>
       <c r="J16" t="n">
-        <v>0.007087023224312781</v>
+        <v>-0.007602509922909678</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.01867843658713746</v>
+        <v>-0.05128112811281128</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.01867843658713746</v>
+        <v>-0.05128112811281128</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>-0.01867843658713746</v>
-      </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
+        <v>-0.05128112811281128</v>
+      </c>
+      <c r="P16" t="n">
+        <v>-0.04484848484848484</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-0.02633063306330633</v>
+      </c>
+      <c r="R16" t="n">
+        <v>-0.02633063306330633</v>
+      </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
@@ -1411,6 +1571,11 @@
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
@@ -1420,41 +1585,47 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.001135276461411058</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>-0.01153963015758521</v>
-      </c>
+        <v>-0.07335133513351336</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.0794119411941194</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>0.006041890801675631</v>
+        <v>0.08656465646564655</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.01297424835896993</v>
+        <v>-0.05215721572157215</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.00791644476465779</v>
+        <v>-0.06681068106810681</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.006570467302818691</v>
+        <v>-0.05272127212721272</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.01915670001997974</v>
+        <v>0.04616753261242464</v>
       </c>
       <c r="K17" t="n">
-        <v>0.01084217678568707</v>
+        <v>0.07468346834683467</v>
       </c>
       <c r="L17" t="n">
-        <v>0.01084217678568707</v>
+        <v>0.07468346834683467</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>0.01084217678568707</v>
-      </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
+        <v>0.07468346834683467</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.05857785778577856</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.08866486648664865</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.08866486648664865</v>
+      </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
@@ -1463,6 +1634,11 @@
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1476,41 +1652,47 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.01989691836387673</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="n">
-        <v>0.003639089425563576</v>
-      </c>
+        <v>-0.02774677467746775</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.04709270927092709</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>-0.000267592426703697</v>
+        <v>0.09158115811581156</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.01052097238883889</v>
+        <v>-0.05412541254125412</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.007381185319247411</v>
+        <v>-0.02691869186918691</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.004741255389650215</v>
+        <v>-0.02072607260726072</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.02729983306254776</v>
+        <v>-0.1435709377858804</v>
       </c>
       <c r="K18" t="n">
-        <v>0.005782498119299924</v>
+        <v>-0.07005100510051004</v>
       </c>
       <c r="L18" t="n">
-        <v>0.005782498119299924</v>
+        <v>-0.07005100510051004</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>0.005782498119299924</v>
-      </c>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
+        <v>-0.07005100510051004</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.05581758175817582</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>-0.05246924692469247</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-0.05246924692469247</v>
+      </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
@@ -1519,6 +1701,11 @@
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1532,41 +1719,47 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.01545339853813594</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="n">
-        <v>0.004322925292917011</v>
-      </c>
+        <v>-0.1481188118811881</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.001716171617161716</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>-0.009711448708457946</v>
+        <v>0.06016201620162015</v>
       </c>
       <c r="G19" t="n">
-        <v>0.006890932979637318</v>
+        <v>-0.04824482448244824</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.006571173478846938</v>
+        <v>0.03411941194119412</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.005024797256991891</v>
+        <v>-0.01914191419141914</v>
       </c>
       <c r="J19" t="n">
-        <v>0.006451798757356922</v>
+        <v>0.01569744149959391</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0007931293757251749</v>
+        <v>-0.05408940894089408</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0007931293757251749</v>
+        <v>-0.05408940894089408</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>0.0007931293757251749</v>
-      </c>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
+        <v>-0.05408940894089408</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.05537353735373536</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>-0.06191419141914191</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-0.06191419141914191</v>
+      </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
@@ -1575,6 +1768,11 @@
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
@@ -1584,41 +1782,47 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.009796079143843164</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="n">
-        <v>-0.004774373854974953</v>
-      </c>
+        <v>-0.008964896489648964</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.02013801380138014</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>-0.001218417936736717</v>
+        <v>0.0738073807380738</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.01659785567191422</v>
+        <v>-0.0008040804080408039</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.00980594525623781</v>
+        <v>-0.03441944194419441</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.006169556118782244</v>
+        <v>0.01422142214221422</v>
       </c>
       <c r="J20" t="n">
-        <v>0.005239006579315293</v>
+        <v>0.03846894041560774</v>
       </c>
       <c r="K20" t="n">
-        <v>0.002764813934592557</v>
+        <v>-0.02442244224422442</v>
       </c>
       <c r="L20" t="n">
-        <v>0.002764813934592557</v>
+        <v>-0.02442244224422442</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0.002764813934592557</v>
-      </c>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
+        <v>-0.02442244224422442</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.006732673267326732</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>-0.03174317431743174</v>
+      </c>
+      <c r="R20" t="n">
+        <v>-0.03174317431743174</v>
+      </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
@@ -1627,6 +1831,11 @@
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+      <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
@@ -1636,41 +1845,47 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.00570230902809236</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>0.01654423390976936</v>
-      </c>
+        <v>0.05174917491749174</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.1197239723972397</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>-0.02003432412937296</v>
+        <v>-0.02221422142214221</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.01258124901524996</v>
+        <v>0.06832283228322832</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.009949458637978345</v>
+        <v>0.08056405640564056</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.01017601365504055</v>
+        <v>0.08284428442844284</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.02343897902993137</v>
+        <v>0.01962480444555199</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.007859911034396439</v>
+        <v>-0.05456945694569457</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.007859911034396439</v>
+        <v>-0.05456945694569457</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-0.007859911034396439</v>
-      </c>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
+        <v>-0.05456945694569457</v>
+      </c>
+      <c r="P21" t="n">
+        <v>-0.05768976897689768</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>-0.07511551155115512</v>
+      </c>
+      <c r="R21" t="n">
+        <v>-0.07511551155115512</v>
+      </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
@@ -1679,6 +1894,11 @@
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
@@ -1688,41 +1908,47 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.007205545152221804</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="n">
-        <v>0.01158410407936416</v>
-      </c>
+        <v>-0.0303990399039904</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0.1012901290129013</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>-0.01994049046161962</v>
+        <v>0.1369216921692169</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.02717386879895475</v>
+        <v>-0.1252565256525653</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.01987639317905572</v>
+        <v>0.01404140414041404</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.01713025143721005</v>
+        <v>-0.1008460846084608</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0004640778625561794</v>
+        <v>0.08596360943637602</v>
       </c>
       <c r="K22" t="n">
-        <v>0.009169012494760499</v>
+        <v>-0.05534953495349534</v>
       </c>
       <c r="L22" t="n">
-        <v>0.009169012494760499</v>
+        <v>-0.05534953495349534</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.009169012494760499</v>
-      </c>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
+        <v>-0.05534953495349534</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.1288808880888089</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-0.05101710171017101</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-0.05101710171017101</v>
+      </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
@@ -1731,6 +1957,11 @@
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1744,41 +1975,47 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.006136369301454772</v>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="n">
-        <v>0.01284851081794043</v>
-      </c>
+        <v>-0.06720672067206719</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-0.08976897689768974</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>-0.01275608134224325</v>
+        <v>0.0592019201920192</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01634454324578173</v>
+        <v>-0.04634863486348634</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.008755867358234692</v>
+        <v>0.001044104410441044</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.01255258629410345</v>
+        <v>-0.03285928592859286</v>
       </c>
       <c r="J23" t="n">
-        <v>0.003824189430728897</v>
+        <v>0.1021774931582213</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.007450953898038154</v>
+        <v>-0.02269426942694269</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.007450953898038154</v>
+        <v>-0.02269426942694269</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>-0.007450953898038154</v>
-      </c>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
+        <v>-0.02269426942694269</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.0548094809480948</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>-0.01015301530153015</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-0.01015301530153015</v>
+      </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
@@ -1787,6 +2024,11 @@
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
@@ -1796,41 +2038,47 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.003185699455427978</v>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="n">
-        <v>0.002374643134985725</v>
-      </c>
+        <v>-0.02325832583258326</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.07839183918391837</v>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>0.006416828896673154</v>
+        <v>0.01690969096909691</v>
       </c>
       <c r="G24" t="n">
-        <v>0.005575577311023092</v>
+        <v>-0.07278727872787277</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02185127319405093</v>
+        <v>0.007956795679567957</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02253726483749059</v>
+        <v>-0.09218121812181217</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.01309152295407683</v>
+        <v>-0.06836854302711427</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.01159524737580989</v>
+        <v>0.04704470447044704</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.01159524737580989</v>
+        <v>0.04704470447044704</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>-0.01159524737580989</v>
-      </c>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
+        <v>0.04704470447044704</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.06468646864686468</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.05486948694869486</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.05486948694869486</v>
+      </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
@@ -1839,6 +2087,11 @@
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr"/>
+      <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1852,41 +2105,47 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.02515687943827517</v>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="n">
-        <v>0.0007909506556380262</v>
-      </c>
+        <v>0.05575757575757576</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.2316951695169517</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>0.004485315347412614</v>
+        <v>-0.1602880288028803</v>
       </c>
       <c r="G25" t="n">
-        <v>0.002973895318955812</v>
+        <v>0.2333753375337533</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01147743617109744</v>
+        <v>-0.09618961896189619</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0109187299727492</v>
+        <v>0.2555295529552955</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0003448332356581201</v>
+        <v>-0.008647404651650818</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.01303921952956878</v>
+        <v>0.02227422742274227</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.01303921952956878</v>
+        <v>0.02227422742274227</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>-0.01303921952956878</v>
-      </c>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
+        <v>0.02227422742274227</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-0.228022802280228</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.01263726372637264</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.01263726372637264</v>
+      </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
@@ -1895,6 +2154,11 @@
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr"/>
+      <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
@@ -1904,41 +2168,47 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-0.01290339862813594</v>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>0.001803960936158437</v>
-      </c>
+        <v>-0.09143714371437144</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.06897089708970895</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>-0.005087429963497197</v>
+        <v>-0.1169276927692769</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.01422859861714394</v>
+        <v>0.02229822982298229</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.005165468366618734</v>
+        <v>0.00294029402940294</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.01001658673666347</v>
+        <v>-0.04523252325232523</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.02199675722573285</v>
+        <v>0.01508491700343531</v>
       </c>
       <c r="K26" t="n">
-        <v>0.00397648623905945</v>
+        <v>0.05492949294929492</v>
       </c>
       <c r="L26" t="n">
-        <v>0.00397648623905945</v>
+        <v>0.05492949294929492</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>0.00397648623905945</v>
-      </c>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
+        <v>0.05492949294929492</v>
+      </c>
+      <c r="P26" t="n">
+        <v>-0.0287068706870687</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.02508250825082508</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.02508250825082508</v>
+      </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
@@ -1947,6 +2217,11 @@
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
+      <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1960,41 +2235,47 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.0164600126264005</v>
-      </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="n">
-        <v>-0.007252641698105667</v>
-      </c>
+        <v>-0.07395139513951395</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.1291689168916892</v>
+      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>0.01292652234106089</v>
+        <v>-0.05028502850285028</v>
       </c>
       <c r="G27" t="n">
-        <v>0.02516431444657257</v>
+        <v>0.09524152415241523</v>
       </c>
       <c r="H27" t="n">
-        <v>0.02216083797443352</v>
+        <v>0.1558955895589559</v>
       </c>
       <c r="I27" t="n">
-        <v>0.01890344744413789</v>
+        <v>0.1097389738973897</v>
       </c>
       <c r="J27" t="n">
-        <v>0.01182696312872424</v>
+        <v>-0.01631597113787172</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.02319023699160948</v>
+        <v>-0.1075787578757876</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.02319023699160948</v>
+        <v>-0.1075787578757876</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-0.02319023699160948</v>
-      </c>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
+        <v>-0.1075787578757876</v>
+      </c>
+      <c r="P27" t="n">
+        <v>-0.09615361536153615</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>-0.1025262526252625</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-0.1025262526252625</v>
+      </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
@@ -2003,6 +2284,11 @@
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -2016,41 +2302,47 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.004742163741686549</v>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="n">
-        <v>-0.001196453423858137</v>
-      </c>
+        <v>-0.2093969396939694</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.05515751575157515</v>
+      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>-0.004674141402965656</v>
+        <v>0.03667566756675668</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.005745953989838158</v>
+        <v>-0.06145814581458145</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.008281227595249102</v>
+        <v>0.1746654665466546</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.008152086854083472</v>
+        <v>-0.067998799879988</v>
       </c>
       <c r="J28" t="n">
-        <v>0.02201875937753802</v>
+        <v>0.02074176087972356</v>
       </c>
       <c r="K28" t="n">
-        <v>0.009894203147768125</v>
+        <v>-0.06095409540954094</v>
       </c>
       <c r="L28" t="n">
-        <v>0.009894203147768125</v>
+        <v>-0.06095409540954094</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>0.009894203147768125</v>
-      </c>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
+        <v>-0.06095409540954094</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.06287428742874286</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>-0.05753375337533752</v>
+      </c>
+      <c r="R28" t="n">
+        <v>-0.05753375337533752</v>
+      </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
@@ -2059,6 +2351,11 @@
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -2072,41 +2369,47 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.004829002561160102</v>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="n">
-        <v>-0.009635420641416825</v>
-      </c>
+        <v>-0.06450645064506449</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-0.1674407440744074</v>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>0.01546226529049061</v>
+        <v>0.03527152715271527</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.02003520944140837</v>
+        <v>-0.08661266126612661</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01746085615443424</v>
+        <v>0.1521032103210321</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01661224492048979</v>
+        <v>-0.1164116411641164</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.01061326536252559</v>
+        <v>-0.08307513607703987</v>
       </c>
       <c r="K29" t="n">
-        <v>0.008761500062460001</v>
+        <v>0.02263426342634263</v>
       </c>
       <c r="L29" t="n">
-        <v>0.008761500062460001</v>
+        <v>0.02263426342634263</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>0.008761500062460001</v>
-      </c>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
+        <v>0.02263426342634263</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.09245724572457245</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.03701170117011701</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.03701170117011701</v>
+      </c>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
@@ -2115,6 +2418,11 @@
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -2128,41 +2436,47 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.005650332322013292</v>
-      </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="n">
-        <v>-0.01517796156711846</v>
-      </c>
+        <v>0.1938433843384338</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.03482748274827482</v>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>-0.003768562902742516</v>
+        <v>0.06258625862586258</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.01611525165261006</v>
+        <v>-0.0275067506750675</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.01728617531544701</v>
+        <v>0.01677767776777678</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.01542497485699899</v>
+        <v>0.01424542454245424</v>
       </c>
       <c r="J30" t="n">
-        <v>0.003241245582398439</v>
+        <v>-0.03368284214660378</v>
       </c>
       <c r="K30" t="n">
-        <v>0.02517635707105428</v>
+        <v>-0.01618961896189619</v>
       </c>
       <c r="L30" t="n">
-        <v>0.02517635707105428</v>
+        <v>-0.01618961896189619</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>0.02517635707105428</v>
-      </c>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
+        <v>-0.01618961896189619</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.02808280828082808</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>-0.01638163816381638</v>
+      </c>
+      <c r="R30" t="n">
+        <v>-0.01638163816381638</v>
+      </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
@@ -2171,6 +2485,11 @@
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr"/>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -2184,41 +2503,47 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01624372730574909</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="n">
-        <v>0.00750373201214928</v>
-      </c>
+        <v>-0.00276027602760276</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.015997599759976</v>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>-0.01408857483554299</v>
+        <v>-0.06035403540354035</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.01487549089901963</v>
+        <v>0.0216021602160216</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.02046772593870904</v>
+        <v>-0.01975397539753975</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.02025557121022284</v>
+        <v>-0.03247524752475248</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.001123116618161756</v>
+        <v>-0.2338282238374858</v>
       </c>
       <c r="K31" t="n">
-        <v>0.006570363430814536</v>
+        <v>0.01646564656465646</v>
       </c>
       <c r="L31" t="n">
-        <v>0.006570363430814536</v>
+        <v>0.01646564656465646</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>0.006570363430814536</v>
-      </c>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
+        <v>0.01646564656465646</v>
+      </c>
+      <c r="P31" t="n">
+        <v>-0.02271827182718272</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.01978997899789979</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.01978997899789979</v>
+      </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
@@ -2227,6 +2552,11 @@
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -2240,41 +2570,47 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.005779685895187434</v>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="n">
-        <v>-0.003752471958098878</v>
-      </c>
+        <v>0.007908790879087909</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-0.1639483948394839</v>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>-0.002625132201005288</v>
+        <v>-0.05189318931893189</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.01447027776281111</v>
+        <v>-0.06085808580858085</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.007723920980956838</v>
+        <v>0.01666966696669667</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.01117334454293378</v>
+        <v>-0.1241884188418842</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.0004864400211933896</v>
+        <v>-0.03391704268925265</v>
       </c>
       <c r="K32" t="n">
-        <v>0.00930496203619848</v>
+        <v>0.1068826882688269</v>
       </c>
       <c r="L32" t="n">
-        <v>0.00930496203619848</v>
+        <v>0.1068826882688269</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>0.00930496203619848</v>
-      </c>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+        <v>0.1068826882688269</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.05227722772277228</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.1059105910591059</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.1059105910591059</v>
+      </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
@@ -2283,6 +2619,11 @@
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -2296,41 +2637,47 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.02880934934437397</v>
-      </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="n">
-        <v>-0.01674910818996432</v>
-      </c>
+        <v>0.03397539753975398</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-0.03914791479147915</v>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>0.01002812824112513</v>
+        <v>0.1348334833483348</v>
       </c>
       <c r="G33" t="n">
-        <v>0.01410188062807522</v>
+        <v>-0.1019021902190219</v>
       </c>
       <c r="H33" t="n">
-        <v>0.004923553060942122</v>
+        <v>0.1082988298829883</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.001813062024522481</v>
+        <v>-0.03152715271527153</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.007722500166711017</v>
+        <v>0.1449641307575352</v>
       </c>
       <c r="K33" t="n">
-        <v>0.01046894288275771</v>
+        <v>-0.07234323432343234</v>
       </c>
       <c r="L33" t="n">
-        <v>0.01046894288275771</v>
+        <v>-0.07234323432343234</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>0.01046894288275771</v>
-      </c>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+        <v>-0.07234323432343234</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.1068586858685869</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>-0.08577257725772576</v>
+      </c>
+      <c r="R33" t="n">
+        <v>-0.08577257725772576</v>
+      </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
@@ -2339,6 +2686,11 @@
       <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -2352,41 +2704,47 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.01080156446406258</v>
-      </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="n">
-        <v>-0.00331645174865807</v>
-      </c>
+        <v>-0.1238403840384038</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-0.0833123312331233</v>
+      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>0.008141933509677339</v>
+        <v>0.02207020702070207</v>
       </c>
       <c r="G34" t="n">
-        <v>0.004613862616554504</v>
+        <v>-0.05749774977497749</v>
       </c>
       <c r="H34" t="n">
-        <v>0.00998423627136945</v>
+        <v>0.03798379837983798</v>
       </c>
       <c r="I34" t="n">
-        <v>0.01138237082329483</v>
+        <v>-0.07822382238223821</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.02112237127770925</v>
+        <v>-0.1151846309884127</v>
       </c>
       <c r="K34" t="n">
-        <v>0.001624897408995896</v>
+        <v>0.04662466246624661</v>
       </c>
       <c r="L34" t="n">
-        <v>0.001624897408995896</v>
+        <v>0.04662466246624661</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>0.001624897408995896</v>
-      </c>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
+        <v>0.04662466246624661</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.05405340534053405</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.059009900990099</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.059009900990099</v>
+      </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
@@ -2395,6 +2753,11 @@
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
+      <c r="AB34" t="inlineStr"/>
+      <c r="AC34" t="inlineStr"/>
+      <c r="AD34" t="inlineStr"/>
+      <c r="AE34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -2408,41 +2771,47 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.0169848050953922</v>
-      </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="n">
-        <v>-0.01677903974316159</v>
-      </c>
+        <v>-0.04296429642964296</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.01956195619561956</v>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
-        <v>0.02338045360721814</v>
+        <v>-0.1094149414941494</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0179972724958909</v>
+        <v>0.06918691869186917</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01635089095803564</v>
+        <v>-0.1854905490549055</v>
       </c>
       <c r="I35" t="n">
-        <v>0.02218259157530366</v>
+        <v>-0.01656165616561656</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.009541144701469696</v>
+        <v>0.01261079845032411</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.008561160918446435</v>
+        <v>0.1831383138313831</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.008561160918446435</v>
+        <v>0.1831383138313831</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>-0.008561160918446435</v>
-      </c>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
+        <v>0.1831383138313831</v>
+      </c>
+      <c r="P35" t="n">
+        <v>-0.08136813681368135</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.1818901890189019</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.1818901890189019</v>
+      </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
@@ -2451,6 +2820,11 @@
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr"/>
       <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr"/>
+      <c r="AB35" t="inlineStr"/>
+      <c r="AC35" t="inlineStr"/>
+      <c r="AD35" t="inlineStr"/>
+      <c r="AE35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -2464,41 +2838,47 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.02243902947356118</v>
-      </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="n">
-        <v>0.01653045157321806</v>
-      </c>
+        <v>-0.005592559255925592</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-0.07501950195019501</v>
+      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>-0.01027687625107505</v>
+        <v>0.1141314131413141</v>
       </c>
       <c r="G36" t="n">
-        <v>0.02402203900888156</v>
+        <v>-0.1101350135013501</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.001596459807858392</v>
+        <v>0.1112631263126312</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.002515635364625415</v>
+        <v>-0.08973297329732971</v>
       </c>
       <c r="J36" t="n">
-        <v>0.004738371838367395</v>
+        <v>-0.02051356547919388</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.01570889275635571</v>
+        <v>-0.1543234323432343</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.01570889275635571</v>
+        <v>-0.1543234323432343</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>-0.01570889275635571</v>
-      </c>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
+        <v>-0.1543234323432343</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0.1185598559855985</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>-0.1419381938193819</v>
+      </c>
+      <c r="R36" t="n">
+        <v>-0.1419381938193819</v>
+      </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
@@ -2507,6 +2887,11 @@
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr"/>
+      <c r="AA36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr"/>
+      <c r="AC36" t="inlineStr"/>
+      <c r="AD36" t="inlineStr"/>
+      <c r="AE36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -2520,41 +2905,47 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.01631056519642261</v>
-      </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="n">
-        <v>0.01129508137980325</v>
-      </c>
+        <v>-0.09300930093009299</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.03245124512451245</v>
+      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>-0.01110811273232451</v>
+        <v>0.05388538853885388</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.0006551590342063613</v>
+        <v>-0.01444944494449445</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.01261031656841266</v>
+        <v>0.02257425742574257</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.01464582970583318</v>
+        <v>0.001272127212721272</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.0008313077398965218</v>
+        <v>0.09300764114219991</v>
       </c>
       <c r="K37" t="n">
-        <v>0.008987598215503927</v>
+        <v>-0.024998499849985</v>
       </c>
       <c r="L37" t="n">
-        <v>0.008987598215503927</v>
+        <v>-0.024998499849985</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>0.008987598215503927</v>
-      </c>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+        <v>-0.024998499849985</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.02342634263426343</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>-0.02241824182418242</v>
+      </c>
+      <c r="R37" t="n">
+        <v>-0.02241824182418242</v>
+      </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
@@ -2563,11 +2954,18 @@
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr"/>
+      <c r="AA37" t="inlineStr"/>
+      <c r="AB37" t="inlineStr"/>
+      <c r="AC37" t="inlineStr"/>
+      <c r="AD37" t="inlineStr"/>
+      <c r="AE37" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="C1:J1"/>
-    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:Z1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A16:A17"/>

</xml_diff>

<commit_message>
implement kde plots and rerun some simulations
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -734,46 +734,46 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.001573882238955289</v>
+        <v>-0.003683041299321651</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002440304641612186</v>
+        <v>-0.0006704834204794681</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>-0.007590607791624311</v>
+        <v>0.003952041566081662</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0002393114975724599</v>
+        <v>0.002317578908703156</v>
       </c>
       <c r="H4" t="n">
-        <v>0.002017268144690725</v>
+        <v>0.0007377123175084925</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0002205411928216477</v>
+        <v>0.00265087325803493</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.005761896560602432</v>
+        <v>-0.02793869307072573</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01238320407932816</v>
+        <v>-0.0260007075680283</v>
       </c>
       <c r="L4" t="n">
-        <v>0.01238320407932816</v>
+        <v>-0.0260007075680283</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.01238320407932816</v>
+        <v>-0.0260007075680283</v>
       </c>
       <c r="P4" t="n">
-        <v>0.009552136702085467</v>
+        <v>-0.02354800414192016</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.01235546891021876</v>
+        <v>-0.02597311361492454</v>
       </c>
       <c r="R4" t="n">
-        <v>0.01235546891021876</v>
+        <v>-0.02597311361492454</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -797,46 +797,46 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.007847830969913238</v>
+        <v>0.01328333630733345</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.01886649176265967</v>
+        <v>-0.00729627293476785</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>-0.001182612143304486</v>
+        <v>-0.008390087279603491</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.01541095213643809</v>
+        <v>-0.01371980128479205</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.03002834318513372</v>
+        <v>-0.006515048420601935</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.01553504644540186</v>
+        <v>-0.0137976325199053</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01735000232280532</v>
+        <v>-0.02272228994808735</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.01980398930415957</v>
+        <v>0.0008110142724405708</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.01980398930415957</v>
+        <v>0.0008110142724405708</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>-0.01980398930415957</v>
+        <v>0.0008110142724405708</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.007009970488398819</v>
+        <v>0.004474588594983544</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.01917856598314263</v>
+        <v>0.001091258827650353</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.01917856598314263</v>
+        <v>0.001091258827650353</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -856,50 +856,50 @@
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Capacity [ton/hr]</t>
+          <t>Cane operating days [day/yr]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2050220979288839</v>
+        <v>0.1647024152280966</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9579101443324056</v>
+        <v>-0.001264774542012799</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>0.9369108263404329</v>
+        <v>-0.8939095590203823</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9999295841891833</v>
+        <v>-0.9998557406982296</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6454598878023954</v>
+        <v>-0.654473448834938</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9999999910719995</v>
+        <v>-0.9999999963519998</v>
       </c>
       <c r="J6" t="n">
-        <v>0.01991940049975821</v>
+        <v>-0.003798025922060888</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.1877089587083583</v>
+        <v>0.1196986640519465</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.1877089587083583</v>
+        <v>0.1196986640519465</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>-0.1877089587083583</v>
+        <v>0.1196986640519465</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.6733568067422722</v>
+        <v>0.469053351498134</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.2345470292858811</v>
+        <v>0.1488071518082861</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.2345470292858811</v>
+        <v>0.1488071518082861</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -916,57 +916,53 @@
       <c r="AE6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Stream-ethanol</t>
-        </is>
-      </c>
+      <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Price [USD/gal]</t>
+          <t>Sorghum operating days [day/yr]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9443060241082409</v>
+        <v>-0.006737889581515583</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02428762417150496</v>
+        <v>0.005517464063567663</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>0.01847437158697486</v>
+        <v>-0.006117530836701232</v>
       </c>
       <c r="G7" t="n">
-        <v>0.02259481731979269</v>
+        <v>-0.006981439383257574</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0197424626136985</v>
+        <v>-0.02262832727313309</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0227738274709531</v>
+        <v>-0.006706927468277097</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.02294466274493687</v>
+        <v>-0.02079875377557708</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.002297450683898027</v>
+        <v>-0.01174169614966784</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.002297450683898027</v>
+        <v>-0.01174169614966784</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.002297450683898027</v>
+        <v>-0.01174169614966784</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.01331974296478972</v>
+        <v>-0.00773200350928014</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.003454306698172267</v>
+        <v>-0.01168885457955418</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.003454306698172267</v>
+        <v>-0.01168885457955418</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -983,57 +979,53 @@
       <c r="AE7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Stream-biodiesel</t>
-        </is>
-      </c>
+      <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Price [USD/gal]</t>
+          <t>Annual crushing capacity [ton/yr]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.02974261299770452</v>
+        <v>0.01922194300887772</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.01683367161734686</v>
+        <v>0.0006311694771535438</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>-0.008615789816631591</v>
+        <v>-0.01494428594177144</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01247093694683748</v>
+        <v>-0.0106725400749016</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0006088764723550588</v>
+        <v>0.01053412890136515</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.01257586034303441</v>
+        <v>-0.01082521176100847</v>
       </c>
       <c r="J8" t="n">
-        <v>0.01640422631759013</v>
+        <v>-0.004561164291027297</v>
       </c>
       <c r="K8" t="n">
-        <v>0.002454651650186066</v>
+        <v>0.0113119400364776</v>
       </c>
       <c r="L8" t="n">
-        <v>0.002454651650186066</v>
+        <v>0.0113119400364776</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>0.002454651650186066</v>
+        <v>0.0113119400364776</v>
       </c>
       <c r="P8" t="n">
-        <v>0.008508289684331585</v>
+        <v>0.01584142162565686</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.003183072319322892</v>
+        <v>0.0116660475706419</v>
       </c>
       <c r="R8" t="n">
-        <v>0.003183072319322892</v>
+        <v>0.0116660475706419</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1052,55 +1044,55 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Stream-natural gas</t>
+          <t>Stream-ethanol</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Price [USD/cf]</t>
+          <t>Price [USD/gal]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.004723728956949158</v>
+        <v>0.9571231419649255</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01662563970502559</v>
+        <v>0.00021203343165476</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.01360631132825245</v>
+        <v>0.002603669864146794</v>
       </c>
       <c r="G9" t="n">
-        <v>0.02038118126324725</v>
+        <v>-0.01539513066380522</v>
       </c>
       <c r="H9" t="n">
-        <v>0.03636032987041319</v>
+        <v>-0.03314305543772221</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0204795650431826</v>
+        <v>-0.01520164428806577</v>
       </c>
       <c r="J9" t="n">
-        <v>0.01202206089107454</v>
+        <v>0.02058910629100252</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0003169392126775685</v>
+        <v>-0.003312657444506297</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0003169392126775685</v>
+        <v>-0.003312657444506297</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.0003169392126775685</v>
+        <v>-0.003312657444506297</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.008699296955971879</v>
+        <v>0.002126737909069516</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.0004104919844196793</v>
+        <v>-0.002817465808698632</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.0004104919844196793</v>
+        <v>-0.002817465808698632</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1119,55 +1111,55 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>biorefinery</t>
+          <t>Stream-biodiesel</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Electricity price [USD/kWhr]</t>
+          <t>Price [USD/gal]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.03157316747092669</v>
+        <v>0.004902343972093758</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.00196987025479481</v>
+        <v>-0.02486662397644808</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>0.003992730399709215</v>
+        <v>-0.02033086439723458</v>
       </c>
       <c r="G10" t="n">
-        <v>0.001903182220127289</v>
+        <v>-0.01840205238408209</v>
       </c>
       <c r="H10" t="n">
-        <v>0.002665656970626279</v>
+        <v>-0.01228166372326655</v>
       </c>
       <c r="I10" t="n">
-        <v>0.001679094691163787</v>
+        <v>-0.01867151729086069</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01123021893332484</v>
+        <v>-0.00762078344449315</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.02212130776485231</v>
+        <v>0.01487417742696709</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.02212130776485231</v>
+        <v>0.01487417742696709</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>-0.02212130776485231</v>
+        <v>0.01487417742696709</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.01895892450235698</v>
+        <v>0.0210917851956714</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0221904875756195</v>
+        <v>0.01522642217705689</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.0221904875756195</v>
+        <v>0.01522642217705689</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -1184,53 +1176,57 @@
       <c r="AE10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n"/>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Stream-natural gas</t>
+        </is>
+      </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Operating days [day/yr]</t>
+          <t>Price [USD/cf]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1242445196897808</v>
+        <v>0.01165381083415243</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2654456043458241</v>
+        <v>-0.02099486956838006</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>-0.01391207978848319</v>
+        <v>0.008090149955605998</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.0138734149229366</v>
+        <v>0.00415569626222785</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.006436084961443397</v>
+        <v>0.005878794091151764</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.01410681618027265</v>
+        <v>0.004433049297321971</v>
       </c>
       <c r="J11" t="n">
-        <v>0.007926619912369462</v>
+        <v>0.02220468838974061</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.01545699325827973</v>
+        <v>0.004287501867500074</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.01545699325827973</v>
+        <v>0.004287501867500074</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.01545699325827973</v>
+        <v>0.004287501867500074</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.003747767189910687</v>
+        <v>0.001825908745036349</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.01462668596106744</v>
+        <v>0.004121994500879779</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.01462668596106744</v>
+        <v>0.004121994500879779</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -1247,53 +1243,57 @@
       <c r="AE11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n"/>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>biorefinery</t>
+        </is>
+      </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>IRR [%]</t>
+          <t>Electricity price [USD/kWhr]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.2179963395678536</v>
+        <v>0.01872312372492495</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0006189252727570108</v>
+        <v>-0.005248624587531768</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>0.00413220602128824</v>
+        <v>0.01800996667239866</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.002375961695038468</v>
+        <v>0.008252312682092507</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.007085799931431996</v>
+        <v>-0.006087236307489452</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.002227657913106316</v>
+        <v>0.008546522741860909</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.001122624158434291</v>
+        <v>0.003029794114640637</v>
       </c>
       <c r="K12" t="n">
-        <v>0.03039114073564562</v>
+        <v>-0.01481429137657165</v>
       </c>
       <c r="L12" t="n">
-        <v>0.03039114073564562</v>
+        <v>-0.01481429137657165</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>0.03039114073564562</v>
+        <v>-0.01481429137657165</v>
       </c>
       <c r="P12" t="n">
-        <v>0.02517019041480761</v>
+        <v>-0.01640038184001527</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.03014378290175131</v>
+        <v>-0.01489783557191342</v>
       </c>
       <c r="R12" t="n">
-        <v>0.03014378290175131</v>
+        <v>-0.01489783557191342</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1310,57 +1310,53 @@
       <c r="AE12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Stream-crude glycerol</t>
-        </is>
-      </c>
+      <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Price [USD/kg]</t>
+          <t>IRR [%]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.006811925552477022</v>
+        <v>-0.2329477237499089</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.01166114235444569</v>
+        <v>0.004479637166228811</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>-0.01411289182851567</v>
+        <v>0.002154771926190877</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.013285049907402</v>
+        <v>0.00155611100624444</v>
       </c>
       <c r="H13" t="n">
-        <v>8.225472329018892e-05</v>
+        <v>0.009981606255264249</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.01321073860842954</v>
+        <v>0.001863486986539479</v>
       </c>
       <c r="J13" t="n">
-        <v>0.003356479532938857</v>
+        <v>-0.004673367602835419</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.004595756535830261</v>
+        <v>0.0005678107427124296</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.004595756535830261</v>
+        <v>0.0005678107427124296</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>-0.004595756535830261</v>
+        <v>0.0005678107427124296</v>
       </c>
       <c r="P13" t="n">
-        <v>0.00503730701749228</v>
+        <v>0.002182446039297841</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.003870913690836547</v>
+        <v>0.0006442350977694038</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.003870913690836547</v>
+        <v>0.0006442350977694038</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -1379,7 +1375,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Stream-pure glycerine</t>
+          <t>Stream-crude glycerol</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -1388,46 +1384,46 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.009527193309087731</v>
+        <v>-0.004754398270175931</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0008059194562367781</v>
+        <v>0.00791319683721948</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>-0.0008467710098708403</v>
+        <v>-0.004364526990581079</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.002881314451252577</v>
+        <v>-0.001241739025669561</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.003532678413307136</v>
+        <v>0.0003660260306410412</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.002979622295184892</v>
+        <v>-0.001199003951960158</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.0003430405629370784</v>
+        <v>0.007864280209741109</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0006056649842265993</v>
+        <v>-0.002773999982959999</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0006056649842265993</v>
+        <v>-0.002773999982959999</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>0.0006056649842265993</v>
+        <v>-0.002773999982959999</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.001634687681387507</v>
+        <v>-0.003144895997795839</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.000601841976073679</v>
+        <v>-0.002986564055462561</v>
       </c>
       <c r="R14" t="n">
-        <v>0.000601841976073679</v>
+        <v>-0.002986564055462561</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -1446,55 +1442,55 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Saccharification</t>
+          <t>Stream-pure glycerine</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Reaction time [hr]</t>
+          <t>Price [USD/kg]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.01317959294318371</v>
+        <v>0.005524681372987254</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.009508359644334384</v>
+        <v>0.00449999467623092</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>-0.00522521300900852</v>
+        <v>0.003524829068993162</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.009501153884046156</v>
+        <v>0.0156300127212005</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.008414760432590415</v>
+        <v>0.01687036022681441</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.00977526730301069</v>
+        <v>0.01548212970728519</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.02147624616984654</v>
+        <v>-0.001038444705665905</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.01732170635686825</v>
+        <v>0.006277320539092821</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.01732170635686825</v>
+        <v>0.006277320539092821</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.01732170635686825</v>
+        <v>0.006277320539092821</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.01006092078643683</v>
+        <v>-0.0008126452165058085</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.0166205474808219</v>
+        <v>0.005730246565209862</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.0166205474808219</v>
+        <v>0.005730246565209862</v>
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
@@ -1513,55 +1509,55 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>cellulase</t>
+          <t>Saccharification</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Price [USD/kg]</t>
+          <t>Reaction time [hr]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.01097265125490605</v>
+        <v>-0.007699014067960562</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001442512665700506</v>
+        <v>0.02301387738798731</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>-0.006280992059239681</v>
+        <v>-0.03346093842643753</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.002741296429651857</v>
+        <v>-0.02664528826581153</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0168738149789526</v>
+        <v>0.00538203851928154</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.002995292087811683</v>
+        <v>-0.02698452895138116</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.01321525713363007</v>
+        <v>-0.01819599467229088</v>
       </c>
       <c r="K16" t="n">
-        <v>0.04384539679381586</v>
+        <v>0.01396515214260608</v>
       </c>
       <c r="L16" t="n">
-        <v>0.04384539679381586</v>
+        <v>0.01396515214260608</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.04384539679381586</v>
+        <v>0.01396515214260608</v>
       </c>
       <c r="P16" t="n">
-        <v>0.03482737060909482</v>
+        <v>0.02087339737893589</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.04370292059611681</v>
+        <v>0.01478241131129645</v>
       </c>
       <c r="R16" t="n">
-        <v>0.04370292059611681</v>
+        <v>0.01478241131129645</v>
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -1578,53 +1574,57 @@
       <c r="AE16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n"/>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>cellulase</t>
+        </is>
+      </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Cellulase loading [wt. % cellulose]</t>
+          <t>Price [USD/kg]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.01446784598671384</v>
+        <v>-0.01678230316729212</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02845959675438387</v>
+        <v>0.01708290692746679</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>0.0301355776854231</v>
+        <v>-0.01623349216933968</v>
       </c>
       <c r="G17" t="n">
-        <v>0.02941467775258711</v>
+        <v>-0.01681085356843414</v>
       </c>
       <c r="H17" t="n">
-        <v>0.01838437321537493</v>
+        <v>-0.00250186925207477</v>
       </c>
       <c r="I17" t="n">
-        <v>0.02929204792368191</v>
+        <v>-0.01696859799074392</v>
       </c>
       <c r="J17" t="n">
-        <v>0.003662528185923501</v>
+        <v>-0.002024604664855332</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.008161895654475825</v>
+        <v>-0.002708749548349982</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.008161895654475825</v>
+        <v>-0.002708749548349982</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.008161895654475825</v>
+        <v>-0.002708749548349982</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.02125580667423226</v>
+        <v>0.001891151787646071</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.009151853646074144</v>
+        <v>-0.002441263297650531</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.009151853646074144</v>
+        <v>-0.002441263297650531</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -1641,57 +1641,53 @@
       <c r="AE17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Pretreatment reactor system</t>
-        </is>
-      </c>
+      <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Base cost [million USD]</t>
+          <t>Cellulase loading [wt. % cellulose]</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.01703739399349576</v>
+        <v>-0.01264724450588978</v>
       </c>
       <c r="D18" t="n">
-        <v>0.004848441889937675</v>
+        <v>0.01548368231051268</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>0.005313079220523168</v>
+        <v>-0.006334407997376319</v>
       </c>
       <c r="G18" t="n">
-        <v>0.003777007639080305</v>
+        <v>-0.01098770367150815</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.002605363304214532</v>
+        <v>-0.0001976472079058883</v>
       </c>
       <c r="I18" t="n">
-        <v>0.004248730537949222</v>
+        <v>-0.01061925008877</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0009233040939198646</v>
+        <v>0.005720417552379425</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.01725818593832744</v>
+        <v>-0.01783157620126305</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.01725818593832744</v>
+        <v>-0.01783157620126305</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.01725818593832744</v>
+        <v>-0.01783157620126305</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.01474762023790481</v>
+        <v>-0.01409787886791515</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.01733585205343408</v>
+        <v>-0.01761623206464928</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.01733585205343408</v>
+        <v>-0.01761623206464928</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -1710,55 +1706,55 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Pretreatment and saccharification</t>
+          <t>Pretreatment reactor system</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Cane glucose yield [%]</t>
+          <t>Base cost [million USD]</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.003822812408912496</v>
+        <v>0.01665299279411971</v>
       </c>
       <c r="D19" t="n">
-        <v>0.003681679443267178</v>
+        <v>0.0001687453247039228</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0.003207784448311378</v>
+        <v>0.01977460562298422</v>
       </c>
       <c r="G19" t="n">
-        <v>0.002336427645457106</v>
+        <v>0.01205151485006059</v>
       </c>
       <c r="H19" t="n">
-        <v>0.003331626373265055</v>
+        <v>-0.01015854079034163</v>
       </c>
       <c r="I19" t="n">
-        <v>0.002073678226947128</v>
+        <v>0.01206131827445273</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.004760601667693599</v>
+        <v>-0.01700380040713933</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.001082759275310371</v>
+        <v>0.005863908138556325</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.001082759275310371</v>
+        <v>0.005863908138556325</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>-0.001082759275310371</v>
+        <v>0.005863908138556325</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.003730550069222003</v>
+        <v>0.000572515126900605</v>
       </c>
       <c r="Q19" t="n">
-        <v>-0.001282645203305808</v>
+        <v>0.005473756154950245</v>
       </c>
       <c r="R19" t="n">
-        <v>-0.001282645203305808</v>
+        <v>0.005473756154950245</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -1775,53 +1771,57 @@
       <c r="AE19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n"/>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Pretreatment and saccharification</t>
+        </is>
+      </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Sorghum glucose yield [%]</t>
+          <t>Cane glucose yield [%]</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.01398436644737466</v>
+        <v>-0.01489467697978708</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0001811943432477737</v>
+        <v>-0.002832194614428476</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>-0.0007089527323581092</v>
+        <v>0.002632597065303882</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0009421087096843482</v>
+        <v>-0.000185742151429686</v>
       </c>
       <c r="H20" t="n">
-        <v>0.004433852241354089</v>
+        <v>0.005649771777990871</v>
       </c>
       <c r="I20" t="n">
-        <v>0.001038338057533522</v>
+        <v>-0.0002332622493304899</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.007752231585881808</v>
+        <v>-0.01495850115745483</v>
       </c>
       <c r="K20" t="n">
-        <v>0.01747503775500151</v>
+        <v>-0.01717931444717257</v>
       </c>
       <c r="L20" t="n">
-        <v>0.01747503775500151</v>
+        <v>-0.01717931444717257</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0.01747503775500151</v>
+        <v>-0.01717931444717257</v>
       </c>
       <c r="P20" t="n">
-        <v>0.01542845543313821</v>
+        <v>-0.01434089769363591</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.0173518676380747</v>
+        <v>-0.0169900125196005</v>
       </c>
       <c r="R20" t="n">
-        <v>0.0173518676380747</v>
+        <v>-0.0169900125196005</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -1841,50 +1841,50 @@
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Cane xylose yield [%]</t>
+          <t>Sorghum glucose yield [%]</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.02263738103349524</v>
+        <v>-0.02261964080878563</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.003839358873574354</v>
+        <v>0.01415952259868855</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>0.0006456910338276413</v>
+        <v>0.01920371654414866</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.0001675289347011574</v>
+        <v>0.02397825523113021</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01474585882983435</v>
+        <v>0.01222807719312309</v>
       </c>
       <c r="I21" t="n">
-        <v>7.048157081926283e-05</v>
+        <v>0.0236253152490126</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.009839898135186756</v>
+        <v>0.01514089759858972</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.01968065925122637</v>
+        <v>0.01043405436936217</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.01968065925122637</v>
+        <v>0.01043405436936217</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-0.01968065925122637</v>
+        <v>0.01043405436936217</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.01258611535144461</v>
+        <v>0.0002556024102240963</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.01926340166653606</v>
+        <v>0.009453543642141746</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.01926340166653606</v>
+        <v>0.009453543642141746</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -1904,50 +1904,50 @@
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Sorghum xylose yield [%]</t>
+          <t>Cane xylose yield [%]</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.03321905537676221</v>
+        <v>-0.02877245078289803</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01242534222501369</v>
+        <v>-0.002906638524898825</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>0.01748945829957833</v>
+        <v>0.001413393464535739</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01764272240170889</v>
+        <v>0.0002261311770452471</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.003962003870480154</v>
+        <v>0.001449778233991129</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01792686148507446</v>
+        <v>0.0003372443654897746</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.006197866728513011</v>
+        <v>-0.0008166847338225691</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.002179014135160565</v>
+        <v>0.001541406205656248</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.002179014135160565</v>
+        <v>0.001541406205656248</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>-0.002179014135160565</v>
+        <v>0.001541406205656248</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.01276904115076164</v>
+        <v>0.001247396209895848</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.002995118711804748</v>
+        <v>0.001609616224384649</v>
       </c>
       <c r="R22" t="n">
-        <v>-0.002995118711804748</v>
+        <v>0.001609616224384649</v>
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
@@ -1964,57 +1964,53 @@
       <c r="AE22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Cofermenation</t>
-        </is>
-      </c>
+      <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Glucose to ethanol yield [%]</t>
+          <t>Sorghum xylose yield [%]</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.001233392401335696</v>
+        <v>0.002329148733165949</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.004003539328141572</v>
+        <v>-0.01490907664545626</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>0.0007999911679996466</v>
+        <v>0.009439969913598795</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.0004007437600297504</v>
+        <v>0.007003516696140666</v>
       </c>
       <c r="H23" t="n">
-        <v>-5.290915411636616e-05</v>
+        <v>0.00563771926550877</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.0004293735531749421</v>
+        <v>0.007234606369384253</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.01044024708163456</v>
+        <v>-0.01618987728833575</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.003154664286186571</v>
+        <v>0.006690518379620734</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.003154664286186571</v>
+        <v>0.006690518379620734</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>-0.003154664286186571</v>
+        <v>0.006690518379620734</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.002282013211280528</v>
+        <v>0.002534787461391498</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.003284146115365844</v>
+        <v>0.006381795711271828</v>
       </c>
       <c r="R23" t="n">
-        <v>-0.003284146115365844</v>
+        <v>0.006381795711271828</v>
       </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
@@ -2031,53 +2027,57 @@
       <c r="AE23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n"/>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Cofermenation</t>
+        </is>
+      </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Xylose to ethanol yield [%]</t>
+          <t>Glucose to ethanol yield [%]</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.004067717538708701</v>
+        <v>-0.02787982124319284</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0008729135389165415</v>
+        <v>-0.007799645578754935</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>-0.003933066397322655</v>
+        <v>-0.003078614523144581</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.006602179944087196</v>
+        <v>-0.008187559815502392</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.001274664434986577</v>
+        <v>-0.0008859348834373952</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.00648658374746335</v>
+        <v>-0.008019336128773443</v>
       </c>
       <c r="J24" t="n">
-        <v>0.01175468096210625</v>
+        <v>0.03318221925975666</v>
       </c>
       <c r="K24" t="n">
-        <v>0.01036616057464642</v>
+        <v>-0.003045804793832191</v>
       </c>
       <c r="L24" t="n">
-        <v>0.01036616057464642</v>
+        <v>-0.003045804793832191</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>0.01036616057464642</v>
+        <v>-0.003045804793832191</v>
       </c>
       <c r="P24" t="n">
-        <v>0.01147591418703657</v>
+        <v>0.001500133212005328</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.01060743364029734</v>
+        <v>-0.002701030956041238</v>
       </c>
       <c r="R24" t="n">
-        <v>0.01060743364029734</v>
+        <v>-0.002701030956041238</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -2094,57 +2094,53 @@
       <c r="AE24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>Cofermentation</t>
-        </is>
-      </c>
+      <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Titer [g/L]</t>
+          <t>Xylose to ethanol yield [%]</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.02290447867617914</v>
+        <v>-0.007994767807790711</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01570372123614885</v>
+        <v>0.01090968354319755</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>0.009256921138276844</v>
+        <v>0.02372836050113442</v>
       </c>
       <c r="G25" t="n">
-        <v>0.01560693969627758</v>
+        <v>0.01358408415936336</v>
       </c>
       <c r="H25" t="n">
-        <v>0.02600414744016589</v>
+        <v>-0.005670220834808832</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0155115449724618</v>
+        <v>0.0134296574971863</v>
       </c>
       <c r="J25" t="n">
-        <v>0.01755490345957871</v>
+        <v>0.01659786417678876</v>
       </c>
       <c r="K25" t="n">
-        <v>0.01525192659407706</v>
+        <v>-0.004055741634229664</v>
       </c>
       <c r="L25" t="n">
-        <v>0.01525192659407706</v>
+        <v>-0.004055741634229664</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.01525192659407706</v>
+        <v>-0.004055741634229664</v>
       </c>
       <c r="P25" t="n">
-        <v>0.003853295866131834</v>
+        <v>-0.009167602638704104</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.01449715901188636</v>
+        <v>-0.004489208339568333</v>
       </c>
       <c r="R25" t="n">
-        <v>0.01449715901188636</v>
+        <v>-0.004489208339568333</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -2161,53 +2157,57 @@
       <c r="AE25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n"/>
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Cofermentation</t>
+        </is>
+      </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>Productivity [g/L]</t>
+          <t>Titer [g/L]</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.004799755007990199</v>
+        <v>0.01797204983888199</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.009466703898668154</v>
+        <v>-0.01028629301877894</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>-0.01761980825679233</v>
+        <v>-0.0006184344247373768</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.01974938910997556</v>
+        <v>0.0007187237087489482</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.01398404225536169</v>
+        <v>0.00223625048945002</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.01985684277827371</v>
+        <v>0.0007012002520480101</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.01849254295229712</v>
+        <v>0.0002161180328896184</v>
       </c>
       <c r="K26" t="n">
-        <v>0.01748624709944988</v>
+        <v>0.02148133919525356</v>
       </c>
       <c r="L26" t="n">
-        <v>0.01748624709944988</v>
+        <v>0.02148133919525356</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>0.01748624709944988</v>
+        <v>0.02148133919525356</v>
       </c>
       <c r="P26" t="n">
-        <v>0.02215192523807701</v>
+        <v>0.01786481322659253</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.01805836843433474</v>
+        <v>0.02118003156720126</v>
       </c>
       <c r="R26" t="n">
-        <v>0.01805836843433474</v>
+        <v>0.02118003156720126</v>
       </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
@@ -2224,57 +2224,53 @@
       <c r="AE26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>oilcane</t>
-        </is>
-      </c>
+      <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Cane PL content [% oil]</t>
+          <t>Productivity [g/L]</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-0.0006682868427314736</v>
+        <v>0.001930785965231439</v>
       </c>
       <c r="D27" t="n">
-        <v>0.007169562910782515</v>
+        <v>0.01216074473849168</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>0.004006884352275373</v>
+        <v>0.002763064334522573</v>
       </c>
       <c r="G27" t="n">
-        <v>0.008770026782801071</v>
+        <v>0.004739190525567621</v>
       </c>
       <c r="H27" t="n">
-        <v>0.005885141899405675</v>
+        <v>0.01283063033722521</v>
       </c>
       <c r="I27" t="n">
-        <v>0.008578593367143733</v>
+        <v>0.004421806736872268</v>
       </c>
       <c r="J27" t="n">
-        <v>0.02344996908074596</v>
+        <v>0.02381018320796716</v>
       </c>
       <c r="K27" t="n">
-        <v>0.02345264484210579</v>
+        <v>-0.01888799422751977</v>
       </c>
       <c r="L27" t="n">
-        <v>0.02345264484210579</v>
+        <v>-0.01888799422751977</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>0.02345264484210579</v>
+        <v>-0.01888799422751977</v>
       </c>
       <c r="P27" t="n">
-        <v>0.01249254184370167</v>
+        <v>-0.01728240664329626</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.02270137473205499</v>
+        <v>-0.01901082344843294</v>
       </c>
       <c r="R27" t="n">
-        <v>0.02270137473205499</v>
+        <v>-0.01901082344843294</v>
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
@@ -2293,55 +2289,55 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>oilsorghum</t>
+          <t>oilcane</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Sorghum PL content [% oil]</t>
+          <t>Cane PL content [% oil]</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.007034497145379884</v>
+        <v>0.01111227558049102</v>
       </c>
       <c r="D28" t="n">
-        <v>0.02042471112098844</v>
+        <v>-0.008119854286134529</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>0.02220508168820326</v>
+        <v>0.04617682197507287</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0272086051523442</v>
+        <v>0.02749165837966633</v>
       </c>
       <c r="H28" t="n">
-        <v>0.03376257763850311</v>
+        <v>-0.01881657080066283</v>
       </c>
       <c r="I28" t="n">
-        <v>0.02712211894088476</v>
+        <v>0.02783297468131898</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.01198376458430668</v>
+        <v>0.02060080915567773</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.01298135178325407</v>
+        <v>0.0009487787899511515</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.01298135178325407</v>
+        <v>0.0009487787899511515</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.01298135178325407</v>
+        <v>0.0009487787899511515</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.02564834291393372</v>
+        <v>-0.009873970858958832</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.01423722162548887</v>
+        <v>1.044470441778818e-05</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.01423722162548887</v>
+        <v>1.044470441778818e-05</v>
       </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
@@ -2360,55 +2356,55 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>oilcane</t>
+          <t>oilsorghum</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>Cane FFA content [% oil]</t>
+          <t>Sorghum PL content [% oil]</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.00666799101871964</v>
+        <v>0.007579546959181878</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01424484632979385</v>
+        <v>0.007642771764285674</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>0.009111874060474961</v>
+        <v>-0.01388457300338292</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01761975200079008</v>
+        <v>-0.0202227051289082</v>
       </c>
       <c r="H29" t="n">
-        <v>0.02252060096482403</v>
+        <v>-0.02165257661010306</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01756381481455259</v>
+        <v>-0.02010371331614853</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.01876858702088136</v>
+        <v>0.003508619011882237</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.02754453230178129</v>
+        <v>0.01859429671177187</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.02754453230178129</v>
+        <v>0.01859429671177187</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>-0.02754453230178129</v>
+        <v>0.01859429671177187</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.0286789376591575</v>
+        <v>0.0247486599659464</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.02796560943862438</v>
+        <v>0.0191453426858137</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.02796560943862438</v>
+        <v>0.0191453426858137</v>
       </c>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
@@ -2427,55 +2423,55 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>oilsorghum</t>
+          <t>oilcane</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>Sorghum FFA content [% oil]</t>
+          <t>Cane FFA content [% oil]</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.01429216108368644</v>
+        <v>-0.01883097348923893</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.03344480927379236</v>
+        <v>-0.008657616688069586</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>-0.04241267238450689</v>
+        <v>0.002828745713149828</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.03711789354871574</v>
+        <v>0.0002632737705309508</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.01560299294411971</v>
+        <v>0.001560571838422873</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.03700483079219322</v>
+        <v>0.0004006892320275692</v>
       </c>
       <c r="J30" t="n">
-        <v>0.003410410448852237</v>
+        <v>0.01940869623878802</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.02272962340518494</v>
+        <v>0.02334521805380872</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.02272962340518494</v>
+        <v>0.02334521805380872</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>-0.02272962340518494</v>
+        <v>0.02334521805380872</v>
       </c>
       <c r="P30" t="n">
-        <v>0.004374119982964799</v>
+        <v>0.02195307630212305</v>
       </c>
       <c r="Q30" t="n">
-        <v>-0.02037962279918491</v>
+        <v>0.0233366526454661</v>
       </c>
       <c r="R30" t="n">
-        <v>-0.02037962279918491</v>
+        <v>0.0233366526454661</v>
       </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
@@ -2494,55 +2490,55 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>oilcane</t>
+          <t>oilsorghum</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Cane oil content [dry wt. %]</t>
+          <t>Sorghum FFA content [% oil]</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.007656255570250223</v>
+        <v>-0.0007381495975259839</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.02334369789374791</v>
+        <v>-0.01901854283963636</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>-0.02528750789150031</v>
+        <v>0.0261843126633725</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.02467730729109229</v>
+        <v>0.02245357779414311</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.01934270707770828</v>
+        <v>0.005015813960632557</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.02427284861891394</v>
+        <v>0.02242468208098728</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.01834454025580248</v>
+        <v>-0.009617254720594104</v>
       </c>
       <c r="K31" t="n">
-        <v>0.003798191383927655</v>
+        <v>-0.01050603046824122</v>
       </c>
       <c r="L31" t="n">
-        <v>0.003798191383927655</v>
+        <v>-0.01050603046824122</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>0.003798191383927655</v>
+        <v>-0.01050603046824122</v>
       </c>
       <c r="P31" t="n">
-        <v>0.01638966353558654</v>
+        <v>-0.01558689153547566</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.004889467587578702</v>
+        <v>-0.01109899618795985</v>
       </c>
       <c r="R31" t="n">
-        <v>0.004889467587578702</v>
+        <v>-0.01109899618795985</v>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
@@ -2561,55 +2557,55 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>oilsorghum</t>
+          <t>oilcane</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Relative sorghum oil content [dry wt. %]</t>
+          <t>Cane oil content [dry wt. %]</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.01773501430940057</v>
+        <v>-0.001712910212516408</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.002615932040637281</v>
+        <v>0.0228111216408942</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>-0.01894599435783977</v>
+        <v>0.009791948071677922</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.007154934334197372</v>
+        <v>0.005788616679544666</v>
       </c>
       <c r="H32" t="n">
-        <v>0.007952763486110539</v>
+        <v>-0.003533406669336266</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.006981006903240275</v>
+        <v>0.005661214210448568</v>
       </c>
       <c r="J32" t="n">
-        <v>0.006529977577555319</v>
+        <v>-0.002278980343493526</v>
       </c>
       <c r="K32" t="n">
-        <v>0.002157825782313031</v>
+        <v>0.0008641006425640256</v>
       </c>
       <c r="L32" t="n">
-        <v>0.002157825782313031</v>
+        <v>0.0008641006425640256</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>0.002157825782313031</v>
+        <v>0.0008641006425640256</v>
       </c>
       <c r="P32" t="n">
-        <v>0.005821812712872508</v>
+        <v>0.0001484888699395548</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.002575570183022807</v>
+        <v>0.0007031910041276401</v>
       </c>
       <c r="R32" t="n">
-        <v>0.002575570183022807</v>
+        <v>0.0007031910041276401</v>
       </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
@@ -2628,55 +2624,55 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>biorefinery</t>
+          <t>oilsorghum</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>TAG to FFA conversion [% oil]</t>
+          <t>Relative sorghum oil content [dry wt. %]</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.01830924121236965</v>
+        <v>-0.00457286677491467</v>
       </c>
       <c r="D33" t="n">
-        <v>0.01630701386828055</v>
+        <v>0.006684842419015412</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>0.01681766169670646</v>
+        <v>0.01372049306081972</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0191229551009182</v>
+        <v>0.01204169241766769</v>
       </c>
       <c r="H33" t="n">
-        <v>0.01937800608712024</v>
+        <v>-0.01256664789466591</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01915612147024486</v>
+        <v>0.0117279801491192</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.01056404361743416</v>
+        <v>0.006755314580630753</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.001846373737854949</v>
+        <v>-0.00910259825210393</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.001846373737854949</v>
+        <v>-0.00910259825210393</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>-0.001846373737854949</v>
+        <v>-0.00910259825210393</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.01251029282041171</v>
+        <v>-0.01329006235560249</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.002899017043960681</v>
+        <v>-0.00949178303567132</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.002899017043960681</v>
+        <v>-0.00949178303567132</v>
       </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
@@ -2695,55 +2691,55 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Stream-sugarcane</t>
+          <t>biorefinery</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>GWP [kg*CO2-eq/kg]</t>
+          <t>TAG to FFA conversion [% oil]</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.008220676744827068</v>
+        <v>0.005734338565373543</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0162324076572963</v>
+        <v>-0.008638064375206082</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>-0.0140646900345876</v>
+        <v>0.01869915645996626</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.01607734739509389</v>
+        <v>0.01887177569887102</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.01846859478674379</v>
+        <v>0.0134311075772443</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.01603446400137856</v>
+        <v>0.0189883275755331</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.02654899063897755</v>
+        <v>-0.01980500408118323</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.006850126546005061</v>
+        <v>0.01670769935630797</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.006850126546005061</v>
+        <v>0.01670769935630797</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>-0.006850126546005061</v>
+        <v>0.01670769935630797</v>
       </c>
       <c r="P34" t="n">
-        <v>0.005181360783254431</v>
+        <v>0.007741128981645158</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.005828563529142541</v>
+        <v>0.01595593023823721</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.005828563529142541</v>
+        <v>0.01595593023823721</v>
       </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
@@ -2762,7 +2758,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Stream-methanol</t>
+          <t>Stream-sugarcane</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
@@ -2771,46 +2767,46 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01411078904443156</v>
+        <v>-0.0183842175993687</v>
       </c>
       <c r="D35" t="n">
-        <v>0.01363320092932804</v>
+        <v>-0.002234491700175619</v>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
-        <v>0.002341465533658621</v>
+        <v>-0.003435594089423763</v>
       </c>
       <c r="G35" t="n">
-        <v>0.01402699409707976</v>
+        <v>-0.006315878748635149</v>
       </c>
       <c r="H35" t="n">
-        <v>0.03360083232003329</v>
+        <v>-0.007159085854363434</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01410023154000926</v>
+        <v>-0.006043941745757669</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.001159715955927264</v>
+        <v>0.02180877585955998</v>
       </c>
       <c r="K35" t="n">
-        <v>0.01405849726633989</v>
+        <v>-0.009616687680667505</v>
       </c>
       <c r="L35" t="n">
-        <v>0.01405849726633989</v>
+        <v>-0.009616687680667505</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>0.01405849726633989</v>
+        <v>-0.009616687680667505</v>
       </c>
       <c r="P35" t="n">
-        <v>0.005229713777188551</v>
+        <v>-0.005340855861634233</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.01330586837223473</v>
+        <v>-0.009477735643109424</v>
       </c>
       <c r="R35" t="n">
-        <v>0.01330586837223473</v>
+        <v>-0.009477735643109424</v>
       </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
@@ -2829,7 +2825,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Stream-pure glycerine</t>
+          <t>Stream-methanol</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
@@ -2838,46 +2834,46 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.00471851826874073</v>
+        <v>-0.02375515083820603</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.009484092667363705</v>
+        <v>0.002787827153285262</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>-0.01346117689044707</v>
+        <v>0.005427899833115993</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.01334177026167081</v>
+        <v>0.005957454766298189</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.01037468633498745</v>
+        <v>0.00649505401980216</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.0134217851128714</v>
+        <v>0.005911961420478456</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.00481157596042992</v>
+        <v>0.01347634903253304</v>
       </c>
       <c r="K36" t="n">
-        <v>0.01526676953867078</v>
+        <v>0.0004830135553205421</v>
       </c>
       <c r="L36" t="n">
-        <v>0.01526676953867078</v>
+        <v>0.0004830135553205421</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>0.01526676953867078</v>
+        <v>0.0004830135553205421</v>
       </c>
       <c r="P36" t="n">
-        <v>0.01817163797486552</v>
+        <v>-0.001882974891318995</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.01574926037397041</v>
+        <v>0.0002838147953525917</v>
       </c>
       <c r="R36" t="n">
-        <v>0.01574926037397041</v>
+        <v>0.0002838147953525917</v>
       </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
@@ -2896,7 +2892,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Stream-cellulase</t>
+          <t>Stream-pure glycerine</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
@@ -2905,46 +2901,46 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.01478725700749028</v>
+        <v>0.004940128805605151</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0137859299274372</v>
+        <v>-0.01963981969681825</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>0.009716747140669883</v>
+        <v>0.007699148179965927</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01255949426237977</v>
+        <v>0.007960766622430664</v>
       </c>
       <c r="H37" t="n">
-        <v>0.007481248907249955</v>
+        <v>0.005826111401044455</v>
       </c>
       <c r="I37" t="n">
-        <v>0.01260839080833563</v>
+        <v>0.007886869659474785</v>
       </c>
       <c r="J37" t="n">
-        <v>0.009993051138921804</v>
+        <v>0.001272588821872038</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.006510530372421215</v>
+        <v>-0.02515643428625737</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.006510530372421215</v>
+        <v>-0.02515643428625737</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.006510530372421215</v>
+        <v>-0.02515643428625737</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.01091054942842198</v>
+        <v>-0.0227632601745304</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.00692412978096519</v>
+        <v>-0.02497036487081459</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.00692412978096519</v>
+        <v>-0.02497036487081459</v>
       </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
@@ -2963,7 +2959,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Stream-natural gas</t>
+          <t>Stream-cellulase</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
@@ -2972,46 +2968,46 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>-0.01235006180600247</v>
+        <v>0.005924393420975737</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.02315309036612361</v>
+        <v>-0.01294290313189781</v>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>-0.02510631623625264</v>
+        <v>-0.02649032793961311</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.01917576844703074</v>
+        <v>-0.02424839837793593</v>
       </c>
       <c r="H38" t="n">
-        <v>-0.01063190730527629</v>
+        <v>-0.01936523203860928</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.01924675382587015</v>
+        <v>-0.02424877431395097</v>
       </c>
       <c r="J38" t="n">
-        <v>0.001928620420792458</v>
+        <v>-0.0005540084591062399</v>
       </c>
       <c r="K38" t="n">
-        <v>0.9850401322016051</v>
+        <v>0.02067460268298411</v>
       </c>
       <c r="L38" t="n">
-        <v>0.9850401322016051</v>
+        <v>0.02067460268298411</v>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
-        <v>0.9850401322016051</v>
+        <v>0.02067460268298411</v>
       </c>
       <c r="P38" t="n">
-        <v>0.735280275203211</v>
+        <v>0.02709318405972736</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.9752928500517138</v>
+        <v>0.02124468372978735</v>
       </c>
       <c r="R38" t="n">
-        <v>0.9752928500517138</v>
+        <v>0.02124468372978735</v>
       </c>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
@@ -3027,18 +3023,85 @@
       <c r="AD38" t="inlineStr"/>
       <c r="AE38" t="inlineStr"/>
     </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Stream-natural gas</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>GWP [kg*CO2-eq/kg]</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>-0.0009401002936040117</v>
+      </c>
+      <c r="D39" t="n">
+        <v>-0.009835984737165975</v>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>-0.01308560740342429</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-0.01862665936906637</v>
+      </c>
+      <c r="H39" t="n">
+        <v>-0.008061708898468356</v>
+      </c>
+      <c r="I39" t="n">
+        <v>-0.01863374551334982</v>
+      </c>
+      <c r="J39" t="n">
+        <v>-0.002249490734189553</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.9947189451327576</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.9947189451327576</v>
+      </c>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="n">
+        <v>0.9947189451327576</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0.8845242662929707</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0.9911770641590825</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0.9911770641590825</v>
+      </c>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr"/>
+      <c r="Z39" t="inlineStr"/>
+      <c r="AA39" t="inlineStr"/>
+      <c r="AB39" t="inlineStr"/>
+      <c r="AC39" t="inlineStr"/>
+      <c r="AD39" t="inlineStr"/>
+      <c r="AE39" t="inlineStr"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="Q1:T1"/>
     <mergeCell ref="U1:Z1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add final montecarlo analyses
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -734,46 +734,46 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.003646828561873142</v>
+        <v>-0.001981087567243502</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007043535938674062</v>
+        <v>0.003529454733178189</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.001906517068260682</v>
+        <v>0.002691628715665148</v>
       </c>
       <c r="G4" t="n">
-        <v>0.002458030370321215</v>
+        <v>-9.089693163587725e-05</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0005778029031121161</v>
+        <v>-0.007891063515642541</v>
       </c>
       <c r="I4" t="n">
-        <v>0.002653589866143594</v>
+        <v>-0.0001278572211142888</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.01336634182053731</v>
+        <v>0.03567766691724603</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.02590386074815442</v>
+        <v>-0.02581511354460454</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.02590386074815442</v>
+        <v>-0.02581511354460454</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>-0.02590386074815442</v>
+        <v>-0.02581511354460454</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.02276153678246147</v>
+        <v>-0.0166109524724381</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.02573568726942748</v>
+        <v>-0.02541449736857989</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.02573568726942748</v>
+        <v>-0.02541449736857989</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -797,46 +797,46 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01347928517917141</v>
+        <v>0.01669288626771545</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01071744197204767</v>
+        <v>0.007570266830810672</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>-0.008397379823895193</v>
+        <v>-0.00998490654339626</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.01375104035804161</v>
+        <v>-0.003539690445587617</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.004874077346963093</v>
+        <v>0.006926079445043177</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.01379932202397288</v>
+        <v>-0.003627023473080938</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.02940441396493397</v>
+        <v>-0.02018644103050018</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0008976869159074765</v>
+        <v>-0.0002487987939519517</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0008976869159074765</v>
+        <v>-0.0002487987939519517</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.0008976869159074765</v>
+        <v>-0.0002487987939519517</v>
       </c>
       <c r="P5" t="n">
-        <v>0.004954424934176997</v>
+        <v>0.001185909839436393</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.001236542737461709</v>
+        <v>-0.0003375250695010027</v>
       </c>
       <c r="R5" t="n">
-        <v>0.001236542737461709</v>
+        <v>-0.0003375250695010027</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -860,46 +860,46 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2194978631479145</v>
+        <v>0.2160015041280601</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0007961513443614221</v>
+        <v>0.0108233524329341</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>-0.8845690323427612</v>
+        <v>-0.563932652925306</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.9998814639952585</v>
+        <v>-0.6033473026938919</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.6612649876345994</v>
+        <v>-0.3537699437187977</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.9999999849279991</v>
+        <v>-0.6031647557105901</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.03719825812957746</v>
+        <v>-0.01357855879495565</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1290232931289317</v>
+        <v>0.1256377155215086</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1290232931289317</v>
+        <v>0.1256377155215086</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.1290232931289317</v>
+        <v>0.1256377155215086</v>
       </c>
       <c r="P6" t="n">
-        <v>0.5021340220053608</v>
+        <v>0.4260346111213844</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1607569812462792</v>
+        <v>0.1551090166683606</v>
       </c>
       <c r="R6" t="n">
-        <v>0.1607569812462792</v>
+        <v>0.1551090166683606</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -923,46 +923,46 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.006347835229913408</v>
+        <v>-0.00711654652466186</v>
       </c>
       <c r="D7" t="n">
-        <v>0.002410459881886084</v>
+        <v>-0.004311911308476452</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>-0.002476143651045746</v>
+        <v>-0.001606011424240457</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.00673336327733453</v>
+        <v>-0.00718743926349757</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.02068808521152341</v>
+        <v>-0.01700430807217232</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.006707185228287409</v>
+        <v>-0.007146824253872969</v>
       </c>
       <c r="J7" t="n">
-        <v>0.001445993851212611</v>
+        <v>0.01254155264794391</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.01177281291891251</v>
+        <v>-0.01132881126915245</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.01177281291891251</v>
+        <v>-0.01132881126915245</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.01177281291891251</v>
+        <v>-0.01132881126915245</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.007347082661883306</v>
+        <v>-0.003662758994510359</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.01172121061284842</v>
+        <v>-0.01104846840993874</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.01172121061284842</v>
+        <v>-0.01104846840993874</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -986,46 +986,46 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.01940328960813158</v>
+        <v>0.214314225820569</v>
       </c>
       <c r="D8" t="n">
-        <v>0.02100482078952759</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>-0.01384762826590513</v>
+        <v>0.720325628941025</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01093343074133723</v>
+        <v>0.7774172114806883</v>
       </c>
       <c r="H8" t="n">
-        <v>0.008624413400976536</v>
+        <v>0.4705695211267807</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.01082084740883389</v>
+        <v>0.7776363104654522</v>
       </c>
       <c r="J8" t="n">
-        <v>0.02574331643721395</v>
+        <v>-0.01631292263716014</v>
       </c>
       <c r="K8" t="n">
-        <v>0.01150293425211737</v>
+        <v>-0.1274815802032632</v>
       </c>
       <c r="L8" t="n">
-        <v>0.01150293425211737</v>
+        <v>-0.1274815802032632</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>0.01150293425211737</v>
+        <v>-0.1274815802032632</v>
       </c>
       <c r="P8" t="n">
-        <v>0.01615549898221996</v>
+        <v>-0.5227168998526759</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.01196655734266229</v>
+        <v>-0.1656055947842238</v>
       </c>
       <c r="R8" t="n">
-        <v>0.01196655734266229</v>
+        <v>-0.1656055947842238</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1053,46 +1053,46 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9392376437135056</v>
+        <v>0.9182517237700688</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.02330559802864298</v>
+        <v>0.01752971628518865</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.00530535650021426</v>
+        <v>0.005848386089935442</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.01524447046577882</v>
+        <v>0.007325336069013442</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.03565004091400163</v>
+        <v>0.00676550878262035</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.01519888486395539</v>
+        <v>0.007335383429415336</v>
       </c>
       <c r="J9" t="n">
-        <v>0.006801740640566988</v>
+        <v>0.0130547926729756</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.003074953850998154</v>
+        <v>-0.005186724495468979</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.003074953850998154</v>
+        <v>-0.005186724495468979</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>-0.003074953850998154</v>
+        <v>-0.005186724495468979</v>
       </c>
       <c r="P9" t="n">
-        <v>0.002918821460752858</v>
+        <v>-0.005742566341702653</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.002496543747861749</v>
+        <v>-0.005446028665841146</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.002496543747861749</v>
+        <v>-0.005446028665841146</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1120,46 +1120,46 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.006143923253756929</v>
+        <v>0.007565449742617988</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.003341772439577051</v>
+        <v>0.003197859583914383</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>-0.02074791730991669</v>
+        <v>-0.01201252838450113</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.01863157140126286</v>
+        <v>-0.01145373962614958</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.01049692313987692</v>
+        <v>-0.01739417791176711</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.01866927972277119</v>
+        <v>-0.01130386576415463</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01241300628228422</v>
+        <v>-0.004743453616201123</v>
       </c>
       <c r="K10" t="n">
-        <v>0.01488416152336646</v>
+        <v>0.01439699155187966</v>
       </c>
       <c r="L10" t="n">
-        <v>0.01488416152336646</v>
+        <v>0.01439699155187966</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>0.01488416152336646</v>
+        <v>0.01439699155187966</v>
       </c>
       <c r="P10" t="n">
-        <v>0.02089438240377529</v>
+        <v>0.01642396577695863</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.01526356515454261</v>
+        <v>0.01487034654681386</v>
       </c>
       <c r="R10" t="n">
-        <v>0.01526356515454261</v>
+        <v>0.01487034654681386</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -1187,46 +1187,46 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.01191191337247653</v>
+        <v>0.0137612451584498</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01261912627379046</v>
+        <v>0.007627171025086841</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.005073460426938416</v>
+        <v>0.008224741384989654</v>
       </c>
       <c r="G11" t="n">
-        <v>0.004262167562486701</v>
+        <v>0.009251631922065276</v>
       </c>
       <c r="H11" t="n">
-        <v>0.008449433233977328</v>
+        <v>0.01050162061206482</v>
       </c>
       <c r="I11" t="n">
-        <v>0.004430364849214594</v>
+        <v>0.009299025107961002</v>
       </c>
       <c r="J11" t="n">
-        <v>0.008914792293505511</v>
+        <v>0.01780943717607295</v>
       </c>
       <c r="K11" t="n">
-        <v>0.004279721547188861</v>
+        <v>0.00407715126708605</v>
       </c>
       <c r="L11" t="n">
-        <v>0.004279721547188861</v>
+        <v>0.00407715126708605</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>0.004279721547188861</v>
+        <v>0.00407715126708605</v>
       </c>
       <c r="P11" t="n">
-        <v>0.00157942124717685</v>
+        <v>0.002271869178874767</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.004051154658046186</v>
+        <v>0.003972715358908614</v>
       </c>
       <c r="R11" t="n">
-        <v>0.004051154658046186</v>
+        <v>0.003972715358908614</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -1254,46 +1254,46 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.01830355599614224</v>
+        <v>0.01733204488528179</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.01689287107576755</v>
+        <v>-0.004942293317691732</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>0.01459431053577242</v>
+        <v>-0.007013254264530169</v>
       </c>
       <c r="G12" t="n">
-        <v>0.008496681459867258</v>
+        <v>0.0002977445879097835</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.004093716451748657</v>
+        <v>-0.001398786295951451</v>
       </c>
       <c r="I12" t="n">
-        <v>0.008544028085761123</v>
+        <v>0.0003649513105980523</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.009351682169459799</v>
+        <v>0.01981871936651867</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0145762049350482</v>
+        <v>-0.01399853835194153</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.0145762049350482</v>
+        <v>-0.01399853835194153</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>-0.0145762049350482</v>
+        <v>-0.01399853835194153</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0156393776175751</v>
+        <v>-0.01132916186116647</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.01459630915985237</v>
+        <v>-0.01404465041778601</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.01459630915985237</v>
+        <v>-0.01404465041778601</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1317,46 +1317,46 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.2554397318815892</v>
+        <v>-0.2521528385341135</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0008614316052246115</v>
+        <v>-0.002908193588327743</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>0.0008788156191526246</v>
+        <v>-0.007877556123102243</v>
       </c>
       <c r="G13" t="n">
-        <v>0.001950384078015363</v>
+        <v>-0.002075730035029201</v>
       </c>
       <c r="H13" t="n">
-        <v>0.007692392947695717</v>
+        <v>0.01462823520912941</v>
       </c>
       <c r="I13" t="n">
-        <v>0.001862848394513936</v>
+        <v>-0.002026353201054128</v>
       </c>
       <c r="J13" t="n">
-        <v>0.001390904848332184</v>
+        <v>-0.006150569657710651</v>
       </c>
       <c r="K13" t="n">
-        <v>0.000420138352805534</v>
+        <v>0.00102105575284223</v>
       </c>
       <c r="L13" t="n">
-        <v>0.000420138352805534</v>
+        <v>0.00102105575284223</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>0.000420138352805534</v>
+        <v>0.00102105575284223</v>
       </c>
       <c r="P13" t="n">
-        <v>0.001015694056627762</v>
+        <v>0.006931826293273051</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0002995970039838801</v>
+        <v>0.001549068157962726</v>
       </c>
       <c r="R13" t="n">
-        <v>0.0002995970039838801</v>
+        <v>0.001549068157962726</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -1384,46 +1384,46 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.005020942952837717</v>
+        <v>-0.01172093653283746</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.01296310757659509</v>
+        <v>-0.03053229702929188</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>-0.002533826405353056</v>
+        <v>-0.02396571436662857</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0008433890257355609</v>
+        <v>-0.0222481626499265</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.00231142425245697</v>
+        <v>-0.003216135296645412</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.001200739824029593</v>
+        <v>-0.02258354355934174</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.009041638932665843</v>
+        <v>-0.008317087876348965</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.002857398354295934</v>
+        <v>0.000915060324602413</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.002857398354295934</v>
+        <v>0.000915060324602413</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>-0.002857398354295934</v>
+        <v>0.000915060324602413</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.003247900929916036</v>
+        <v>0.01291845968473839</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.003025480249019209</v>
+        <v>0.001783917863356714</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.003025480249019209</v>
+        <v>0.001783917863356714</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -1451,46 +1451,46 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.004298829675953186</v>
+        <v>0.00250652976426119</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01143851657580549</v>
+        <v>0.002746113805844552</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>0.007924564444982577</v>
+        <v>0.01088856648354266</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01566746520269861</v>
+        <v>0.01123400291336011</v>
       </c>
       <c r="H15" t="n">
-        <v>0.01364144128165765</v>
+        <v>-0.003405879976235199</v>
       </c>
       <c r="I15" t="n">
-        <v>0.01548056097122244</v>
+        <v>0.01109354127574165</v>
       </c>
       <c r="J15" t="n">
-        <v>0.001766270233166282</v>
+        <v>0.006490788878954224</v>
       </c>
       <c r="K15" t="n">
-        <v>0.006091158195646327</v>
+        <v>0.005768182118727283</v>
       </c>
       <c r="L15" t="n">
-        <v>0.006091158195646327</v>
+        <v>0.005768182118727283</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>0.006091158195646327</v>
+        <v>0.005768182118727283</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.001800305064012202</v>
+        <v>-0.002993503799740151</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.005431293625251745</v>
+        <v>0.004892334147693365</v>
       </c>
       <c r="R15" t="n">
-        <v>0.005431293625251745</v>
+        <v>0.004892334147693365</v>
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
@@ -1518,46 +1518,46 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.005653669378146775</v>
+        <v>-0.00757579729503189</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04237660556566892</v>
+        <v>-0.004229653321186132</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>-0.03715786372631454</v>
+        <v>-0.01057259274290371</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.02710069279602771</v>
+        <v>-0.01750070086002803</v>
       </c>
       <c r="H16" t="n">
-        <v>0.005559034302361371</v>
+        <v>-0.0125676850787074</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.02698751704750068</v>
+        <v>-0.01747838527513541</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.01694762435027908</v>
+        <v>0.01984456958246259</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01417636280705451</v>
+        <v>0.01460859456834378</v>
       </c>
       <c r="L16" t="n">
-        <v>0.01417636280705451</v>
+        <v>0.01460859456834378</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.01417636280705451</v>
+        <v>0.01460859456834378</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0208311050572442</v>
+        <v>0.02000200611208024</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.01493561781342471</v>
+        <v>0.01558223687928947</v>
       </c>
       <c r="R16" t="n">
-        <v>0.01493561781342471</v>
+        <v>0.01558223687928947</v>
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -1585,46 +1585,46 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.01524309411372376</v>
+        <v>-0.01344451541778062</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02223876627529953</v>
+        <v>0.001087392523495701</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>-0.01548651777146071</v>
+        <v>-0.001673615682944627</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.0172628800505152</v>
+        <v>-0.00947748277909931</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.004913672356546894</v>
+        <v>-0.01002837227313489</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.01697573031102921</v>
+        <v>-0.009413965912558636</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0004287815651000785</v>
+        <v>0.01309544051578936</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.002800927312037092</v>
+        <v>-0.003404443624177744</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.002800927312037092</v>
+        <v>-0.003404443624177744</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.002800927312037092</v>
+        <v>-0.003404443624177744</v>
       </c>
       <c r="P17" t="n">
-        <v>0.001677878371115135</v>
+        <v>0.002472568418902736</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.002454049730161989</v>
+        <v>-0.003054677594187103</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.002454049730161989</v>
+        <v>-0.003054677594187103</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -1648,46 +1648,46 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.01189405813976232</v>
+        <v>-0.01079580110383204</v>
       </c>
       <c r="D18" t="n">
-        <v>0.005934156125018485</v>
+        <v>1.123824044952962e-05</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>-0.008750272574010901</v>
+        <v>-0.006863862034554481</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.01068197562727902</v>
+        <v>-0.006181653463266138</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.001271698322867933</v>
+        <v>0.0009357823094312921</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.01062007655280306</v>
+        <v>-0.006111397588455902</v>
       </c>
       <c r="J18" t="n">
-        <v>0.002459519838645024</v>
+        <v>0.01811681354576014</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.01783831415353257</v>
+        <v>-0.01753561980542479</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.01783831415353257</v>
+        <v>-0.01753561980542479</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.01783831415353257</v>
+        <v>-0.01753561980542479</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.01406248606649944</v>
+        <v>-0.00949046303561852</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.01755987852639514</v>
+        <v>-0.01720851083234043</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.01755987852639514</v>
+        <v>-0.01720851083234043</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -1715,46 +1715,46 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0152217399688696</v>
+        <v>0.01489478680379147</v>
       </c>
       <c r="D19" t="n">
-        <v>0.03470776694905495</v>
+        <v>0.005544996989799878</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0.02437291623891664</v>
+        <v>0.01582147445685897</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01190156610806264</v>
+        <v>0.01463873597754944</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.01354190962967638</v>
+        <v>0.001187082767483311</v>
       </c>
       <c r="I19" t="n">
-        <v>0.01206320688252827</v>
+        <v>0.01461244935249797</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.005036609632446783</v>
+        <v>-0.02255692366241218</v>
       </c>
       <c r="K19" t="n">
-        <v>0.005830806281232251</v>
+        <v>0.004885644099425763</v>
       </c>
       <c r="L19" t="n">
-        <v>0.005830806281232251</v>
+        <v>0.004885644099425763</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>0.005830806281232251</v>
+        <v>0.004885644099425763</v>
       </c>
       <c r="P19" t="n">
-        <v>0.0002664905386596216</v>
+        <v>-0.00150449526017981</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.005445516793820672</v>
+        <v>0.004245403753816149</v>
       </c>
       <c r="R19" t="n">
-        <v>0.005445516793820672</v>
+        <v>0.004245403753816149</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -1782,46 +1782,46 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.0146182275927291</v>
+        <v>-0.01304478983379159</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01171039935412517</v>
+        <v>-0.0007818678072747121</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>0.001682485219299409</v>
+        <v>-0.001487210843488433</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.0001139402925576117</v>
+        <v>0.000340301101612044</v>
       </c>
       <c r="H20" t="n">
-        <v>0.005736791845471673</v>
+        <v>0.00299039349561574</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.0002335876893435075</v>
+        <v>0.0004238591209543648</v>
       </c>
       <c r="J20" t="n">
-        <v>0.01068637276366789</v>
+        <v>0.004983708866629796</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.01713155194926208</v>
+        <v>-0.01586996194679847</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.01713155194926208</v>
+        <v>-0.01586996194679847</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>-0.01713155194926208</v>
+        <v>-0.01586996194679847</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.01379992557599702</v>
+        <v>-0.008952486406099455</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.01690873555634942</v>
+        <v>-0.01523008918520357</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.01690873555634942</v>
+        <v>-0.01523008918520357</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -1845,46 +1845,46 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.02365294232211769</v>
+        <v>-0.02406885283475411</v>
       </c>
       <c r="D21" t="n">
-        <v>0.004910407989048378</v>
+        <v>0.002703635724145429</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>0.01970623394024935</v>
+        <v>0.01935088771803551</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0232075800643032</v>
+        <v>0.01822441685697667</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01319242113569684</v>
+        <v>0.006605646408225856</v>
       </c>
       <c r="I21" t="n">
-        <v>0.02362501246500049</v>
+        <v>0.0179326151493046</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.006885243185743782</v>
+        <v>0.009024643304414874</v>
       </c>
       <c r="K21" t="n">
-        <v>0.01027890578715623</v>
+        <v>0.009950289518011579</v>
       </c>
       <c r="L21" t="n">
-        <v>0.01027890578715623</v>
+        <v>0.009950289518011579</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0.01027890578715623</v>
+        <v>0.009950289518011579</v>
       </c>
       <c r="P21" t="n">
-        <v>0.0001958234958329398</v>
+        <v>0.001612530784501231</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.0094033425521337</v>
+        <v>0.009133109549324381</v>
       </c>
       <c r="R21" t="n">
-        <v>0.0094033425521337</v>
+        <v>0.009133109549324381</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -1908,46 +1908,46 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.02845372145814885</v>
+        <v>-0.02979840051993602</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.005165712851008712</v>
+        <v>-0.007685123731404949</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>0.006075724083028962</v>
+        <v>-0.01547446535497861</v>
       </c>
       <c r="G22" t="n">
-        <v>-5.616019424640776e-05</v>
+        <v>-0.009003568584142741</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.001382999287319971</v>
+        <v>0.01293372186134887</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0003369158534766341</v>
+        <v>-0.009188743087549722</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.008980729336871699</v>
+        <v>0.01215688690766466</v>
       </c>
       <c r="K22" t="n">
-        <v>0.001570892222835689</v>
+        <v>0.002083030931321237</v>
       </c>
       <c r="L22" t="n">
-        <v>0.001570892222835689</v>
+        <v>0.002083030931321237</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.001570892222835689</v>
+        <v>0.002083030931321237</v>
       </c>
       <c r="P22" t="n">
-        <v>0.00119370100774804</v>
+        <v>0.007236263425450537</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.001486156187446248</v>
+        <v>0.002269215354768614</v>
       </c>
       <c r="R22" t="n">
-        <v>0.001486156187446248</v>
+        <v>0.002269215354768614</v>
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
@@ -1971,46 +1971,46 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.002454939266197571</v>
+        <v>0.001658177538327101</v>
       </c>
       <c r="D23" t="n">
-        <v>0.02339182599563995</v>
+        <v>-0.001372140150885606</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>0.007265098754603949</v>
+        <v>-0.001804323624172945</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00726539203461568</v>
+        <v>0.003535517709420708</v>
       </c>
       <c r="H23" t="n">
-        <v>0.009265063474602538</v>
+        <v>0.001598797215951888</v>
       </c>
       <c r="I23" t="n">
-        <v>0.00724022726560909</v>
+        <v>0.003463363050534521</v>
       </c>
       <c r="J23" t="n">
-        <v>0.02528705258050536</v>
+        <v>0.01822706221659564</v>
       </c>
       <c r="K23" t="n">
-        <v>0.006553624198144967</v>
+        <v>0.007247328193893126</v>
       </c>
       <c r="L23" t="n">
-        <v>0.006553624198144967</v>
+        <v>0.007247328193893126</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>0.006553624198144967</v>
+        <v>0.007247328193893126</v>
       </c>
       <c r="P23" t="n">
-        <v>0.002279264731170589</v>
+        <v>0.007226590177063607</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.006308300124332003</v>
+        <v>0.007130669373226775</v>
       </c>
       <c r="R23" t="n">
-        <v>0.006308300124332003</v>
+        <v>0.007130669373226775</v>
       </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
@@ -2038,46 +2038,46 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.02729398822775952</v>
+        <v>-0.02329348384373935</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0008926292950134078</v>
+        <v>0.01651558885262355</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>-0.004664269818570791</v>
+        <v>0.005120454732818189</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.007824648792985951</v>
+        <v>0.01320030888001236</v>
       </c>
       <c r="H24" t="n">
-        <v>0.000264292426571697</v>
+        <v>0.02138318667932746</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.008017887584715501</v>
+        <v>0.01332821851712874</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.00717053195161576</v>
+        <v>0.03298953944641232</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.003105312700212508</v>
+        <v>-0.005299281907971276</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.003105312700212508</v>
+        <v>-0.005299281907971276</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>-0.003105312700212508</v>
+        <v>-0.005299281907971276</v>
       </c>
       <c r="P24" t="n">
-        <v>0.001157697070307882</v>
+        <v>-0.009435208985408358</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.002790075471603019</v>
+        <v>-0.005419061112762444</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.002790075471603019</v>
+        <v>-0.005419061112762444</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -2101,46 +2101,46 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.008994435431777416</v>
+        <v>-0.01058492269539691</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01743691375436066</v>
+        <v>-0.02022354388094175</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>0.02464181820167272</v>
+        <v>-0.0003974210078968403</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0135749324789973</v>
+        <v>-0.005952787630111505</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.002656131946245277</v>
+        <v>-0.0148964200518568</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0134264975610599</v>
+        <v>-0.006019732848789313</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.005608375081455526</v>
+        <v>0.01613827558543973</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.004090888867635555</v>
+        <v>-0.001420953272838131</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.004090888867635555</v>
+        <v>-0.001420953272838131</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>-0.004090888867635555</v>
+        <v>-0.001420953272838131</v>
       </c>
       <c r="P25" t="n">
-        <v>-0.009162533454501336</v>
+        <v>0.0008184400647376026</v>
       </c>
       <c r="Q25" t="n">
-        <v>-0.004444369425774777</v>
+        <v>-0.00100427399217096</v>
       </c>
       <c r="R25" t="n">
-        <v>-0.004444369425774777</v>
+        <v>-0.00100427399217096</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -2168,46 +2168,46 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.01774695949387838</v>
+        <v>0.01406782971471319</v>
       </c>
       <c r="D26" t="n">
-        <v>0.007725442863024937</v>
+        <v>-0.01490230658009226</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>-0.00276254401450176</v>
+        <v>-0.00490661126826445</v>
       </c>
       <c r="G26" t="n">
-        <v>0.001005200488208019</v>
+        <v>-0.01217557795902312</v>
       </c>
       <c r="H26" t="n">
-        <v>0.004971258150850325</v>
+        <v>-0.02671977985279119</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0006990901719636069</v>
+        <v>-0.01197286204691448</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.003728443332053025</v>
+        <v>0.002513406420174452</v>
       </c>
       <c r="K26" t="n">
-        <v>0.02113133777325351</v>
+        <v>0.02341370599254824</v>
       </c>
       <c r="L26" t="n">
-        <v>0.02113133777325351</v>
+        <v>0.02341370599254824</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>0.02113133777325351</v>
+        <v>0.02341370599254824</v>
       </c>
       <c r="P26" t="n">
-        <v>0.01640330638413225</v>
+        <v>0.02464453164178126</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.02075838054233522</v>
+        <v>0.02383228732129149</v>
       </c>
       <c r="R26" t="n">
-        <v>0.02075838054233522</v>
+        <v>0.02383228732129149</v>
       </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
@@ -2231,46 +2231,46 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.0006582425543297021</v>
+        <v>0.006530090853203633</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.009126280473120675</v>
+        <v>0.01960177316807092</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>-0.002578364551134582</v>
+        <v>0.01741712085668483</v>
       </c>
       <c r="G27" t="n">
-        <v>0.004154058214162327</v>
+        <v>0.01557557985502319</v>
       </c>
       <c r="H27" t="n">
-        <v>0.01652795019711801</v>
+        <v>0.008336320557452821</v>
       </c>
       <c r="I27" t="n">
-        <v>0.004423851824954073</v>
+        <v>0.01530699594027984</v>
       </c>
       <c r="J27" t="n">
-        <v>0.006858881775564433</v>
+        <v>0.007932186981751981</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.0189499699099988</v>
+        <v>-0.02260214692008587</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.0189499699099988</v>
+        <v>-0.02260214692008587</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-0.0189499699099988</v>
+        <v>-0.02260214692008587</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.01707742484309699</v>
+        <v>-0.02690461134818445</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.01907497765899911</v>
+        <v>-0.02379751151190046</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.01907497765899911</v>
+        <v>-0.02379751151190046</v>
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
@@ -2298,46 +2298,46 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.009422242552889702</v>
+        <v>0.0132205900328236</v>
       </c>
       <c r="D28" t="n">
-        <v>0.01313904259382564</v>
+        <v>0.01176916271076651</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>0.04540652783226111</v>
+        <v>0.03305523108220924</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02730709107628364</v>
+        <v>0.02653274112530964</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.01781124416844976</v>
+        <v>-0.01178896069555843</v>
       </c>
       <c r="I28" t="n">
-        <v>0.02783673941746957</v>
+        <v>0.02640052118402084</v>
       </c>
       <c r="J28" t="n">
-        <v>0.006877698292840408</v>
+        <v>0.0243887700831779</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0006104059444162377</v>
+        <v>-0.001224893136995725</v>
       </c>
       <c r="L28" t="n">
-        <v>0.0006104059444162377</v>
+        <v>-0.001224893136995725</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>0.0006104059444162377</v>
+        <v>-0.001224893136995725</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.01088601835544073</v>
+        <v>-0.01568703653148146</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.0003529469901178796</v>
+        <v>-0.00261307776852311</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.0003529469901178796</v>
+        <v>-0.00261307776852311</v>
       </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
@@ -2365,46 +2365,46 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.008110547940421917</v>
+        <v>0.005116735404669416</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.00120621003123871</v>
+        <v>-0.01346903641076145</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>-0.009814426664577065</v>
+        <v>-0.0167711300148452</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.020079600035184</v>
+        <v>-0.02121814673672587</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.02268926135557045</v>
+        <v>-0.01634871607794864</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.02010203197208128</v>
+        <v>-0.02119111380764455</v>
       </c>
       <c r="J29" t="n">
-        <v>0.006635524181680764</v>
+        <v>-0.0008650728058904444</v>
       </c>
       <c r="K29" t="n">
-        <v>0.01866423117856924</v>
+        <v>0.02038781236751249</v>
       </c>
       <c r="L29" t="n">
-        <v>0.01866423117856924</v>
+        <v>0.02038781236751249</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>0.01866423117856924</v>
+        <v>0.02038781236751249</v>
       </c>
       <c r="P29" t="n">
-        <v>0.02476831337473253</v>
+        <v>0.02862204863288194</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.0192413699536548</v>
+        <v>0.02164319356972774</v>
       </c>
       <c r="R29" t="n">
-        <v>0.0192413699536548</v>
+        <v>0.02164319356972774</v>
       </c>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
@@ -2432,46 +2432,46 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.01817332191093287</v>
+        <v>-0.02277520574300822</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.01720307153048579</v>
+        <v>-0.02053317413332696</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>0.001825771177030847</v>
+        <v>-0.01564689019387561</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0005187530127501205</v>
+        <v>-0.0203086676603467</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0003288196931527877</v>
+        <v>-0.02038831492753259</v>
       </c>
       <c r="I30" t="n">
-        <v>0.0003994732959789318</v>
+        <v>-0.01999129961565198</v>
       </c>
       <c r="J30" t="n">
-        <v>0.002367387918249874</v>
+        <v>-0.01562967343549799</v>
       </c>
       <c r="K30" t="n">
-        <v>0.02310354351614174</v>
+        <v>0.0261552126622085</v>
       </c>
       <c r="L30" t="n">
-        <v>0.02310354351614174</v>
+        <v>0.0261552126622085</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>0.02310354351614174</v>
+        <v>0.0261552126622085</v>
       </c>
       <c r="P30" t="n">
-        <v>0.02025834215433368</v>
+        <v>0.0301511575260463</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.02306500815460032</v>
+        <v>0.02698308587932343</v>
       </c>
       <c r="R30" t="n">
-        <v>0.02306500815460032</v>
+        <v>0.02698308587932343</v>
       </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
@@ -2499,46 +2499,46 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.002042385585695423</v>
+        <v>-0.001160504398420176</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.001809425503016991</v>
+        <v>-0.002391382367655294</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>0.0271946699837868</v>
+        <v>0.007411642472465697</v>
       </c>
       <c r="G31" t="n">
-        <v>0.02208185128327405</v>
+        <v>0.01309077076363083</v>
       </c>
       <c r="H31" t="n">
-        <v>0.003468937482757499</v>
+        <v>0.01535019162200766</v>
       </c>
       <c r="I31" t="n">
-        <v>0.02242167900886716</v>
+        <v>0.01309952932398117</v>
       </c>
       <c r="J31" t="n">
-        <v>0.03158258718662511</v>
+        <v>-0.02339965752841897</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.01042549462501978</v>
+        <v>-0.009856782154271285</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.01042549462501978</v>
+        <v>-0.009856782154271285</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.01042549462501978</v>
+        <v>-0.009856782154271285</v>
       </c>
       <c r="P31" t="n">
-        <v>-0.01526771091470843</v>
+        <v>-0.01195964140638566</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.01099040443961618</v>
+        <v>-0.01008477717139108</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.01099040443961618</v>
+        <v>-0.01008477717139108</v>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
@@ -2566,46 +2566,46 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-0.002240712665628506</v>
+        <v>-0.002703026892121075</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.0225759394033914</v>
+        <v>-0.001273986386959456</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>0.007676998291079931</v>
+        <v>0.003664351826574073</v>
       </c>
       <c r="G32" t="n">
-        <v>0.005887446091497842</v>
+        <v>0.002101736244069449</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.003206272448250897</v>
+        <v>-0.006463727586549102</v>
       </c>
       <c r="I32" t="n">
-        <v>0.005656732642269305</v>
+        <v>0.002181935607277424</v>
       </c>
       <c r="J32" t="n">
-        <v>0.01815772135287096</v>
+        <v>0.002686926968905323</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0006708062668322506</v>
+        <v>0.0009779361991174478</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0006708062668322506</v>
+        <v>0.0009779361991174478</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>0.0006708062668322506</v>
+        <v>0.0009779361991174478</v>
       </c>
       <c r="P32" t="n">
-        <v>-0.0002521523620860945</v>
+        <v>0.002621674280866971</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.0004646546105861843</v>
+        <v>0.0007598308143932324</v>
       </c>
       <c r="R32" t="n">
-        <v>0.0004646546105861843</v>
+        <v>0.0007598308143932324</v>
       </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
@@ -2633,46 +2633,46 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.005099865227994608</v>
+        <v>-0.005380277495211099</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.01082878749563794</v>
+        <v>-0.003106481884259275</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>0.01520581558423262</v>
+        <v>0.006393684831747392</v>
       </c>
       <c r="G33" t="n">
-        <v>0.01162488718499548</v>
+        <v>0.001896060939842437</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.01212471667698867</v>
+        <v>-0.00685405976216239</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01172521035700841</v>
+        <v>0.002008212944328517</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.002385046530723285</v>
+        <v>0.02027661082638242</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.009106814764272591</v>
+        <v>-0.00941764156070566</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.009106814764272591</v>
+        <v>-0.00941764156070566</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>-0.009106814764272591</v>
+        <v>-0.00941764156070566</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.01338007061520282</v>
+        <v>-0.01491103038844121</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.009475847803033911</v>
+        <v>-0.01004795924991837</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.009475847803033911</v>
+        <v>-0.01004795924991837</v>
       </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
@@ -2700,46 +2700,46 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.004698232795929311</v>
+        <v>0.004701084956043397</v>
       </c>
       <c r="D34" t="n">
-        <v>0.000825380603515067</v>
+        <v>0.002479635075185403</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>0.01819923845596954</v>
+        <v>0.01354547986981919</v>
       </c>
       <c r="G34" t="n">
-        <v>0.01899542946381718</v>
+        <v>0.0128617875224715</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0142185024887401</v>
+        <v>0.006741715853668633</v>
       </c>
       <c r="I34" t="n">
-        <v>0.01898466181538647</v>
+        <v>0.01291435664457426</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.002534036172432607</v>
+        <v>0.005875111561014671</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01638904903956196</v>
+        <v>0.01586664821866593</v>
       </c>
       <c r="L34" t="n">
-        <v>0.01638904903956196</v>
+        <v>0.01586664821866593</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>0.01638904903956196</v>
+        <v>0.01586664821866593</v>
       </c>
       <c r="P34" t="n">
-        <v>0.006429044609161784</v>
+        <v>0.001772511526900461</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.01555763534230541</v>
+        <v>0.01486564389062575</v>
       </c>
       <c r="R34" t="n">
-        <v>0.01555763534230541</v>
+        <v>0.01486564389062575</v>
       </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
@@ -2767,46 +2767,46 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.0176207275528291</v>
+        <v>-0.01550356314814252</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.005777601454693781</v>
+        <v>0.007347835109913403</v>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
-        <v>-0.003016383096655323</v>
+        <v>-0.003360366950414678</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.005913478604539144</v>
+        <v>0.001238096593523863</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.008837224001488959</v>
+        <v>0.007503951756158069</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.006038788849551553</v>
+        <v>0.001068125706725028</v>
       </c>
       <c r="J35" t="n">
-        <v>0.008360038196204874</v>
+        <v>-0.01773635998258703</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.009601231392049254</v>
+        <v>-0.01054295811771832</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.009601231392049254</v>
+        <v>-0.01054295811771832</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>-0.009601231392049254</v>
+        <v>-0.01054295811771832</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.004805093952203758</v>
+        <v>-0.005926812621072504</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.0094249625209985</v>
+        <v>-0.01043680371347215</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.0094249625209985</v>
+        <v>-0.01043680371347215</v>
       </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
@@ -2834,46 +2834,46 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.02436408788656352</v>
+        <v>-0.02432562903702516</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.00747774747370779</v>
+        <v>-0.005466936218677448</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>0.004991029735641189</v>
+        <v>0.001642986305719452</v>
       </c>
       <c r="G36" t="n">
-        <v>0.005688560579542421</v>
+        <v>0.0008755103390204134</v>
       </c>
       <c r="H36" t="n">
-        <v>0.005711477988459119</v>
+        <v>0.001102200812088032</v>
       </c>
       <c r="I36" t="n">
-        <v>0.005911277228451089</v>
+        <v>0.0009113484844539394</v>
       </c>
       <c r="J36" t="n">
-        <v>0.006338198017460051</v>
+        <v>0.0240747876394992</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0004751938750077549</v>
+        <v>0.001646594849863794</v>
       </c>
       <c r="L36" t="n">
-        <v>0.0004751938750077549</v>
+        <v>0.001646594849863794</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>0.0004751938750077549</v>
+        <v>0.001646594849863794</v>
       </c>
       <c r="P36" t="n">
-        <v>-0.001773342022933681</v>
+        <v>0.0006253346170133846</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.0002687854187514167</v>
+        <v>0.001687245859489834</v>
       </c>
       <c r="R36" t="n">
-        <v>0.0002687854187514167</v>
+        <v>0.001687245859489834</v>
       </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
@@ -2901,46 +2901,46 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.003930700093228003</v>
+        <v>0.006738285101531403</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.00931794946698741</v>
+        <v>0.01341683295267332</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>0.007232154049286161</v>
+        <v>0.007585475727419028</v>
       </c>
       <c r="G37" t="n">
-        <v>0.007508999148359965</v>
+        <v>0.01621331776853271</v>
       </c>
       <c r="H37" t="n">
-        <v>0.006852281074091242</v>
+        <v>0.01759075980763039</v>
       </c>
       <c r="I37" t="n">
-        <v>0.00788960853958434</v>
+        <v>0.01612718397308736</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.003440873571032096</v>
+        <v>0.02171840014874861</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.02527203816288152</v>
+        <v>-0.02635575215823008</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.02527203816288152</v>
+        <v>-0.02635575215823008</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.02527203816288152</v>
+        <v>-0.02635575215823008</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.02309213621968545</v>
+        <v>-0.02463861784954471</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.02508177594727104</v>
+        <v>-0.02656828474273139</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.02508177594727104</v>
+        <v>-0.02656828474273139</v>
       </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
@@ -2968,46 +2968,46 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.00750077578803103</v>
+        <v>0.0131242425089697</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.01479495282217837</v>
+        <v>0.02909218925968757</v>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>-0.02418561418342456</v>
+        <v>0.003514339820573592</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.02415674995826999</v>
+        <v>0.00702758831310353</v>
       </c>
       <c r="H38" t="n">
-        <v>-0.02107670637906825</v>
+        <v>0.01139832890393315</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.02425562237822489</v>
+        <v>0.006988223415528935</v>
       </c>
       <c r="J38" t="n">
-        <v>0.01157996270946172</v>
+        <v>0.03180076891889724</v>
       </c>
       <c r="K38" t="n">
-        <v>0.0209359901494396</v>
+        <v>0.01636106811044272</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0209359901494396</v>
+        <v>0.01636106811044272</v>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
-        <v>0.0209359901494396</v>
+        <v>0.01636106811044272</v>
       </c>
       <c r="P38" t="n">
-        <v>0.02773988290159532</v>
+        <v>0.006167889558715581</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.02154806150192246</v>
+        <v>0.01571242987649719</v>
       </c>
       <c r="R38" t="n">
-        <v>0.02154806150192246</v>
+        <v>0.01571242987649719</v>
       </c>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
@@ -3035,46 +3035,46 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.000149005925960237</v>
+        <v>0.00151507849260314</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.01762884272400572</v>
+        <v>0.009771227334849092</v>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>-0.01421486197659448</v>
+        <v>-0.00677386203095448</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.01828741282749651</v>
+        <v>-0.003723678772947151</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.006541213893648554</v>
+        <v>0.01134341421373657</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.01863386954535478</v>
+        <v>-0.00355128599805144</v>
       </c>
       <c r="J39" t="n">
-        <v>0.0003222161954320616</v>
+        <v>0.002708158901950766</v>
       </c>
       <c r="K39" t="n">
-        <v>0.9936877132835085</v>
+        <v>0.9837618257184729</v>
       </c>
       <c r="L39" t="n">
-        <v>0.9936877132835085</v>
+        <v>0.9837618257184729</v>
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
-        <v>0.9936877132835085</v>
+        <v>0.9837618257184729</v>
       </c>
       <c r="P39" t="n">
-        <v>0.8655223714208947</v>
+        <v>0.7163593490383737</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.9894557933062316</v>
+        <v>0.9732053123042123</v>
       </c>
       <c r="R39" t="n">
-        <v>0.9894557933062316</v>
+        <v>0.9732053123042123</v>
       </c>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>

</xml_diff>

<commit_message>
remove DAP and CSL from sugarcane biorefineries and rerun
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -730,50 +730,50 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Oil retention [%]</t>
+          <t>Oil extraction efficiency [%]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.001981087567243502</v>
+        <v>-0.001805598696223948</v>
       </c>
       <c r="D4" t="n">
         <v>0.003529454733178189</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.002691628715665148</v>
+        <v>0.002815131472605259</v>
       </c>
       <c r="G4" t="n">
-        <v>-9.089693163587725e-05</v>
+        <v>-8.951001958040078e-05</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.007891063515642541</v>
+        <v>-0.008031360993254438</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.0001278572211142888</v>
+        <v>-0.0001250898290035931</v>
       </c>
       <c r="J4" t="n">
-        <v>0.03567766691724603</v>
+        <v>-0.003406548333611173</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.02581511354460454</v>
+        <v>-0.02582483988099359</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.02581511354460454</v>
+        <v>-0.02582483988099359</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>-0.02581511354460454</v>
+        <v>-0.02582483988099359</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0166109524724381</v>
+        <v>-0.01661295157651806</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.02541449736857989</v>
+        <v>-0.0254064900082596</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.02541449736857989</v>
+        <v>-0.0254064900082596</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -797,46 +797,46 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01669288626771545</v>
+        <v>0.01691192650047706</v>
       </c>
       <c r="D5" t="n">
         <v>0.007570266830810672</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>-0.00998490654339626</v>
+        <v>-0.009807110888284435</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.003539690445587617</v>
+        <v>-0.003540789069631563</v>
       </c>
       <c r="H5" t="n">
-        <v>0.006926079445043177</v>
+        <v>0.006190136791605471</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.003627023473080938</v>
+        <v>-0.003626354641054185</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.02018644103050018</v>
+        <v>0.0211044324088877</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0002487987939519517</v>
+        <v>-0.000243219849728794</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.0002487987939519517</v>
+        <v>-0.000243219849728794</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>-0.0002487987939519517</v>
+        <v>-0.000243219849728794</v>
       </c>
       <c r="P5" t="n">
-        <v>0.001185909839436393</v>
+        <v>0.00118259351930374</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0003375250695010027</v>
+        <v>-0.0003506409740256389</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.0003375250695010027</v>
+        <v>-0.0003506409740256389</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -860,46 +860,46 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2160015041280601</v>
+        <v>0.2151594933743797</v>
       </c>
       <c r="D6" t="n">
         <v>0.0108233524329341</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>-0.563932652925306</v>
+        <v>-0.5638260619130424</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.6033473026938919</v>
+        <v>-0.6033498936379956</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.3537699437187977</v>
+        <v>-0.3537427894457115</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.6031647557105901</v>
+        <v>-0.6031578122223124</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.01357855879495565</v>
+        <v>0.0008550462748406081</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1256377155215086</v>
+        <v>0.1253767402790696</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1256377155215086</v>
+        <v>0.1253767402790696</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.1256377155215086</v>
+        <v>0.1253767402790696</v>
       </c>
       <c r="P6" t="n">
-        <v>0.4260346111213844</v>
+        <v>0.4260310026732401</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1551090166683606</v>
+        <v>0.1546804332912173</v>
       </c>
       <c r="R6" t="n">
-        <v>0.1551090166683606</v>
+        <v>0.1546804332912173</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -923,46 +923,46 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.00711654652466186</v>
+        <v>-0.007262751938510077</v>
       </c>
       <c r="D7" t="n">
         <v>-0.004311911308476452</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>-0.001606011424240457</v>
+        <v>-0.001757649574305983</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.00718743926349757</v>
+        <v>-0.007191082655643306</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.01700430807217232</v>
+        <v>-0.01679513481580539</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.007146824253872969</v>
+        <v>-0.007145027805801111</v>
       </c>
       <c r="J7" t="n">
-        <v>0.01254155264794391</v>
+        <v>-0.01459581159757058</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.01132881126915245</v>
+        <v>-0.01133216022928641</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.01132881126915245</v>
+        <v>-0.01133216022928641</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.01132881126915245</v>
+        <v>-0.01133216022928641</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.003662758994510359</v>
+        <v>-0.003662699282507971</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.01104846840993874</v>
+        <v>-0.01107397801095912</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.01104846840993874</v>
+        <v>-0.01107397801095912</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -986,46 +986,46 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.214314225820569</v>
+        <v>0.2132259085290363</v>
       </c>
       <c r="D8" t="n">
         <v>0.9999999999999999</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>0.720325628941025</v>
+        <v>0.7203509601740383</v>
       </c>
       <c r="G8" t="n">
-        <v>0.7774172114806883</v>
+        <v>0.7774153547446141</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4705695211267807</v>
+        <v>0.4704548058261921</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7776363104654522</v>
+        <v>0.7776420480976819</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.01631292263716014</v>
+        <v>3.587245612355099e-05</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.1274815802032632</v>
+        <v>-0.1271341606053664</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.1274815802032632</v>
+        <v>-0.1271341606053664</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>-0.1274815802032632</v>
+        <v>-0.1271341606053664</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.5227168998526759</v>
+        <v>-0.5227086724603469</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.1656055947842238</v>
+        <v>-0.1650400090336003</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1656055947842238</v>
+        <v>-0.1650400090336003</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1053,46 +1053,46 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9182517237700688</v>
+        <v>0.9187926533597061</v>
       </c>
       <c r="D9" t="n">
         <v>0.01752971628518865</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.005848386089935442</v>
+        <v>0.005978610863144434</v>
       </c>
       <c r="G9" t="n">
-        <v>0.007325336069013442</v>
+        <v>0.007325240069009602</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00676550878262035</v>
+        <v>0.006343667581746702</v>
       </c>
       <c r="I9" t="n">
-        <v>0.007335383429415336</v>
+        <v>0.007334970341398813</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0130547926729756</v>
+        <v>0.008582926013091819</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.005186724495468979</v>
+        <v>-0.005183439471337578</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.005186724495468979</v>
+        <v>-0.005183439471337578</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>-0.005186724495468979</v>
+        <v>-0.005183439471337578</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.005742566341702653</v>
+        <v>-0.005739506149580246</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.005446028665841146</v>
+        <v>-0.005448242617929704</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.005446028665841146</v>
+        <v>-0.005448242617929704</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1120,46 +1120,46 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.007565449742617988</v>
+        <v>0.007911417532456701</v>
       </c>
       <c r="D10" t="n">
         <v>0.003197859583914383</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>-0.01201252838450113</v>
+        <v>-0.01238593527943741</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.01145373962614958</v>
+        <v>-0.01145660935426437</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.01739417791176711</v>
+        <v>-0.01643041380921655</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.01130386576415463</v>
+        <v>-0.01130444339617773</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.004743453616201123</v>
+        <v>-0.03443317322613024</v>
       </c>
       <c r="K10" t="n">
-        <v>0.01439699155187966</v>
+        <v>0.01439521161580846</v>
       </c>
       <c r="L10" t="n">
-        <v>0.01439699155187966</v>
+        <v>0.01439521161580846</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>0.01439699155187966</v>
+        <v>0.01439521161580846</v>
       </c>
       <c r="P10" t="n">
-        <v>0.01642396577695863</v>
+        <v>0.01642423668896947</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.01487034654681386</v>
+        <v>0.01489065870762635</v>
       </c>
       <c r="R10" t="n">
-        <v>0.01487034654681386</v>
+        <v>0.01489065870762635</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -1187,46 +1187,46 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0137612451584498</v>
+        <v>-0.005134877101395083</v>
       </c>
       <c r="D11" t="n">
         <v>0.007627171025086841</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.008224741384989654</v>
+        <v>0.007772764918910595</v>
       </c>
       <c r="G11" t="n">
-        <v>0.009251631922065276</v>
+        <v>0.009254838418193535</v>
       </c>
       <c r="H11" t="n">
-        <v>0.01050162061206482</v>
+        <v>0.01152697649307906</v>
       </c>
       <c r="I11" t="n">
-        <v>0.009299025107961002</v>
+        <v>0.009303624180144967</v>
       </c>
       <c r="J11" t="n">
-        <v>0.01780943717607295</v>
+        <v>-0.005856193396860967</v>
       </c>
       <c r="K11" t="n">
-        <v>0.00407715126708605</v>
+        <v>0.004075133251005329</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00407715126708605</v>
+        <v>0.004075133251005329</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>0.00407715126708605</v>
+        <v>0.004075133251005329</v>
       </c>
       <c r="P11" t="n">
-        <v>0.002271869178874767</v>
+        <v>0.002271675066867002</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.003972715358908614</v>
+        <v>0.003992690463707618</v>
       </c>
       <c r="R11" t="n">
-        <v>0.003972715358908614</v>
+        <v>0.003992690463707618</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -1254,46 +1254,46 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.01733204488528179</v>
+        <v>0.01762163849686554</v>
       </c>
       <c r="D12" t="n">
         <v>-0.004942293317691732</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>-0.007013254264530169</v>
+        <v>-0.006885461939418476</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0002977445879097835</v>
+        <v>0.0002937789237511569</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.001398786295951451</v>
+        <v>-0.001662464322498573</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0003649513105980523</v>
+        <v>0.0003655281746211269</v>
       </c>
       <c r="J12" t="n">
-        <v>0.01981871936651867</v>
+        <v>-0.007518890583750679</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.01399853835194153</v>
+        <v>-0.01400107976004319</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.01399853835194153</v>
+        <v>-0.01400107976004319</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>-0.01399853835194153</v>
+        <v>-0.01400107976004319</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.01132916186116647</v>
+        <v>-0.01132544541301781</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.01404465041778601</v>
+        <v>-0.01403174465726978</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.01404465041778601</v>
+        <v>-0.01403174465726978</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1317,46 +1317,46 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.2521528385341135</v>
+        <v>-0.2511357147494286</v>
       </c>
       <c r="D13" t="n">
         <v>-0.002908193588327743</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>-0.007877556123102243</v>
+        <v>-0.007574787374991494</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.002075730035029201</v>
+        <v>-0.002082747635309905</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01462823520912941</v>
+        <v>0.01348539836341593</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.002026353201054128</v>
+        <v>-0.002026440369057614</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.006150569657710651</v>
+        <v>-0.02078204207866716</v>
       </c>
       <c r="K13" t="n">
-        <v>0.00102105575284223</v>
+        <v>0.001018452040738081</v>
       </c>
       <c r="L13" t="n">
-        <v>0.00102105575284223</v>
+        <v>0.001018452040738081</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>0.00102105575284223</v>
+        <v>0.001018452040738081</v>
       </c>
       <c r="P13" t="n">
-        <v>0.006931826293273051</v>
+        <v>0.006932053909282155</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.001549068157962726</v>
+        <v>0.001544063677762547</v>
       </c>
       <c r="R13" t="n">
-        <v>0.001549068157962726</v>
+        <v>0.001544063677762547</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -1384,46 +1384,46 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.01172093653283746</v>
+        <v>-0.01189095455563818</v>
       </c>
       <c r="D14" t="n">
         <v>-0.03053229702929188</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>-0.02396571436662857</v>
+        <v>-0.02384057663362307</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0222481626499265</v>
+        <v>-0.02224848626593945</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.003216135296645412</v>
+        <v>-0.003485854123434165</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.02258354355934174</v>
+        <v>-0.02258457469538298</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.008317087876348965</v>
+        <v>0.01880537086035513</v>
       </c>
       <c r="K14" t="n">
-        <v>0.000915060324602413</v>
+        <v>0.0008861699874467995</v>
       </c>
       <c r="L14" t="n">
-        <v>0.000915060324602413</v>
+        <v>0.0008861699874467995</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>0.000915060324602413</v>
+        <v>0.0008861699874467995</v>
       </c>
       <c r="P14" t="n">
-        <v>0.01291845968473839</v>
+        <v>0.0129218225648729</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.001783917863356714</v>
+        <v>0.00178535200741408</v>
       </c>
       <c r="R14" t="n">
-        <v>0.001783917863356714</v>
+        <v>0.00178535200741408</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -1451,46 +1451,46 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.00250652976426119</v>
+        <v>0.002690847659633906</v>
       </c>
       <c r="D15" t="n">
         <v>0.002746113805844552</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>0.01088856648354266</v>
+        <v>0.01115647964625919</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01123400291336011</v>
+        <v>0.01122936937717477</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.003405879976235199</v>
+        <v>-0.003778300567132022</v>
       </c>
       <c r="I15" t="n">
-        <v>0.01109354127574165</v>
+        <v>0.01109426098777044</v>
       </c>
       <c r="J15" t="n">
-        <v>0.006490788878954224</v>
+        <v>-0.002515029909963574</v>
       </c>
       <c r="K15" t="n">
-        <v>0.005768182118727283</v>
+        <v>0.005770485830819433</v>
       </c>
       <c r="L15" t="n">
-        <v>0.005768182118727283</v>
+        <v>0.005770485830819433</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>0.005768182118727283</v>
+        <v>0.005770485830819433</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.002993503799740151</v>
+        <v>-0.00299773701590948</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.004892334147693365</v>
+        <v>0.004906316836252673</v>
       </c>
       <c r="R15" t="n">
-        <v>0.004892334147693365</v>
+        <v>0.004906316836252673</v>
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
@@ -1518,46 +1518,46 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.00757579729503189</v>
+        <v>-0.007293548547741942</v>
       </c>
       <c r="D16" t="n">
         <v>-0.004229653321186132</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>-0.01057259274290371</v>
+        <v>-0.01021424392856976</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.01750070086002803</v>
+        <v>-0.01750016940400678</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.0125676850787074</v>
+        <v>-0.01331496178059847</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.01747838527513541</v>
+        <v>-0.01748220357928814</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01984456958246259</v>
+        <v>-0.005780761776838957</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01460859456834378</v>
+        <v>0.0146004950480198</v>
       </c>
       <c r="L16" t="n">
-        <v>0.01460859456834378</v>
+        <v>0.0146004950480198</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.01460859456834378</v>
+        <v>0.0146004950480198</v>
       </c>
       <c r="P16" t="n">
-        <v>0.02000200611208024</v>
+        <v>0.02000229200009167</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.01558223687928947</v>
+        <v>0.01557386097495444</v>
       </c>
       <c r="R16" t="n">
-        <v>0.01558223687928947</v>
+        <v>0.01557386097495444</v>
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -1585,46 +1585,46 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.01344451541778062</v>
+        <v>-0.01344671093786844</v>
       </c>
       <c r="D17" t="n">
         <v>0.001087392523495701</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>-0.001673615682944627</v>
+        <v>-0.001535002909400116</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.00947748277909931</v>
+        <v>-0.009470677626827103</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.01002837227313489</v>
+        <v>-0.0104784726111389</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.009413965912558636</v>
+        <v>-0.009410701144428045</v>
       </c>
       <c r="J17" t="n">
-        <v>0.01309544051578936</v>
+        <v>0.02217066472651216</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.003404443624177744</v>
+        <v>-0.003417342568693702</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.003404443624177744</v>
+        <v>-0.003417342568693702</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.003404443624177744</v>
+        <v>-0.003417342568693702</v>
       </c>
       <c r="P17" t="n">
-        <v>0.002472568418902736</v>
+        <v>0.002472059330882373</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.003054677594187103</v>
+        <v>-0.003061271834450873</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.003054677594187103</v>
+        <v>-0.003061271834450873</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -1648,46 +1648,46 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.01079580110383204</v>
+        <v>-0.01050978483639139</v>
       </c>
       <c r="D18" t="n">
         <v>1.123824044952962e-05</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>-0.006863862034554481</v>
+        <v>-0.007231256449250257</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.006181653463266138</v>
+        <v>-0.006180894583235783</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0009357823094312921</v>
+        <v>0.001794827975793119</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.006111397588455902</v>
+        <v>-0.006105130900205235</v>
       </c>
       <c r="J18" t="n">
-        <v>0.01811681354576014</v>
+        <v>0.009853945266474828</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.01753561980542479</v>
+        <v>-0.01753253033330121</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.01753561980542479</v>
+        <v>-0.01753253033330121</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.01753561980542479</v>
+        <v>-0.01753253033330121</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.00949046303561852</v>
+        <v>-0.009489838171593525</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.01720851083234043</v>
+        <v>-0.01720934459237378</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.01720851083234043</v>
+        <v>-0.01720934459237378</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -1715,46 +1715,46 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.01489478680379147</v>
+        <v>0.01451281603651264</v>
       </c>
       <c r="D19" t="n">
         <v>0.005544996989799878</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0.01582147445685897</v>
+        <v>0.01596993558279742</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01463873597754944</v>
+        <v>0.01463981040959242</v>
       </c>
       <c r="H19" t="n">
-        <v>0.001187082767483311</v>
+        <v>0.0005128939405157576</v>
       </c>
       <c r="I19" t="n">
-        <v>0.01461244935249797</v>
+        <v>0.01460855040834201</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.02255692366241218</v>
+        <v>-0.00185630802736403</v>
       </c>
       <c r="K19" t="n">
-        <v>0.004885644099425763</v>
+        <v>0.004881343875253755</v>
       </c>
       <c r="L19" t="n">
-        <v>0.004885644099425763</v>
+        <v>0.004881343875253755</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>0.004885644099425763</v>
+        <v>0.004881343875253755</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.00150449526017981</v>
+        <v>-0.001506079932243197</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.004245403753816149</v>
+        <v>0.004264372490574899</v>
       </c>
       <c r="R19" t="n">
-        <v>0.004245403753816149</v>
+        <v>0.004264372490574899</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -1782,46 +1782,46 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.01304478983379159</v>
+        <v>-0.0130072726482909</v>
       </c>
       <c r="D20" t="n">
         <v>-0.0007818678072747121</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>-0.001487210843488433</v>
+        <v>-0.001272394898895796</v>
       </c>
       <c r="G20" t="n">
-        <v>0.000340301101612044</v>
+        <v>0.0003402039496081579</v>
       </c>
       <c r="H20" t="n">
-        <v>0.00299039349561574</v>
+        <v>0.002682344363293774</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0004238591209543648</v>
+        <v>0.0004260121130404845</v>
       </c>
       <c r="J20" t="n">
-        <v>0.004983708866629796</v>
+        <v>-0.0170249013393125</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.01586996194679847</v>
+        <v>-0.01587805205912208</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.01586996194679847</v>
+        <v>-0.01587805205912208</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>-0.01586996194679847</v>
+        <v>-0.01587805205912208</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.008952486406099455</v>
+        <v>-0.008954255494170218</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.01523008918520357</v>
+        <v>-0.01523813705752548</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.01523008918520357</v>
+        <v>-0.01523813705752548</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -1845,46 +1845,46 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.02406885283475411</v>
+        <v>-0.02364617614584704</v>
       </c>
       <c r="D21" t="n">
         <v>0.002703635724145429</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>0.01935088771803551</v>
+        <v>0.01924752163390086</v>
       </c>
       <c r="G21" t="n">
-        <v>0.01822441685697667</v>
+        <v>0.01822039320881573</v>
       </c>
       <c r="H21" t="n">
-        <v>0.006605646408225856</v>
+        <v>0.007110738620429544</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0179326151493046</v>
+        <v>0.01793340801333632</v>
       </c>
       <c r="J21" t="n">
-        <v>0.009024643304414874</v>
+        <v>0.009888705880453945</v>
       </c>
       <c r="K21" t="n">
-        <v>0.009950289518011579</v>
+        <v>0.009969521390780854</v>
       </c>
       <c r="L21" t="n">
-        <v>0.009950289518011579</v>
+        <v>0.009969521390780854</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0.009950289518011579</v>
+        <v>0.009969521390780854</v>
       </c>
       <c r="P21" t="n">
-        <v>0.001612530784501231</v>
+        <v>0.001609194400367776</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.009133109549324381</v>
+        <v>0.009145103693804148</v>
       </c>
       <c r="R21" t="n">
-        <v>0.009133109549324381</v>
+        <v>0.009145103693804148</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -1908,46 +1908,46 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.02979840051993602</v>
+        <v>-0.02952673174106926</v>
       </c>
       <c r="D22" t="n">
         <v>-0.007685123731404949</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>-0.01547446535497861</v>
+        <v>-0.01527155360286214</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.009003568584142741</v>
+        <v>-0.009002664264106569</v>
       </c>
       <c r="H22" t="n">
-        <v>0.01293372186134887</v>
+        <v>0.0127147375005895</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.009188743087549722</v>
+        <v>-0.009189696559587861</v>
       </c>
       <c r="J22" t="n">
-        <v>0.01215688690766466</v>
+        <v>0.003210977927182304</v>
       </c>
       <c r="K22" t="n">
-        <v>0.002083030931321237</v>
+        <v>0.002099995667999826</v>
       </c>
       <c r="L22" t="n">
-        <v>0.002083030931321237</v>
+        <v>0.002099995667999826</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.002083030931321237</v>
+        <v>0.002099995667999826</v>
       </c>
       <c r="P22" t="n">
-        <v>0.007236263425450537</v>
+        <v>0.007236529825461192</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.002269215354768614</v>
+        <v>0.002265104154604166</v>
       </c>
       <c r="R22" t="n">
-        <v>0.002269215354768614</v>
+        <v>0.002265104154604166</v>
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
@@ -1971,46 +1971,46 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.001658177538327101</v>
+        <v>0.001957645134305805</v>
       </c>
       <c r="D23" t="n">
         <v>-0.001372140150885606</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>-0.001804323624172945</v>
+        <v>-0.002050627474025099</v>
       </c>
       <c r="G23" t="n">
-        <v>0.003535517709420708</v>
+        <v>0.003535035981401439</v>
       </c>
       <c r="H23" t="n">
-        <v>0.001598797215951888</v>
+        <v>0.002474883458995338</v>
       </c>
       <c r="I23" t="n">
-        <v>0.003463363050534521</v>
+        <v>0.003462032874481314</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01822706221659564</v>
+        <v>0.009523365106922345</v>
       </c>
       <c r="K23" t="n">
-        <v>0.007247328193893126</v>
+        <v>0.007243646593745863</v>
       </c>
       <c r="L23" t="n">
-        <v>0.007247328193893126</v>
+        <v>0.007243646593745863</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>0.007247328193893126</v>
+        <v>0.007243646593745863</v>
       </c>
       <c r="P23" t="n">
-        <v>0.007226590177063607</v>
+        <v>0.007230679297227172</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.007130669373226775</v>
+        <v>0.007132603293304131</v>
       </c>
       <c r="R23" t="n">
-        <v>0.007130669373226775</v>
+        <v>0.007132603293304131</v>
       </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
@@ -2038,46 +2038,46 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.02329348384373935</v>
+        <v>-0.02295857621434304</v>
       </c>
       <c r="D24" t="n">
         <v>0.01651558885262355</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>0.005120454732818189</v>
+        <v>0.005183313519332541</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01320030888001236</v>
+        <v>0.01320048456001938</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02138318667932746</v>
+        <v>0.0212871452034858</v>
       </c>
       <c r="I24" t="n">
-        <v>0.01332821851712874</v>
+        <v>0.01332495374899815</v>
       </c>
       <c r="J24" t="n">
-        <v>0.03298953944641232</v>
+        <v>-0.01615954580556087</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.005299281907971276</v>
+        <v>-0.005293945363757813</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.005299281907971276</v>
+        <v>-0.005293945363757813</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>-0.005299281907971276</v>
+        <v>-0.005293945363757813</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.009435208985408358</v>
+        <v>-0.009431745593269822</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.005419061112762444</v>
+        <v>-0.005409388152375526</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.005419061112762444</v>
+        <v>-0.005409388152375526</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -2101,46 +2101,46 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.01058492269539691</v>
+        <v>-0.01082286312091452</v>
       </c>
       <c r="D25" t="n">
         <v>-0.02022354388094175</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>-0.0003974210078968403</v>
+        <v>-0.0007422615656904625</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.005952787630111505</v>
+        <v>-0.005953189486127578</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.0148964200518568</v>
+        <v>-0.01361732032069281</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.006019732848789313</v>
+        <v>-0.006024482736979309</v>
       </c>
       <c r="J25" t="n">
-        <v>0.01613827558543973</v>
+        <v>-0.00752563986366575</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.001420953272838131</v>
+        <v>-0.001426840281073611</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.001420953272838131</v>
+        <v>-0.001426840281073611</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>-0.001420953272838131</v>
+        <v>-0.001426840281073611</v>
       </c>
       <c r="P25" t="n">
-        <v>0.0008184400647376026</v>
+        <v>0.0008193361287734451</v>
       </c>
       <c r="Q25" t="n">
-        <v>-0.00100427399217096</v>
+        <v>-0.001010676904427076</v>
       </c>
       <c r="R25" t="n">
-        <v>-0.00100427399217096</v>
+        <v>-0.001010676904427076</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -2168,46 +2168,46 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.01406782971471319</v>
+        <v>0.01419598779983951</v>
       </c>
       <c r="D26" t="n">
         <v>-0.01490230658009226</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>-0.00490661126826445</v>
+        <v>-0.005162550158502006</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.01217557795902312</v>
+        <v>-0.01217381693495268</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.02671977985279119</v>
+        <v>-0.02583780381751215</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.01197286204691448</v>
+        <v>-0.01197669436706778</v>
       </c>
       <c r="J26" t="n">
-        <v>0.002513406420174452</v>
+        <v>0.02075481503199147</v>
       </c>
       <c r="K26" t="n">
-        <v>0.02341370599254824</v>
+        <v>0.02339740327189613</v>
       </c>
       <c r="L26" t="n">
-        <v>0.02341370599254824</v>
+        <v>0.02339740327189613</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>0.02341370599254824</v>
+        <v>0.02339740327189613</v>
       </c>
       <c r="P26" t="n">
-        <v>0.02464453164178126</v>
+        <v>0.0246451976898079</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.02383228732129149</v>
+        <v>0.02383049202521968</v>
       </c>
       <c r="R26" t="n">
-        <v>0.02383228732129149</v>
+        <v>0.02383049202521968</v>
       </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
@@ -2231,46 +2231,46 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.006530090853203633</v>
+        <v>0.007133530941341238</v>
       </c>
       <c r="D27" t="n">
         <v>0.01960177316807092</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>0.01741712085668483</v>
+        <v>0.01721078795243152</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01557557985502319</v>
+        <v>0.01557929908717196</v>
       </c>
       <c r="H27" t="n">
-        <v>0.008336320557452821</v>
+        <v>0.009237486513499458</v>
       </c>
       <c r="I27" t="n">
-        <v>0.01530699594027984</v>
+        <v>0.01530807277232291</v>
       </c>
       <c r="J27" t="n">
-        <v>0.007932186981751981</v>
+        <v>-0.00224691277604614</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.02260214692008587</v>
+        <v>-0.02259794307991772</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.02260214692008587</v>
+        <v>-0.02259794307991772</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-0.02260214692008587</v>
+        <v>-0.02259794307991772</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.02690461134818445</v>
+        <v>-0.02690492958819718</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.02379751151190046</v>
+        <v>-0.02376893787875751</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.02379751151190046</v>
+        <v>-0.02376893787875751</v>
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
@@ -2298,46 +2298,46 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.0132205900328236</v>
+        <v>0.01287512825900513</v>
       </c>
       <c r="D28" t="n">
         <v>0.01176916271076651</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>0.03305523108220924</v>
+        <v>0.03251121749244869</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02653274112530964</v>
+        <v>0.02653272202130888</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.01178896069555843</v>
+        <v>-0.01038889347155574</v>
       </c>
       <c r="I28" t="n">
-        <v>0.02640052118402084</v>
+        <v>0.02639951193598047</v>
       </c>
       <c r="J28" t="n">
-        <v>0.0243887700831779</v>
+        <v>0.0006902726904724974</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.001224893136995725</v>
+        <v>-0.001212469776498791</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.001224893136995725</v>
+        <v>-0.001212469776498791</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.001224893136995725</v>
+        <v>-0.001212469776498791</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.01568703653148146</v>
+        <v>-0.01568794459551778</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.00261307776852311</v>
+        <v>-0.002582062375282494</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.00261307776852311</v>
+        <v>-0.002582062375282494</v>
       </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
@@ -2365,46 +2365,46 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.005116735404669416</v>
+        <v>0.005465404538616181</v>
       </c>
       <c r="D29" t="n">
         <v>-0.01346903641076145</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>-0.0167711300148452</v>
+        <v>-0.01664815420192617</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.02121814673672587</v>
+        <v>-0.02122227704089108</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.01634871607794864</v>
+        <v>-0.0162852625714105</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.02119111380764455</v>
+        <v>-0.02118560916742437</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.0008650728058904444</v>
+        <v>-0.002910759130589568</v>
       </c>
       <c r="K29" t="n">
-        <v>0.02038781236751249</v>
+        <v>0.02036664801466592</v>
       </c>
       <c r="L29" t="n">
-        <v>0.02038781236751249</v>
+        <v>0.02036664801466592</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>0.02038781236751249</v>
+        <v>0.02036664801466592</v>
       </c>
       <c r="P29" t="n">
-        <v>0.02862204863288194</v>
+        <v>0.02862029701681188</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.02164319356972774</v>
+        <v>0.02160576182423047</v>
       </c>
       <c r="R29" t="n">
-        <v>0.02164319356972774</v>
+        <v>0.02160576182423047</v>
       </c>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
@@ -2432,46 +2432,46 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.02277520574300822</v>
+        <v>-0.02302936556117462</v>
       </c>
       <c r="D30" t="n">
         <v>-0.02053317413332696</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>-0.01564689019387561</v>
+        <v>-0.01543973274558931</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.0203086676603467</v>
+        <v>-0.02030884910035396</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.02038831492753259</v>
+        <v>-0.02095646464625858</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.01999129961565198</v>
+        <v>-0.01999433868777355</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.01562967343549799</v>
+        <v>0.01939671918122654</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0261552126622085</v>
+        <v>0.02614809291792371</v>
       </c>
       <c r="L30" t="n">
-        <v>0.0261552126622085</v>
+        <v>0.02614809291792371</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>0.0261552126622085</v>
+        <v>0.02614809291792371</v>
       </c>
       <c r="P30" t="n">
-        <v>0.0301511575260463</v>
+        <v>0.03015261883810475</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.02698308587932343</v>
+        <v>0.02697630415105217</v>
       </c>
       <c r="R30" t="n">
-        <v>0.02698308587932343</v>
+        <v>0.02697630415105217</v>
       </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
@@ -2499,46 +2499,46 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.001160504398420176</v>
+        <v>-0.001214912592596503</v>
       </c>
       <c r="D31" t="n">
         <v>-0.002391382367655294</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>0.007411642472465697</v>
+        <v>0.007305746596229863</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01309077076363083</v>
+        <v>0.01309103533964141</v>
       </c>
       <c r="H31" t="n">
-        <v>0.01535019162200766</v>
+        <v>0.01528675241947009</v>
       </c>
       <c r="I31" t="n">
-        <v>0.01309952932398117</v>
+        <v>0.01309746436389857</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.02339965752841897</v>
+        <v>0.01855897731537051</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.009856782154271285</v>
+        <v>-0.009851901514076059</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.009856782154271285</v>
+        <v>-0.009851901514076059</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.009856782154271285</v>
+        <v>-0.009851901514076059</v>
       </c>
       <c r="P31" t="n">
-        <v>-0.01195964140638566</v>
+        <v>-0.01195953974238159</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.01008477717139108</v>
+        <v>-0.01007417550696702</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.01008477717139108</v>
+        <v>-0.01007417550696702</v>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
@@ -2566,46 +2566,46 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-0.002703026892121075</v>
+        <v>-0.002753270030130801</v>
       </c>
       <c r="D32" t="n">
         <v>-0.001273986386959456</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>0.003664351826574073</v>
+        <v>0.003660464690418587</v>
       </c>
       <c r="G32" t="n">
-        <v>0.002101736244069449</v>
+        <v>0.002098619315944772</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.006463727586549102</v>
+        <v>-0.006531707493268299</v>
       </c>
       <c r="I32" t="n">
-        <v>0.002181935607277424</v>
+        <v>0.002184631959385278</v>
       </c>
       <c r="J32" t="n">
-        <v>0.002686926968905323</v>
+        <v>-0.01722698912975891</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0009779361991174478</v>
+        <v>0.0009818671112746843</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0009779361991174478</v>
+        <v>0.0009818671112746843</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>0.0009779361991174478</v>
+        <v>0.0009818671112746843</v>
       </c>
       <c r="P32" t="n">
-        <v>0.002621674280866971</v>
+        <v>0.002623267880930715</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.0007598308143932324</v>
+        <v>0.0007635674225426968</v>
       </c>
       <c r="R32" t="n">
-        <v>0.0007598308143932324</v>
+        <v>0.0007635674225426968</v>
       </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
@@ -2633,46 +2633,46 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.005380277495211099</v>
+        <v>-0.005091689483667579</v>
       </c>
       <c r="D33" t="n">
         <v>-0.003106481884259275</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>0.006393684831747392</v>
+        <v>0.006007470480298819</v>
       </c>
       <c r="G33" t="n">
-        <v>0.001896060939842437</v>
+        <v>0.001896694443867777</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.00685405976216239</v>
+        <v>-0.006041034097641364</v>
       </c>
       <c r="I33" t="n">
-        <v>0.002008212944328517</v>
+        <v>0.002008726640349065</v>
       </c>
       <c r="J33" t="n">
-        <v>0.02027661082638242</v>
+        <v>-0.006245130790509308</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.00941764156070566</v>
+        <v>-0.009416572120662884</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.00941764156070566</v>
+        <v>-0.009416572120662884</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>-0.00941764156070566</v>
+        <v>-0.009416572120662884</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.01491103038844121</v>
+        <v>-0.01491292629251705</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.01004795924991837</v>
+        <v>-0.01003373819334953</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.01004795924991837</v>
+        <v>-0.01003373819334953</v>
       </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
@@ -2700,46 +2700,46 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.004701084956043397</v>
+        <v>0.004613064376522574</v>
       </c>
       <c r="D34" t="n">
         <v>0.002479635075185403</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>0.01354547986981919</v>
+        <v>0.01384288528971541</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0128617875224715</v>
+        <v>0.01286356313854252</v>
       </c>
       <c r="H34" t="n">
-        <v>0.006741715853668633</v>
+        <v>0.006014563920582556</v>
       </c>
       <c r="I34" t="n">
-        <v>0.01291435664457426</v>
+        <v>0.01291468093258723</v>
       </c>
       <c r="J34" t="n">
-        <v>0.005875111561014671</v>
+        <v>-0.01959765445530503</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01586664821866593</v>
+        <v>0.01587386079495443</v>
       </c>
       <c r="L34" t="n">
-        <v>0.01586664821866593</v>
+        <v>0.01587386079495443</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>0.01586664821866593</v>
+        <v>0.01587386079495443</v>
       </c>
       <c r="P34" t="n">
-        <v>0.001772511526900461</v>
+        <v>0.001770624070824963</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.01486564389062575</v>
+        <v>0.0148866274754651</v>
       </c>
       <c r="R34" t="n">
-        <v>0.01486564389062575</v>
+        <v>0.0148866274754651</v>
       </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
@@ -2767,46 +2767,46 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.01550356314814252</v>
+        <v>-0.01546540813861632</v>
       </c>
       <c r="D35" t="n">
         <v>0.007347835109913403</v>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
-        <v>-0.003360366950414678</v>
+        <v>-0.003571419886856795</v>
       </c>
       <c r="G35" t="n">
-        <v>0.001238096593523863</v>
+        <v>0.001239669841586793</v>
       </c>
       <c r="H35" t="n">
-        <v>0.007503951756158069</v>
+        <v>0.007796640695865626</v>
       </c>
       <c r="I35" t="n">
-        <v>0.001068125706725028</v>
+        <v>0.001071938154877526</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.01773635998258703</v>
+        <v>-0.02293361543529613</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.01054295811771832</v>
+        <v>-0.01053959619758385</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.01054295811771832</v>
+        <v>-0.01053959619758385</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>-0.01054295811771832</v>
+        <v>-0.01053959619758385</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.005926812621072504</v>
+        <v>-0.005929022253160889</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.01043680371347215</v>
+        <v>-0.01043539779341591</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.01043680371347215</v>
+        <v>-0.01043539779341591</v>
       </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
@@ -2834,46 +2834,46 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.02432562903702516</v>
+        <v>-0.02411534544461381</v>
       </c>
       <c r="D36" t="n">
         <v>-0.005466936218677448</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>0.001642986305719452</v>
+        <v>0.001786294151451766</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0008755103390204134</v>
+        <v>0.0008720476188819045</v>
       </c>
       <c r="H36" t="n">
-        <v>0.001102200812088032</v>
+        <v>0.0004182676967307078</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0009113484844539394</v>
+        <v>0.0009082205163288206</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0240747876394992</v>
+        <v>0.005141694380141208</v>
       </c>
       <c r="K36" t="n">
-        <v>0.001646594849863794</v>
+        <v>0.001642024673680987</v>
       </c>
       <c r="L36" t="n">
-        <v>0.001646594849863794</v>
+        <v>0.001642024673680987</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>0.001646594849863794</v>
+        <v>0.001642024673680987</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0006253346170133846</v>
+        <v>0.0006281669051266762</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.001687245859489834</v>
+        <v>0.001686587299463492</v>
       </c>
       <c r="R36" t="n">
-        <v>0.001687245859489834</v>
+        <v>0.001686587299463492</v>
       </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
@@ -2901,46 +2901,46 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.006738285101531403</v>
+        <v>0.006192028567681141</v>
       </c>
       <c r="D37" t="n">
         <v>0.01341683295267332</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>0.007585475727419028</v>
+        <v>0.007506448620257943</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01621331776853271</v>
+        <v>0.01620987972039518</v>
       </c>
       <c r="H37" t="n">
-        <v>0.01759075980763039</v>
+        <v>0.01774623603784944</v>
       </c>
       <c r="I37" t="n">
-        <v>0.01612718397308736</v>
+        <v>0.01612340445293618</v>
       </c>
       <c r="J37" t="n">
-        <v>0.02171840014874861</v>
+        <v>-0.001911049097291001</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.02635575215823008</v>
+        <v>-0.02636290799851632</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.02635575215823008</v>
+        <v>-0.02636290799851632</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.02635575215823008</v>
+        <v>-0.02636290799851632</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.02463861784954471</v>
+        <v>-0.02463688264947531</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.02656828474273139</v>
+        <v>-0.02657315539892621</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.02656828474273139</v>
+        <v>-0.02657315539892621</v>
       </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
@@ -2968,46 +2968,46 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.0131242425089697</v>
+        <v>0.01301542765661711</v>
       </c>
       <c r="D38" t="n">
         <v>0.02909218925968757</v>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>0.003514339820573592</v>
+        <v>0.003802690904107636</v>
       </c>
       <c r="G38" t="n">
-        <v>0.00702758831310353</v>
+        <v>0.007032090617283624</v>
       </c>
       <c r="H38" t="n">
-        <v>0.01139832890393315</v>
+        <v>0.01084284993771399</v>
       </c>
       <c r="I38" t="n">
-        <v>0.006988223415528935</v>
+        <v>0.006990152823606112</v>
       </c>
       <c r="J38" t="n">
-        <v>0.03180076891889724</v>
+        <v>0.01796494929790066</v>
       </c>
       <c r="K38" t="n">
-        <v>0.01636106811044272</v>
+        <v>0.01635881211035248</v>
       </c>
       <c r="L38" t="n">
-        <v>0.01636106811044272</v>
+        <v>0.01635881211035248</v>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
-        <v>0.01636106811044272</v>
+        <v>0.01635881211035248</v>
       </c>
       <c r="P38" t="n">
-        <v>0.006167889558715581</v>
+        <v>0.006166452918658116</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.01571242987649719</v>
+        <v>0.01573487707739508</v>
       </c>
       <c r="R38" t="n">
-        <v>0.01571242987649719</v>
+        <v>0.01573487707739508</v>
       </c>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
@@ -3035,46 +3035,46 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.00151507849260314</v>
+        <v>0.00142821624912865</v>
       </c>
       <c r="D39" t="n">
         <v>0.009771227334849092</v>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>-0.00677386203095448</v>
+        <v>-0.006923709108948363</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.003723678772947151</v>
+        <v>-0.003730086389203455</v>
       </c>
       <c r="H39" t="n">
-        <v>0.01134341421373657</v>
+        <v>0.01193340316533613</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.00355128599805144</v>
+        <v>-0.003545384301815372</v>
       </c>
       <c r="J39" t="n">
-        <v>0.002708158901950766</v>
+        <v>-0.02244946563913866</v>
       </c>
       <c r="K39" t="n">
-        <v>0.9837618257184729</v>
+        <v>0.9838443065217721</v>
       </c>
       <c r="L39" t="n">
-        <v>0.9837618257184729</v>
+        <v>0.9838443065217721</v>
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
-        <v>0.9837618257184729</v>
+        <v>0.9838443065217721</v>
       </c>
       <c r="P39" t="n">
-        <v>0.7163593490383737</v>
+        <v>0.7163679787667191</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.9732053123042123</v>
+        <v>0.9733811086632442</v>
       </c>
       <c r="R39" t="n">
-        <v>0.9732053123042123</v>
+        <v>0.9733811086632442</v>
       </c>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>

</xml_diff>

<commit_message>
rerun simulations and enhancements to sankey
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -734,44 +734,44 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.001805844552233782</v>
+        <v>-0.00184922426596897</v>
       </c>
       <c r="D4" t="n">
         <v>0.003529454733178189</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.002584851367394054</v>
+        <v>0.00238636924745477</v>
       </c>
       <c r="G4" t="n">
-        <v>-8.859581154383245e-05</v>
+        <v>0.0003519480140779205</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>-0.0001278198771127951</v>
+        <v>-3.319564932782597e-05</v>
       </c>
       <c r="J4" t="n">
-        <v>0.03804884094020192</v>
+        <v>0.04168032677546655</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0001135041645401666</v>
+        <v>-0.0003277541891101675</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0001135041645401666</v>
+        <v>-0.0003277541891101675</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.0001135041645401666</v>
+        <v>-0.0003277541891101675</v>
       </c>
       <c r="P4" t="n">
-        <v>9.043373161734926e-05</v>
+        <v>-0.0003506251340250053</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0001097805163912206</v>
+        <v>-0.000330794125231765</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0001097805163912206</v>
+        <v>-0.000330794125231765</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -795,44 +795,44 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01691155315646212</v>
+        <v>0.01691633606865344</v>
       </c>
       <c r="D5" t="n">
         <v>0.007570266830810672</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>-0.009959291342371652</v>
+        <v>-0.009949394605975784</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.003539646573585863</v>
+        <v>-0.003523219052928762</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>-0.003626937361077494</v>
+        <v>-0.003620335632813425</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.01418937067533941</v>
+        <v>-0.01300384867918394</v>
       </c>
       <c r="K5" t="n">
-        <v>0.003590375375615015</v>
+        <v>0.003572860942914437</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003590375375615015</v>
+        <v>0.003572860942914437</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.003590375375615015</v>
+        <v>0.003572860942914437</v>
       </c>
       <c r="P5" t="n">
-        <v>0.003533651949346078</v>
+        <v>0.003517566188702647</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.003579272399170896</v>
+        <v>0.003561755374470215</v>
       </c>
       <c r="R5" t="n">
-        <v>0.003579272399170896</v>
+        <v>0.003561755374470215</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -856,44 +856,44 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2151618357744734</v>
+        <v>0.2151542118381685</v>
       </c>
       <c r="D6" t="n">
         <v>0.0108233524329341</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>-0.5638309637692385</v>
+        <v>-0.5638750636750025</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.6033493912699756</v>
+        <v>-0.6033449879417995</v>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>-0.6031652913906116</v>
+        <v>-0.6031666201266648</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0108304790441561</v>
+        <v>-0.01178114270977414</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6033727334789093</v>
+        <v>0.6033684559107382</v>
       </c>
       <c r="L6" t="n">
-        <v>0.6033727334789093</v>
+        <v>0.6033684559107382</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.6033727334789093</v>
+        <v>0.6033684559107382</v>
       </c>
       <c r="P6" t="n">
-        <v>0.6033464970618598</v>
+        <v>0.6033416494456659</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.6033669716546788</v>
+        <v>0.6033623790144951</v>
       </c>
       <c r="R6" t="n">
-        <v>0.6033669716546788</v>
+        <v>0.6033623790144951</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -917,44 +917,44 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.007264125602565023</v>
+        <v>-0.007259253218370128</v>
       </c>
       <c r="D7" t="n">
         <v>-0.004311911308476452</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>-0.001643261153730446</v>
+        <v>-0.001692830371713215</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.007191420479656818</v>
+        <v>-0.007264447394577896</v>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>-0.00714604454184178</v>
+        <v>-0.007155901150236045</v>
       </c>
       <c r="J7" t="n">
-        <v>0.009673926209092874</v>
+        <v>0.008109601455384056</v>
       </c>
       <c r="K7" t="n">
-        <v>0.007161275614451023</v>
+        <v>0.00723402576136103</v>
       </c>
       <c r="L7" t="n">
-        <v>0.007161275614451023</v>
+        <v>0.00723402576136103</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>0.007161275614451023</v>
+        <v>0.00723402576136103</v>
       </c>
       <c r="P7" t="n">
-        <v>0.007187802047512081</v>
+        <v>0.007260546530421861</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.007163600350544013</v>
+        <v>0.007236749377469973</v>
       </c>
       <c r="R7" t="n">
-        <v>0.007163600350544013</v>
+        <v>0.007236749377469973</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -978,44 +978,44 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.2132256870570274</v>
+        <v>0.2132344790253791</v>
       </c>
       <c r="D8" t="n">
         <v>0.9999999999999999</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>0.7203864281434571</v>
+        <v>0.7203630320785213</v>
       </c>
       <c r="G8" t="n">
-        <v>0.7774157845366312</v>
+        <v>0.7774027243121089</v>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>0.7776358569614341</v>
+        <v>0.7776331572493262</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.01409187221380823</v>
+        <v>-0.01565270889423975</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.7773991385199656</v>
+        <v>-0.7773860245354408</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.7773991385199656</v>
+        <v>-0.7773860245354408</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>-0.7773991385199656</v>
+        <v>-0.7773860245354408</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.7774175510327019</v>
+        <v>-0.7774047565361901</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.7774042726001709</v>
+        <v>-0.7773914105196563</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.7774042726001709</v>
+        <v>-0.7773914105196563</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1043,44 +1043,44 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9187919191516767</v>
+        <v>0.9187915719196627</v>
       </c>
       <c r="D9" t="n">
         <v>0.01752971628518865</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.005917023116680925</v>
+        <v>0.006087433587497343</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00732586051703442</v>
+        <v>0.007281402339256092</v>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>0.007337838821513552</v>
+        <v>0.007332860549314421</v>
       </c>
       <c r="J9" t="n">
-        <v>0.01093697962726478</v>
+        <v>0.01042116651380094</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.007312048324481932</v>
+        <v>-0.007267442498697699</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.007312048324481932</v>
+        <v>-0.007267442498697699</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>-0.007312048324481932</v>
+        <v>-0.007267442498697699</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.007327155173086206</v>
+        <v>-0.007282979043319161</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.007314350500574019</v>
+        <v>-0.007269743426789737</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.007314350500574019</v>
+        <v>-0.007269743426789737</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1108,44 +1108,44 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.007912075516483019</v>
+        <v>0.007906585276263409</v>
       </c>
       <c r="D10" t="n">
         <v>0.003197859583914383</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>-0.01199890214395609</v>
+        <v>-0.01216646333465853</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.01145673309826932</v>
+        <v>-0.01137640077505603</v>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>-0.01130340976413639</v>
+        <v>-0.01128572598742904</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.005768287771149647</v>
+        <v>-0.004980844051904113</v>
       </c>
       <c r="K10" t="n">
-        <v>0.01149289725971589</v>
+        <v>0.011411824968473</v>
       </c>
       <c r="L10" t="n">
-        <v>0.01149289725971589</v>
+        <v>0.011411824968473</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>0.01149289725971589</v>
+        <v>0.011411824968473</v>
       </c>
       <c r="P10" t="n">
-        <v>0.01144733402589336</v>
+        <v>0.01136712832668513</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.01149307399572296</v>
+        <v>0.01141177658447106</v>
       </c>
       <c r="R10" t="n">
-        <v>0.01149307399572296</v>
+        <v>0.01141177658447106</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -1173,44 +1173,44 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.005134295821371832</v>
+        <v>-0.005128774573150982</v>
       </c>
       <c r="D11" t="n">
         <v>0.007627171025086841</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.008201244904049795</v>
+        <v>0.008106874404274975</v>
       </c>
       <c r="G11" t="n">
-        <v>0.009254492338179694</v>
+        <v>0.009174046062961842</v>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>0.009299371667974865</v>
+        <v>0.009280396883215873</v>
       </c>
       <c r="J11" t="n">
-        <v>0.01433523403938443</v>
+        <v>0.01358975910455809</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.009211035440441417</v>
+        <v>-0.009127408877096354</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.009211035440441417</v>
+        <v>-0.009127408877096354</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.009211035440441417</v>
+        <v>-0.009127408877096354</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.00925607576224303</v>
+        <v>-0.009175120495004819</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.009223396592935864</v>
+        <v>-0.009141106157644244</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.009223396592935864</v>
+        <v>-0.009141106157644244</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -1238,44 +1238,44 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.01762512924900516</v>
+        <v>0.01762530992101239</v>
       </c>
       <c r="D12" t="n">
         <v>-0.004942293317691732</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>-0.007052732922109316</v>
+        <v>-0.007062323130492924</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0002949775797991031</v>
+        <v>0.0002926671477066859</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>0.0003650690066027602</v>
+        <v>0.0003588559823542392</v>
       </c>
       <c r="J12" t="n">
-        <v>0.01639256850164576</v>
+        <v>0.01692155358897093</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0002308894172355766</v>
+        <v>-0.0002276041051041642</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.0002308894172355766</v>
+        <v>-0.0002276041051041642</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>-0.0002308894172355766</v>
+        <v>-0.0002276041051041642</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0002985863159434526</v>
+        <v>-0.0002961436918457476</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0002596739623869585</v>
+        <v>-0.0002573568102942724</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0002596739623869585</v>
+        <v>-0.0002573568102942724</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1299,44 +1299,44 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.2511363084134523</v>
+        <v>-0.2511372571814902</v>
       </c>
       <c r="D13" t="n">
         <v>-0.002908193588327743</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>-0.007768626358745053</v>
+        <v>-0.007567986830719473</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.002082072659282906</v>
+        <v>-0.002080322867212915</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>-0.002026543377061735</v>
+        <v>-0.002023955888958235</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.009044453388408291</v>
+        <v>-0.009865042897565256</v>
       </c>
       <c r="K13" t="n">
-        <v>0.002131954357278174</v>
+        <v>0.002128789429151577</v>
       </c>
       <c r="L13" t="n">
-        <v>0.002131954357278174</v>
+        <v>0.002128789429151577</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>0.002131954357278174</v>
+        <v>0.002128789429151577</v>
       </c>
       <c r="P13" t="n">
-        <v>0.002065505554620222</v>
+        <v>0.002063832946553318</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.002112601236504049</v>
+        <v>0.00211058350842334</v>
       </c>
       <c r="R13" t="n">
-        <v>0.002112601236504049</v>
+        <v>0.00211058350842334</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -1364,44 +1364,44 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.01189032316361292</v>
+        <v>-0.01188200226728009</v>
       </c>
       <c r="D14" t="n">
         <v>-0.03053229702929188</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>-0.02387686386707455</v>
+        <v>-0.02395718899028756</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.02224837653793506</v>
+        <v>-0.02228456873138275</v>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>-0.02258418128736725</v>
+        <v>-0.02259708320788333</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.001335949397307528</v>
+        <v>-0.002738659257197447</v>
       </c>
       <c r="K14" t="n">
-        <v>0.02223925922557037</v>
+        <v>0.02227615202704608</v>
       </c>
       <c r="L14" t="n">
-        <v>0.02223925922557037</v>
+        <v>0.02227615202704608</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>0.02223925922557037</v>
+        <v>0.02227615202704608</v>
       </c>
       <c r="P14" t="n">
-        <v>0.02224349848973994</v>
+        <v>0.02228003810720152</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.02223330914533237</v>
+        <v>0.02227058114682325</v>
       </c>
       <c r="R14" t="n">
-        <v>0.02223330914533237</v>
+        <v>0.02227058114682325</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -1429,44 +1429,44 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.002689273163570926</v>
+        <v>0.002682374699294988</v>
       </c>
       <c r="D15" t="n">
         <v>0.002746113805844552</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>0.01083661809746472</v>
+        <v>0.01081864900874596</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01123067372922695</v>
+        <v>0.0112815601632624</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>0.01109396233175849</v>
+        <v>0.01110893132435725</v>
       </c>
       <c r="J15" t="n">
-        <v>0.002583796122807539</v>
+        <v>0.002619608252733698</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.01124325654573026</v>
+        <v>-0.01129223190768927</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.01124325654573026</v>
+        <v>-0.01129223190768927</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.01124325654573026</v>
+        <v>-0.01129223190768927</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.01123492460939698</v>
+        <v>-0.01128591808343672</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.01124569350582774</v>
+        <v>-0.01129501533180061</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.01124569350582774</v>
+        <v>-0.01129501533180061</v>
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
@@ -1494,44 +1494,44 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.007294307139772285</v>
+        <v>-0.007288015875520634</v>
       </c>
       <c r="D16" t="n">
         <v>-0.004229653321186132</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>-0.01056880410275216</v>
+        <v>-0.01049203357168134</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.01749906165996246</v>
+        <v>-0.01757174806286992</v>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
-        <v>-0.01747784162711366</v>
+        <v>-0.01749576329183053</v>
       </c>
       <c r="J16" t="n">
-        <v>0.02468550089944768</v>
+        <v>0.0245645605978325</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01749021285960851</v>
+        <v>0.01756185401447416</v>
       </c>
       <c r="L16" t="n">
-        <v>0.01749021285960851</v>
+        <v>0.01756185401447416</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.01749021285960851</v>
+        <v>0.01756185401447416</v>
       </c>
       <c r="P16" t="n">
-        <v>0.01749700956388038</v>
+        <v>0.01756979100679164</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.01749587810783512</v>
+        <v>0.01756769398270776</v>
       </c>
       <c r="R16" t="n">
-        <v>0.01749587810783512</v>
+        <v>0.01756769398270776</v>
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -1559,44 +1559,44 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.01344977381799095</v>
+        <v>-0.01344857976994319</v>
       </c>
       <c r="D17" t="n">
         <v>0.001087392523495701</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>-0.001738698693547947</v>
+        <v>-0.001548514237940569</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.009470441562817662</v>
+        <v>-0.009480109243204369</v>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>-0.009413533144541325</v>
+        <v>-0.00941377180055087</v>
       </c>
       <c r="J17" t="n">
-        <v>0.01040087597833847</v>
+        <v>0.008501954525064137</v>
       </c>
       <c r="K17" t="n">
-        <v>0.009428257433130296</v>
+        <v>0.009437853209514128</v>
       </c>
       <c r="L17" t="n">
-        <v>0.009428257433130296</v>
+        <v>0.009437853209514128</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>0.009428257433130296</v>
+        <v>0.009437853209514128</v>
       </c>
       <c r="P17" t="n">
-        <v>0.009488397115535884</v>
+        <v>0.009497478715899147</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.009450099642003985</v>
+        <v>0.009460304634412183</v>
       </c>
       <c r="R17" t="n">
-        <v>0.009450099642003985</v>
+        <v>0.009460304634412183</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -1620,44 +1620,44 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.01050909872436395</v>
+        <v>-0.01051422358856894</v>
       </c>
       <c r="D18" t="n">
         <v>1.123824044952962e-05</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>-0.006786097999443918</v>
+        <v>-0.006879256595170263</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.006182345239293809</v>
+        <v>-0.006111393652455745</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>-0.006112113652484546</v>
+        <v>-0.006093746931749876</v>
       </c>
       <c r="J18" t="n">
-        <v>0.01460986520720924</v>
+        <v>0.01563704923444978</v>
       </c>
       <c r="K18" t="n">
-        <v>0.006164756886590275</v>
+        <v>0.006093843315753731</v>
       </c>
       <c r="L18" t="n">
-        <v>0.006164756886590275</v>
+        <v>0.006093843315753731</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>0.006164756886590275</v>
+        <v>0.006093843315753731</v>
       </c>
       <c r="P18" t="n">
-        <v>0.006188201719528068</v>
+        <v>0.006117555892702235</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.006164530422581217</v>
+        <v>0.006093580371743215</v>
       </c>
       <c r="R18" t="n">
-        <v>0.006164530422581217</v>
+        <v>0.006093580371743215</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -1685,44 +1685,44 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0145118475884739</v>
+        <v>0.014511950020478</v>
       </c>
       <c r="D19" t="n">
         <v>0.005544996989799878</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0.01582747080909883</v>
+        <v>0.01600095328003813</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01463993328959733</v>
+        <v>0.01463416042536641</v>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>0.01461174068046962</v>
+        <v>0.01461531101661244</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.02195453353925658</v>
+        <v>-0.02237638995333701</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.01459265098370604</v>
+        <v>-0.01458827415153096</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.01459265098370604</v>
+        <v>-0.01458827415153096</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>-0.01459265098370604</v>
+        <v>-0.01458827415153096</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.01464447303377892</v>
+        <v>-0.01463896474555859</v>
       </c>
       <c r="Q19" t="n">
-        <v>-0.01460914676036587</v>
+        <v>-0.01460508442420337</v>
       </c>
       <c r="R19" t="n">
-        <v>-0.01460914676036587</v>
+        <v>-0.01460508442420337</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -1750,44 +1750,44 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.01300741876029675</v>
+        <v>-0.01301575636063025</v>
       </c>
       <c r="D20" t="n">
         <v>-0.0007818678072747121</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>-0.001579809663192386</v>
+        <v>-0.001526585437063417</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0003402395656095826</v>
+        <v>0.000358218926328757</v>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>0.0004241469289658771</v>
+        <v>0.0004287831531513261</v>
       </c>
       <c r="J20" t="n">
-        <v>0.01127834758205226</v>
+        <v>0.01088337726208154</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.00035324075012963</v>
+        <v>-0.000371732174869287</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.00035324075012963</v>
+        <v>-0.000371732174869287</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>-0.00035324075012963</v>
+        <v>-0.000371732174869287</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.0003394153095766124</v>
+        <v>-0.000357072302282892</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.0003619585104783404</v>
+        <v>-0.0003807764312310571</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.0003619585104783404</v>
+        <v>-0.0003807764312310571</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -1811,44 +1811,44 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.02364736097789443</v>
+        <v>-0.02364964836998593</v>
       </c>
       <c r="D21" t="n">
         <v>0.002703635724145429</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>0.01925385427415417</v>
+        <v>0.01911232377249295</v>
       </c>
       <c r="G21" t="n">
-        <v>0.01822020888880835</v>
+        <v>0.01828667458746698</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
-        <v>0.01793291658931666</v>
+        <v>0.01794317236572689</v>
       </c>
       <c r="J21" t="n">
-        <v>0.00751791612246362</v>
+        <v>0.008357868050862539</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.01821745032869801</v>
+        <v>-0.01828548533941941</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.01821745032869801</v>
+        <v>-0.01828548533941941</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-0.01821745032869801</v>
+        <v>-0.01828548533941941</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.01822856664914266</v>
+        <v>-0.01829508889180355</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.0182104901364196</v>
+        <v>-0.01827865148314606</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.0182104901364196</v>
+        <v>-0.01827865148314606</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -1872,44 +1872,44 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.02952803302112132</v>
+        <v>-0.02953433897337356</v>
       </c>
       <c r="D22" t="n">
         <v>-0.007685123731404949</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>-0.01537544883901795</v>
+        <v>-0.01540475840819033</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.009001503720060146</v>
+        <v>-0.008950856326034252</v>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>-0.009189229903569195</v>
+        <v>-0.009178314319132573</v>
       </c>
       <c r="J22" t="n">
-        <v>0.01332662052196802</v>
+        <v>0.01411884328020478</v>
       </c>
       <c r="K22" t="n">
-        <v>0.009074662826986513</v>
+        <v>0.009025850857034032</v>
       </c>
       <c r="L22" t="n">
-        <v>0.009074662826986513</v>
+        <v>0.009025850857034032</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.009074662826986513</v>
+        <v>0.009025850857034032</v>
       </c>
       <c r="P22" t="n">
-        <v>0.0090057675602307</v>
+        <v>0.008954404198176166</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.009046668073866721</v>
+        <v>0.008997719207908766</v>
       </c>
       <c r="R22" t="n">
-        <v>0.009046668073866721</v>
+        <v>0.008997719207908766</v>
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
@@ -1933,44 +1933,44 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.001955933166237326</v>
+        <v>0.001958246574329863</v>
       </c>
       <c r="D23" t="n">
         <v>-0.001372140150885606</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>-0.001862657450506298</v>
+        <v>-0.001980266671210667</v>
       </c>
       <c r="G23" t="n">
-        <v>0.003534301485372059</v>
+        <v>0.003562988686519547</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>0.003463434282537371</v>
+        <v>0.003469011882760475</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01330033383331592</v>
+        <v>0.0141841549049263</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.003494736235789449</v>
+        <v>-0.003522202604888103</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.003494736235789449</v>
+        <v>-0.003522202604888103</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>-0.003494736235789449</v>
+        <v>-0.003522202604888103</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.003540878637635145</v>
+        <v>-0.003569571982782879</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.003499263211970528</v>
+        <v>-0.003526684749067389</v>
       </c>
       <c r="R23" t="n">
-        <v>-0.003499263211970528</v>
+        <v>-0.003526684749067389</v>
       </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
@@ -1998,44 +1998,44 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.02295922104636884</v>
+        <v>-0.02295060984602439</v>
       </c>
       <c r="D24" t="n">
         <v>0.01651558885262355</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>0.005040906825636272</v>
+        <v>0.005096766635870664</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01319956055998242</v>
+        <v>0.01313478878139155</v>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>0.01332876677315067</v>
+        <v>0.0133140150285606</v>
       </c>
       <c r="J24" t="n">
-        <v>0.03518205701313737</v>
+        <v>0.03427202253541432</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.01312913351716534</v>
+        <v>-0.01306666151466646</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.01312913351716534</v>
+        <v>-0.01306666151466646</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>-0.01312913351716534</v>
+        <v>-0.01306666151466646</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.0132008374560335</v>
+        <v>-0.01313588980543559</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.0131583176143327</v>
+        <v>-0.01309550289182011</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.0131583176143327</v>
+        <v>-0.01309550289182011</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -2059,44 +2059,44 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.01082170632086825</v>
+        <v>-0.01081784203271368</v>
       </c>
       <c r="D25" t="n">
         <v>-0.02022354388094175</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>-0.0002936761077470443</v>
+        <v>-0.0004862027714481108</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.005953951150158046</v>
+        <v>-0.005991658031666321</v>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>-0.006018913872756554</v>
+        <v>-0.006021687696867507</v>
       </c>
       <c r="J25" t="n">
-        <v>0.008089233622364066</v>
+        <v>0.009164276927549401</v>
       </c>
       <c r="K25" t="n">
-        <v>0.005918186156727445</v>
+        <v>0.005958317710332707</v>
       </c>
       <c r="L25" t="n">
-        <v>0.005918186156727445</v>
+        <v>0.005958317710332707</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.005918186156727445</v>
+        <v>0.005958317710332707</v>
       </c>
       <c r="P25" t="n">
-        <v>0.005954738926189557</v>
+        <v>0.005992211855688473</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.00593516174140647</v>
+        <v>0.005974650670986026</v>
       </c>
       <c r="R25" t="n">
-        <v>0.00593516174140647</v>
+        <v>0.005974650670986026</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -2124,44 +2124,44 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.01419539173581567</v>
+        <v>0.01420792175231687</v>
       </c>
       <c r="D26" t="n">
         <v>-0.01490230658009226</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>-0.004845749089829963</v>
+        <v>-0.004996577575863102</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.01217521277500851</v>
+        <v>-0.01225024263400971</v>
       </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>-0.01197416409496656</v>
+        <v>-0.01199469811178792</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0007612073014674436</v>
+        <v>-0.0002636530694596723</v>
       </c>
       <c r="K26" t="n">
-        <v>0.01214295216571809</v>
+        <v>0.01222116941684677</v>
       </c>
       <c r="L26" t="n">
-        <v>0.01214295216571809</v>
+        <v>0.01222116941684677</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>0.01214295216571809</v>
+        <v>0.01222116941684677</v>
       </c>
       <c r="P26" t="n">
-        <v>0.01217804093512164</v>
+        <v>0.01225386653815466</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.01215138903005556</v>
+        <v>0.01222929159317166</v>
       </c>
       <c r="R26" t="n">
-        <v>0.01215138903005556</v>
+        <v>0.01222929159317166</v>
       </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
@@ -2185,44 +2185,44 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.007133051229322048</v>
+        <v>0.007135999389439974</v>
       </c>
       <c r="D27" t="n">
         <v>0.01960177316807092</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>0.01743568716142748</v>
+        <v>0.01730088472403539</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01557812087912483</v>
+        <v>0.01552706078108243</v>
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
-        <v>0.01530606464424258</v>
+        <v>0.01529896400395856</v>
       </c>
       <c r="J27" t="n">
-        <v>0.003695611295792419</v>
+        <v>0.005790076841028518</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.01558311556732462</v>
+        <v>-0.01553181921327276</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.01558311556732462</v>
+        <v>-0.01553181921327276</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-0.01558311556732462</v>
+        <v>-0.01553181921327276</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.01557511358300454</v>
+        <v>-0.01552441799697672</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.01558157390326295</v>
+        <v>-0.01552962964518518</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.01558157390326295</v>
+        <v>-0.01552962964518518</v>
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
@@ -2250,44 +2250,44 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.01287703299508132</v>
+        <v>0.01288056838722273</v>
       </c>
       <c r="D28" t="n">
         <v>0.01176916271076651</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>0.03295749664629986</v>
+        <v>0.03283637977745519</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02653205002128199</v>
+        <v>0.0265090576363623</v>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>0.02639952422398096</v>
+        <v>0.02639508566380342</v>
       </c>
       <c r="J28" t="n">
-        <v>0.02236649073534873</v>
+        <v>0.02221156431123024</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.02659445722377829</v>
+        <v>-0.02656952880678115</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.02659445722377829</v>
+        <v>-0.02656952880678115</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.02659445722377829</v>
+        <v>-0.02656952880678115</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.02652941875717675</v>
+        <v>-0.02650646496425859</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.02657463821498553</v>
+        <v>-0.02655084586203383</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.02657463821498553</v>
+        <v>-0.02655084586203383</v>
       </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
@@ -2315,44 +2315,44 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.005465765114630604</v>
+        <v>0.005463616634544665</v>
       </c>
       <c r="D29" t="n">
         <v>-0.01346903641076145</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>-0.01678217039928681</v>
+        <v>-0.0168773302110932</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.02122148705685948</v>
+        <v>-0.02114994103799764</v>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>-0.02119142417565697</v>
+        <v>-0.02117890980715639</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.008267907483266565</v>
+        <v>-0.00649367925670323</v>
       </c>
       <c r="K29" t="n">
-        <v>0.02122401972896079</v>
+        <v>0.02115176974207078</v>
       </c>
       <c r="L29" t="n">
-        <v>0.02122401972896079</v>
+        <v>0.02115176974207078</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>0.02122401972896079</v>
+        <v>0.02115176974207078</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0212157651686306</v>
+        <v>0.02114396196575848</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.02121905556876222</v>
+        <v>0.02114788356591534</v>
       </c>
       <c r="R29" t="n">
-        <v>0.02121905556876222</v>
+        <v>0.02114788356591534</v>
       </c>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
@@ -2380,44 +2380,44 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.02303220725728829</v>
+        <v>-0.02303425580137023</v>
       </c>
       <c r="D30" t="n">
         <v>-0.02053317413332696</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>-0.01561562299262492</v>
+        <v>-0.01552161393286455</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.02030785540431421</v>
+        <v>-0.02024978164199126</v>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
-        <v>-0.01999088931163557</v>
+        <v>-0.01997610694304428</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.0182333515813707</v>
+        <v>-0.01717351359511857</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0203074299322972</v>
+        <v>0.02024713338588533</v>
       </c>
       <c r="L30" t="n">
-        <v>0.0203074299322972</v>
+        <v>0.02024713338588533</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>0.0203074299322972</v>
+        <v>0.02024713338588533</v>
       </c>
       <c r="P30" t="n">
-        <v>0.02030496282819851</v>
+        <v>0.02024675840987033</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.0203148725245949</v>
+        <v>0.020255350122214</v>
       </c>
       <c r="R30" t="n">
-        <v>0.0203148725245949</v>
+        <v>0.020255350122214</v>
       </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
@@ -2445,44 +2445,44 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.001215606960624278</v>
+        <v>-0.00121864574474583</v>
       </c>
       <c r="D31" t="n">
         <v>-0.002391382367655294</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>0.007495244939809797</v>
+        <v>0.007686476083459042</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01309010385160415</v>
+        <v>0.01309294170771767</v>
       </c>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>0.01309946049197842</v>
+        <v>0.01310757297230292</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.01464484011055036</v>
+        <v>-0.01554636619203501</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.01309484471579379</v>
+        <v>-0.01309981156399246</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.01309484471579379</v>
+        <v>-0.01309981156399246</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.01309484471579379</v>
+        <v>-0.01309981156399246</v>
       </c>
       <c r="P31" t="n">
-        <v>-0.01309820202792808</v>
+        <v>-0.01310075140403005</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.0130885200435408</v>
+        <v>-0.01309314090772563</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.0130885200435408</v>
+        <v>-0.01309314090772563</v>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
@@ -2510,44 +2510,44 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-0.002753235470129419</v>
+        <v>-0.002749313389972535</v>
       </c>
       <c r="D32" t="n">
         <v>-0.001273986386959456</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>0.003662077874483115</v>
+        <v>0.003525228621009144</v>
       </c>
       <c r="G32" t="n">
-        <v>0.002099504819980193</v>
+        <v>0.002132700277308011</v>
       </c>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>0.002182463991298559</v>
+        <v>0.002188794615551784</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.001257720554549767</v>
+        <v>-0.0008692926099525761</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.002061993586479743</v>
+        <v>-0.002097491315899652</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.002061993586479743</v>
+        <v>-0.002097491315899652</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>-0.002061993586479743</v>
+        <v>-0.002097491315899652</v>
       </c>
       <c r="P32" t="n">
-        <v>-0.002102214420088577</v>
+        <v>-0.002135499061419962</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.002079762611190504</v>
+        <v>-0.002114081076563243</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.002079762611190504</v>
+        <v>-0.002114081076563243</v>
       </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
@@ -2575,44 +2575,44 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.005093518667740746</v>
+        <v>-0.005092019531680781</v>
       </c>
       <c r="D33" t="n">
         <v>-0.003106481884259275</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>0.006309903612396144</v>
+        <v>0.006113728660549146</v>
       </c>
       <c r="G33" t="n">
-        <v>0.001896517419860697</v>
+        <v>0.001938849485553979</v>
       </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>0.00200792225631689</v>
+        <v>0.002014004720560189</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0180374348347733</v>
+        <v>0.01865297993850179</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.001897583691903347</v>
+        <v>-0.001939987565599502</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.001897583691903347</v>
+        <v>-0.001939987565599502</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>-0.001897583691903347</v>
+        <v>-0.001939987565599502</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.001899182667967307</v>
+        <v>-0.001941209549648382</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.001898629707945188</v>
+        <v>-0.001940464781618591</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.001898629707945188</v>
+        <v>-0.001940464781618591</v>
       </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
@@ -2640,44 +2640,44 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.004613594392543776</v>
+        <v>0.004612543576501742</v>
       </c>
       <c r="D34" t="n">
         <v>0.002479635075185403</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>0.01366211872248475</v>
+        <v>0.01379169213566768</v>
       </c>
       <c r="G34" t="n">
-        <v>0.01286407971456319</v>
+        <v>0.01285461113818444</v>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>0.01291478394059136</v>
+        <v>0.01291294131651765</v>
       </c>
       <c r="J34" t="n">
-        <v>0.006144753560536398</v>
+        <v>0.005417428588344622</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.01286126931445077</v>
+        <v>-0.01285070729802829</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.01286126931445077</v>
+        <v>-0.01285070729802829</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>-0.01286126931445077</v>
+        <v>-0.01285070729802829</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.0128641800345672</v>
+        <v>-0.0128547476501899</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.01285700134628005</v>
+        <v>-0.01284699190587967</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.01285700134628005</v>
+        <v>-0.01284699190587967</v>
       </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
@@ -2705,44 +2705,44 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.01546387156255486</v>
+        <v>-0.01547285025091401</v>
       </c>
       <c r="D35" t="n">
         <v>0.007347835109913403</v>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
-        <v>-0.00335594327023773</v>
+        <v>-0.003296374691854987</v>
       </c>
       <c r="G35" t="n">
-        <v>0.001238278897531156</v>
+        <v>0.001338123221524929</v>
       </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
-        <v>0.001069398954775958</v>
+        <v>0.001090265707610628</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.0132879310297701</v>
+        <v>-0.01172757725849025</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.001241942737677709</v>
+        <v>-0.001342345301693812</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.001241942737677709</v>
+        <v>-0.001342345301693812</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>-0.001241942737677709</v>
+        <v>-0.001342345301693812</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.001240326673613067</v>
+        <v>-0.00134001701360068</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.001242796081711843</v>
+        <v>-0.001343149781725991</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.001242796081711843</v>
+        <v>-0.001343149781725991</v>
       </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
@@ -2770,44 +2770,44 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.02411637869265515</v>
+        <v>-0.02411212474048499</v>
       </c>
       <c r="D36" t="n">
         <v>-0.005466936218677448</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>0.001641779489671179</v>
+        <v>0.001655633058225322</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0008730113629204544</v>
+        <v>0.0008665168666606747</v>
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
-        <v>0.0009117167404686694</v>
+        <v>0.0009083076843323072</v>
       </c>
       <c r="J36" t="n">
-        <v>0.02271529747185433</v>
+        <v>0.02109655319132765</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.0008641800345672013</v>
+        <v>-0.0008589173143566925</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.0008641800345672013</v>
+        <v>-0.0008589173143566925</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>-0.0008641800345672013</v>
+        <v>-0.0008589173143566925</v>
       </c>
       <c r="P36" t="n">
-        <v>-0.0008744127709765108</v>
+        <v>-0.0008682755867310234</v>
       </c>
       <c r="Q36" t="n">
-        <v>-0.0008797140831885631</v>
+        <v>-0.0008748648349945933</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.0008797140831885631</v>
+        <v>-0.0008748648349945933</v>
       </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
@@ -2835,44 +2835,44 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.006189497335579893</v>
+        <v>0.006196465015858601</v>
       </c>
       <c r="D37" t="n">
         <v>0.01341683295267332</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>0.007611331984453277</v>
+        <v>0.007529681293187251</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01621072807242912</v>
+        <v>0.01625210945008438</v>
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="n">
-        <v>0.01612875558915022</v>
+        <v>0.0161297850931914</v>
       </c>
       <c r="J37" t="n">
-        <v>0.01306677025327373</v>
+        <v>0.0146345010144168</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.01620907274436291</v>
+        <v>-0.01625207441008297</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.01620907274436291</v>
+        <v>-0.01625207441008297</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.01620907274436291</v>
+        <v>-0.01625207441008297</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.01621060807242432</v>
+        <v>-0.01625189921007596</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.01621809943272397</v>
+        <v>-0.0162614652264586</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.01621809943272397</v>
+        <v>-0.0162614652264586</v>
       </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
@@ -2900,44 +2900,44 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.01301658637666345</v>
+        <v>0.01301712080868483</v>
       </c>
       <c r="D38" t="n">
         <v>0.02909218925968757</v>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>0.003451901130076044</v>
+        <v>0.003423950152958006</v>
       </c>
       <c r="G38" t="n">
-        <v>0.007033299257331969</v>
+        <v>0.007033671065346842</v>
       </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="n">
-        <v>0.006988205943528237</v>
+        <v>0.006982184727287388</v>
       </c>
       <c r="J38" t="n">
-        <v>0.02826036325505277</v>
+        <v>0.02954150864266611</v>
       </c>
       <c r="K38" t="n">
-        <v>-0.007045985177839406</v>
+        <v>-0.007043530265741209</v>
       </c>
       <c r="L38" t="n">
-        <v>-0.007045985177839406</v>
+        <v>-0.007043530265741209</v>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
-        <v>-0.007045985177839406</v>
+        <v>-0.007043530265741209</v>
       </c>
       <c r="P38" t="n">
-        <v>-0.007022572696902907</v>
+        <v>-0.007023616024944641</v>
       </c>
       <c r="Q38" t="n">
-        <v>-0.007053949338157972</v>
+        <v>-0.007051709946068397</v>
       </c>
       <c r="R38" t="n">
-        <v>-0.007053949338157972</v>
+        <v>-0.007051709946068397</v>
       </c>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
@@ -2965,44 +2965,44 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.001426990329079613</v>
+        <v>0.001433028537321141</v>
       </c>
       <c r="D39" t="n">
         <v>0.009771227334849092</v>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>-0.00678985102359404</v>
+        <v>-0.006959549846381992</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.003729617237184689</v>
+        <v>-0.00369196200367848</v>
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>-0.003550056622002265</v>
+        <v>-0.003548829741953189</v>
       </c>
       <c r="J39" t="n">
-        <v>0.009476461969243599</v>
+        <v>0.009902477132609493</v>
       </c>
       <c r="K39" t="n">
-        <v>0.003768960534758421</v>
+        <v>0.003733234997329399</v>
       </c>
       <c r="L39" t="n">
-        <v>0.003768960534758421</v>
+        <v>0.003733234997329399</v>
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
-        <v>0.003768960534758421</v>
+        <v>0.003733234997329399</v>
       </c>
       <c r="P39" t="n">
-        <v>0.003717735220709408</v>
+        <v>0.003680404371216175</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.003748503989940159</v>
+        <v>0.003712135636485425</v>
       </c>
       <c r="R39" t="n">
-        <v>0.003748503989940159</v>
+        <v>0.003712135636485425</v>
       </c>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>

</xml_diff>